<commit_message>
Cleaned up instructions, checked validity of Scheduler
</commit_message>
<xml_diff>
--- a/WMS_Scheduler.xlsx
+++ b/WMS_Scheduler.xlsx
@@ -208,9 +208,6 @@
     <t xml:space="preserve">4. Enter date of a Past A Day of Sem I in Fig.4 (e.g 8/15/2013) </t>
   </si>
   <si>
-    <t>2. All the break / holiday dates from the Calendar have been added, except for wms exam days. This Scheduler works only for Semester I.</t>
-  </si>
-  <si>
     <t>1. Use the LATEST A day (before Date to Schedule)</t>
   </si>
   <si>
@@ -223,9 +220,6 @@
     <t xml:space="preserve">4. Enter date of a Past A Day of Sem II in Fig.4 (e.g 1/6/2013) </t>
   </si>
   <si>
-    <t>2. All the break / holiday dates from the Calendar have been added, except for wms exam days. This Scheduler works only for Semester II.</t>
-  </si>
-  <si>
     <t>Office Hours</t>
   </si>
   <si>
@@ -269,6 +263,12 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>2. All the break / holiday dates from the Calendar have been added, except for wms exam days. This Scheduler works only for Semester I. See "Sheet2" (below) for the Semester II Scheduler.</t>
+  </si>
+  <si>
+    <t>2. All the break / holiday dates from the Calendar have been added, except for wms exam days. This Scheduler works only for Semester II. See "Sheet1" (below) for the Semester I Scheduler.</t>
   </si>
 </sst>
 </file>
@@ -995,63 +995,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
@@ -1135,6 +1078,63 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1458,7 +1458,7 @@
   <sheetData>
     <row r="1" spans="2:21">
       <c r="B1" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9" t="s">
@@ -1475,25 +1475,25 @@
         <v>26</v>
       </c>
       <c r="E3" s="37"/>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="45"/>
-      <c r="P3" s="43" t="s">
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="82"/>
+      <c r="P3" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="45"/>
-      <c r="T3" s="46" t="s">
+      <c r="Q3" s="95"/>
+      <c r="R3" s="82"/>
+      <c r="T3" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="U3" s="47"/>
+      <c r="U3" s="78"/>
     </row>
     <row r="4" spans="2:21" ht="15.75" thickBot="1">
       <c r="B4" s="13" t="s">
@@ -1502,7 +1502,7 @@
       <c r="D4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="72"/>
+      <c r="E4" s="53"/>
       <c r="G4" s="33" t="s">
         <v>1</v>
       </c>
@@ -1527,17 +1527,17 @@
       <c r="N4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="P4" s="76" t="str">
+      <c r="P4" s="57" t="str">
         <f>INDEX(H4:N4, 1, Q4)</f>
-        <v>A</v>
-      </c>
-      <c r="Q4" s="77">
+        <v>G</v>
+      </c>
+      <c r="Q4" s="58">
         <f>MOD(D9, 7)+1</f>
-        <v>1</v>
-      </c>
-      <c r="R4" s="78">
+        <v>7</v>
+      </c>
+      <c r="R4" s="59">
         <f>D7</f>
-        <v>41512</v>
+        <v>41509</v>
       </c>
       <c r="S4" s="18"/>
       <c r="T4" s="19" t="s">
@@ -1554,7 +1554,7 @@
       <c r="D5" s="2">
         <v>41501</v>
       </c>
-      <c r="E5" s="73"/>
+      <c r="E5" s="54"/>
       <c r="F5" s="21"/>
       <c r="G5" s="22">
         <v>1</v>
@@ -1580,17 +1580,17 @@
       <c r="N5" s="4">
         <v>4</v>
       </c>
-      <c r="P5" s="79" t="s">
+      <c r="P5" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="Q5" s="80" t="s">
+      <c r="Q5" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="R5" s="81" t="s">
+      <c r="R5" s="62" t="s">
         <v>5</v>
       </c>
       <c r="S5" s="23"/>
-      <c r="T5" s="48" t="s">
+      <c r="T5" s="79" t="s">
         <v>30</v>
       </c>
       <c r="U5" s="24" t="s">
@@ -1632,7 +1632,7 @@
       <c r="P6" s="29">
         <v>0.5</v>
       </c>
-      <c r="Q6" s="87">
+      <c r="Q6" s="68">
         <f>INDEX(H12:N15, 1, D11)</f>
         <v>9</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>Office Hours</v>
       </c>
       <c r="S6" s="23"/>
-      <c r="T6" s="49"/>
+      <c r="T6" s="80"/>
       <c r="U6" s="26" t="s">
         <v>38</v>
       </c>
@@ -1651,9 +1651,9 @@
         <v>41561</v>
       </c>
       <c r="D7" s="2">
-        <v>41512</v>
-      </c>
-      <c r="E7" s="73"/>
+        <v>41509</v>
+      </c>
+      <c r="E7" s="54"/>
       <c r="G7" s="22">
         <v>3</v>
       </c>
@@ -1678,23 +1678,23 @@
       <c r="N7" s="4">
         <v>6</v>
       </c>
-      <c r="P7" s="82">
+      <c r="P7" s="63">
         <v>1</v>
       </c>
-      <c r="Q7" s="83">
+      <c r="Q7" s="64">
         <f>INDEX(H5:N8,P7, Q4)</f>
-        <v>1</v>
-      </c>
-      <c r="R7" s="84" t="str">
+        <v>4</v>
+      </c>
+      <c r="R7" s="65" t="str">
         <f>INDEX(E16:E23, Q7, 1)</f>
-        <v>History</v>
+        <v>Bible</v>
       </c>
       <c r="S7" s="23"/>
-      <c r="T7" s="48" t="s">
+      <c r="T7" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="U7" s="58" t="s">
-        <v>43</v>
+      <c r="U7" s="91" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="2:21" ht="15.75" thickBot="1">
@@ -1732,41 +1732,41 @@
       <c r="P8" s="29">
         <v>1.5</v>
       </c>
-      <c r="Q8" s="88">
+      <c r="Q8" s="69">
         <f>INDEX(H12:N15, 2, D11)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="R8" s="30" t="str">
         <f>INDEX(E15:E30, Q8+1, 1)</f>
-        <v>Break</v>
-      </c>
-      <c r="T8" s="49"/>
-      <c r="U8" s="59"/>
+        <v>ADV</v>
+      </c>
+      <c r="T8" s="80"/>
+      <c r="U8" s="92"/>
     </row>
     <row r="9" spans="2:21" ht="15.75" thickBot="1">
       <c r="B9" s="7">
         <v>41565</v>
       </c>
-      <c r="D9" s="93">
+      <c r="D9" s="74">
         <f>MAX(NETWORKDAYS(D5, D7,B5:B106)-1, 0)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" s="35"/>
-      <c r="P9" s="82">
+      <c r="P9" s="63">
         <v>2</v>
       </c>
-      <c r="Q9" s="83">
+      <c r="Q9" s="64">
         <f>INDEX(H5:N8,P9, Q4)</f>
-        <v>2</v>
-      </c>
-      <c r="R9" s="84" t="str">
+        <v>5</v>
+      </c>
+      <c r="R9" s="65" t="str">
         <f>INDEX(E16:E23, Q9, 1)</f>
-        <v>Math</v>
-      </c>
-      <c r="T9" s="48" t="s">
+        <v>English</v>
+      </c>
+      <c r="T9" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="U9" s="58" t="s">
+      <c r="U9" s="91" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1775,31 +1775,31 @@
         <v>41575</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="45"/>
-      <c r="P10" s="82">
+        <v>58</v>
+      </c>
+      <c r="G10" s="81" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="95"/>
+      <c r="I10" s="95"/>
+      <c r="J10" s="95"/>
+      <c r="K10" s="95"/>
+      <c r="L10" s="95"/>
+      <c r="M10" s="95"/>
+      <c r="N10" s="82"/>
+      <c r="P10" s="63">
         <v>3</v>
       </c>
-      <c r="Q10" s="83">
+      <c r="Q10" s="64">
         <f>INDEX(H5:N8,P10, Q4)</f>
-        <v>3</v>
-      </c>
-      <c r="R10" s="84" t="str">
+        <v>6</v>
+      </c>
+      <c r="R10" s="65" t="str">
         <f>INDEX(E16:E23, Q10, 1)</f>
-        <v>Physics</v>
-      </c>
-      <c r="T10" s="49"/>
-      <c r="U10" s="59"/>
+        <v>Orchestra</v>
+      </c>
+      <c r="T10" s="80"/>
+      <c r="U10" s="92"/>
     </row>
     <row r="11" spans="2:21" ht="15.75" thickBot="1">
       <c r="B11" s="7">
@@ -1807,47 +1807,47 @@
       </c>
       <c r="D11" s="28">
         <f>WEEKDAY(R4)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="68" t="s">
-        <v>62</v>
-      </c>
-      <c r="I11" s="68" t="s">
+      <c r="H11" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="L11" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="J11" s="68" t="s">
-        <v>58</v>
-      </c>
-      <c r="K11" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="L11" s="68" t="s">
-        <v>57</v>
-      </c>
-      <c r="M11" s="68" t="s">
+      <c r="M11" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="N11" s="69" t="s">
-        <v>62</v>
+      <c r="N11" s="50" t="s">
+        <v>60</v>
       </c>
       <c r="P11" s="29">
         <v>3.5</v>
       </c>
-      <c r="Q11" s="88">
+      <c r="Q11" s="69">
         <f>INDEX(H12:N15, 3, D11)</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="R11" s="30" t="str">
         <f>INDEX(E15:E30, Q11+1, 1)</f>
-        <v>ARTS/ADV</v>
-      </c>
-      <c r="T11" s="48" t="s">
+        <v>Break</v>
+      </c>
+      <c r="T11" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="U11" s="58" t="s">
+      <c r="U11" s="91" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1855,86 +1855,86 @@
       <c r="B12" s="7">
         <v>41604</v>
       </c>
-      <c r="G12" s="90">
+      <c r="G12" s="71">
         <v>0.5</v>
       </c>
-      <c r="H12" s="85">
+      <c r="H12" s="66">
         <v>0</v>
       </c>
-      <c r="I12" s="85">
+      <c r="I12" s="66">
         <v>9</v>
       </c>
-      <c r="J12" s="85">
+      <c r="J12" s="66">
         <v>13</v>
       </c>
-      <c r="K12" s="85">
+      <c r="K12" s="66">
         <v>14</v>
       </c>
-      <c r="L12" s="85">
+      <c r="L12" s="66">
         <v>13</v>
       </c>
-      <c r="M12" s="85">
+      <c r="M12" s="66">
         <v>9</v>
       </c>
-      <c r="N12" s="74">
+      <c r="N12" s="55">
         <v>0</v>
       </c>
-      <c r="P12" s="82">
+      <c r="P12" s="63">
         <v>4</v>
       </c>
-      <c r="Q12" s="83">
+      <c r="Q12" s="64">
         <f>INDEX(H5:N8,P12, Q4)</f>
-        <v>4</v>
-      </c>
-      <c r="R12" s="84" t="str">
+        <v>7</v>
+      </c>
+      <c r="R12" s="65" t="str">
         <f>INDEX(E16:E23, Q12, 1)</f>
-        <v>Bible</v>
-      </c>
-      <c r="T12" s="60"/>
-      <c r="U12" s="61"/>
+        <v>Physics</v>
+      </c>
+      <c r="T12" s="93"/>
+      <c r="U12" s="94"/>
     </row>
     <row r="13" spans="2:21" ht="15.75" thickBot="1">
       <c r="B13" s="7">
         <v>41605</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="45"/>
-      <c r="G13" s="90">
+      <c r="E13" s="82"/>
+      <c r="G13" s="71">
         <v>1.5</v>
       </c>
-      <c r="H13" s="85">
+      <c r="H13" s="66">
         <v>0</v>
       </c>
-      <c r="I13" s="85">
+      <c r="I13" s="66">
         <v>10</v>
       </c>
-      <c r="J13" s="85">
+      <c r="J13" s="66">
         <v>10</v>
       </c>
-      <c r="K13" s="85">
+      <c r="K13" s="66">
         <v>10</v>
       </c>
-      <c r="L13" s="85">
+      <c r="L13" s="66">
         <v>11</v>
       </c>
-      <c r="M13" s="85">
+      <c r="M13" s="66">
         <v>12</v>
       </c>
-      <c r="N13" s="74">
+      <c r="N13" s="55">
         <v>0</v>
       </c>
       <c r="P13" s="31">
         <v>4.5</v>
       </c>
-      <c r="Q13" s="89">
+      <c r="Q13" s="70">
         <f>INDEX(H12:N15, 4, D11)</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="R13" s="32" t="str">
         <f>INDEX(E15:E30, Q13+1, 1)</f>
-        <v>Office Hours</v>
+        <v>Empty</v>
       </c>
     </row>
     <row r="14" spans="2:21" ht="15.75" thickBot="1">
@@ -1944,38 +1944,38 @@
       <c r="D14" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="65" t="s">
+      <c r="E14" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="90">
+      <c r="G14" s="71">
         <v>3.5</v>
       </c>
-      <c r="H14" s="85">
+      <c r="H14" s="66">
         <v>0</v>
       </c>
-      <c r="I14" s="85">
+      <c r="I14" s="66">
         <v>15</v>
       </c>
-      <c r="J14" s="85">
+      <c r="J14" s="66">
         <v>15</v>
       </c>
-      <c r="K14" s="85">
+      <c r="K14" s="66">
         <v>10</v>
       </c>
-      <c r="L14" s="85">
+      <c r="L14" s="66">
         <v>10</v>
       </c>
-      <c r="M14" s="85">
+      <c r="M14" s="66">
         <v>10</v>
       </c>
-      <c r="N14" s="74">
+      <c r="N14" s="55">
         <v>0</v>
       </c>
       <c r="P14" s="39"/>
-      <c r="T14" s="43" t="s">
+      <c r="T14" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="U14" s="45"/>
+      <c r="U14" s="82"/>
     </row>
     <row r="15" spans="2:21" ht="15.75" thickBot="1">
       <c r="B15" s="7">
@@ -1984,51 +1984,51 @@
       <c r="D15" s="22">
         <v>0</v>
       </c>
-      <c r="E15" s="86" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="91">
+      <c r="E15" s="67" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="72">
         <v>4.5</v>
       </c>
-      <c r="H15" s="92">
+      <c r="H15" s="73">
         <v>0</v>
       </c>
-      <c r="I15" s="92">
+      <c r="I15" s="73">
         <v>9</v>
       </c>
-      <c r="J15" s="92">
+      <c r="J15" s="73">
         <v>9</v>
       </c>
-      <c r="K15" s="92">
+      <c r="K15" s="73">
         <v>9</v>
       </c>
-      <c r="L15" s="92">
+      <c r="L15" s="73">
         <v>9</v>
       </c>
-      <c r="M15" s="92">
+      <c r="M15" s="73">
         <v>0</v>
       </c>
-      <c r="N15" s="75">
+      <c r="N15" s="56">
         <v>0</v>
       </c>
       <c r="P15" s="39"/>
-      <c r="T15" s="50" t="s">
+      <c r="T15" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="U15" s="51"/>
+      <c r="U15" s="84"/>
     </row>
     <row r="16" spans="2:21">
       <c r="B16" s="7"/>
       <c r="D16" s="22">
         <v>1</v>
       </c>
-      <c r="E16" s="66" t="s">
+      <c r="E16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="63"/>
+      <c r="G16" s="44"/>
       <c r="P16" s="39"/>
-      <c r="T16" s="52"/>
-      <c r="U16" s="53"/>
+      <c r="T16" s="85"/>
+      <c r="U16" s="86"/>
     </row>
     <row r="17" spans="2:21">
       <c r="B17" s="7"/>
@@ -2036,14 +2036,14 @@
         <f>D16+1</f>
         <v>2</v>
       </c>
-      <c r="E17" s="66" t="s">
+      <c r="E17" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="63"/>
-      <c r="T17" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="U17" s="55"/>
+      <c r="G17" s="44"/>
+      <c r="T17" s="87" t="s">
+        <v>61</v>
+      </c>
+      <c r="U17" s="88"/>
     </row>
     <row r="18" spans="2:21">
       <c r="B18" s="7"/>
@@ -2051,13 +2051,13 @@
         <f t="shared" ref="D18:D30" si="0">D17+1</f>
         <v>3</v>
       </c>
-      <c r="E18" s="66" t="s">
+      <c r="E18" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="63"/>
+      <c r="G18" s="44"/>
       <c r="P18" s="34"/>
-      <c r="T18" s="54"/>
-      <c r="U18" s="55"/>
+      <c r="T18" s="87"/>
+      <c r="U18" s="88"/>
     </row>
     <row r="19" spans="2:21" ht="15.75" thickBot="1">
       <c r="B19" s="7"/>
@@ -2065,13 +2065,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E19" s="66" t="s">
+      <c r="E19" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="63"/>
+      <c r="G19" s="44"/>
       <c r="P19" s="37"/>
-      <c r="T19" s="56"/>
-      <c r="U19" s="57"/>
+      <c r="T19" s="89"/>
+      <c r="U19" s="90"/>
     </row>
     <row r="20" spans="2:21">
       <c r="B20" s="7"/>
@@ -2079,10 +2079,10 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E20" s="66" t="s">
+      <c r="E20" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="64"/>
+      <c r="G20" s="45"/>
       <c r="P20" s="39"/>
     </row>
     <row r="21" spans="2:21">
@@ -2091,7 +2091,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E21" s="66" t="s">
+      <c r="E21" s="47" t="s">
         <v>11</v>
       </c>
       <c r="P21" s="39"/>
@@ -2102,7 +2102,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="E22" s="66" t="s">
+      <c r="E22" s="47" t="s">
         <v>8</v>
       </c>
       <c r="P22" s="39"/>
@@ -2113,7 +2113,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E23" s="70" t="s">
+      <c r="E23" s="51" t="s">
         <v>16</v>
       </c>
       <c r="P23" s="39"/>
@@ -2124,8 +2124,8 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="E24" s="71" t="s">
-        <v>48</v>
+      <c r="E24" s="52" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="2:21">
@@ -2134,8 +2134,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E25" s="71" t="s">
-        <v>49</v>
+      <c r="E25" s="52" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="2:21">
@@ -2144,8 +2144,8 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="E26" s="71" t="s">
-        <v>51</v>
+      <c r="E26" s="52" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="2:21">
@@ -2154,8 +2154,8 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E27" s="71" t="s">
-        <v>54</v>
+      <c r="E27" s="52" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="2:21">
@@ -2164,8 +2164,8 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="E28" s="71" t="s">
-        <v>52</v>
+      <c r="E28" s="52" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="2:21">
@@ -2174,8 +2174,8 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="E29" s="71" t="s">
-        <v>53</v>
+      <c r="E29" s="52" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="2:21" ht="15.75" thickBot="1">
@@ -2184,8 +2184,8 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="E30" s="67" t="s">
-        <v>50</v>
+      <c r="E30" s="48" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="2:21">
@@ -2419,6 +2419,10 @@
   </sheetData>
   <sheetProtection password="C836" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
   <mergeCells count="15">
+    <mergeCell ref="G3:N3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="G10:N10"/>
     <mergeCell ref="T3:U3"/>
     <mergeCell ref="T5:T6"/>
     <mergeCell ref="T14:U14"/>
@@ -2430,10 +2434,6 @@
     <mergeCell ref="U9:U10"/>
     <mergeCell ref="T11:T12"/>
     <mergeCell ref="U11:U12"/>
-    <mergeCell ref="G3:N3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="G10:N10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2455,7 +2455,7 @@
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="3.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="95" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="76" customWidth="1"/>
     <col min="6" max="6" width="3.85546875" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
     <col min="8" max="14" width="2.7109375" customWidth="1"/>
@@ -2471,13 +2471,13 @@
     <row r="1" spans="1:21">
       <c r="A1" s="10"/>
       <c r="B1" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="94"/>
+      <c r="E1" s="75"/>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
@@ -2529,27 +2529,27 @@
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="45"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="82"/>
       <c r="O3" s="10"/>
-      <c r="P3" s="43" t="s">
+      <c r="P3" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="45"/>
+      <c r="Q3" s="95"/>
+      <c r="R3" s="82"/>
       <c r="S3" s="10"/>
-      <c r="T3" s="46" t="s">
+      <c r="T3" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="U3" s="47"/>
+      <c r="U3" s="78"/>
     </row>
     <row r="4" spans="1:21" ht="15.75" thickBot="1">
       <c r="A4" s="10"/>
@@ -2560,7 +2560,7 @@
       <c r="D4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="72"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="10"/>
       <c r="G4" s="33" t="s">
         <v>1</v>
@@ -2587,15 +2587,15 @@
         <v>21</v>
       </c>
       <c r="O4" s="10"/>
-      <c r="P4" s="76" t="str">
+      <c r="P4" s="57" t="str">
         <f>INDEX(H4:N4, 1, Q4)</f>
         <v>G</v>
       </c>
-      <c r="Q4" s="77">
+      <c r="Q4" s="58">
         <f>MOD(D9, 7)+1</f>
         <v>7</v>
       </c>
-      <c r="R4" s="78">
+      <c r="R4" s="59">
         <f>D7</f>
         <v>41773</v>
       </c>
@@ -2616,7 +2616,7 @@
       <c r="D5" s="2">
         <v>41645</v>
       </c>
-      <c r="E5" s="73"/>
+      <c r="E5" s="54"/>
       <c r="F5" s="21"/>
       <c r="G5" s="22">
         <v>1</v>
@@ -2643,17 +2643,17 @@
         <v>4</v>
       </c>
       <c r="O5" s="10"/>
-      <c r="P5" s="79" t="s">
+      <c r="P5" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="Q5" s="80" t="s">
+      <c r="Q5" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="R5" s="81" t="s">
+      <c r="R5" s="62" t="s">
         <v>5</v>
       </c>
       <c r="S5" s="23"/>
-      <c r="T5" s="48" t="s">
+      <c r="T5" s="79" t="s">
         <v>30</v>
       </c>
       <c r="U5" s="41" t="s">
@@ -2699,7 +2699,7 @@
       <c r="P6" s="29">
         <v>0.5</v>
       </c>
-      <c r="Q6" s="87">
+      <c r="Q6" s="68">
         <f>INDEX(H12:N15, 1, D11)</f>
         <v>14</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>FAC MTGS</v>
       </c>
       <c r="S6" s="23"/>
-      <c r="T6" s="49"/>
+      <c r="T6" s="80"/>
       <c r="U6" s="42" t="s">
         <v>38</v>
       </c>
@@ -2722,7 +2722,7 @@
       <c r="D7" s="2">
         <v>41773</v>
       </c>
-      <c r="E7" s="73"/>
+      <c r="E7" s="54"/>
       <c r="F7" s="10"/>
       <c r="G7" s="22">
         <v>3</v>
@@ -2749,23 +2749,23 @@
         <v>6</v>
       </c>
       <c r="O7" s="10"/>
-      <c r="P7" s="82">
+      <c r="P7" s="63">
         <v>1</v>
       </c>
-      <c r="Q7" s="83">
+      <c r="Q7" s="64">
         <f>INDEX(H5:N8,P7, Q4)</f>
         <v>4</v>
       </c>
-      <c r="R7" s="84" t="str">
+      <c r="R7" s="65" t="str">
         <f>INDEX(E16:E23, Q7, 1)</f>
         <v>Bible</v>
       </c>
       <c r="S7" s="23"/>
-      <c r="T7" s="48" t="s">
+      <c r="T7" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="U7" s="58" t="s">
-        <v>43</v>
+      <c r="U7" s="91" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1">
@@ -2807,7 +2807,7 @@
       <c r="P8" s="29">
         <v>1.5</v>
       </c>
-      <c r="Q8" s="88">
+      <c r="Q8" s="69">
         <f>INDEX(H12:N15, 2, D11)</f>
         <v>10</v>
       </c>
@@ -2816,8 +2816,8 @@
         <v>Break</v>
       </c>
       <c r="S8" s="10"/>
-      <c r="T8" s="49"/>
-      <c r="U8" s="59"/>
+      <c r="T8" s="80"/>
+      <c r="U8" s="92"/>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1">
       <c r="A9" s="10"/>
@@ -2825,7 +2825,7 @@
         <v>41708</v>
       </c>
       <c r="C9" s="10"/>
-      <c r="D9" s="93">
+      <c r="D9" s="74">
         <f>MAX(NETWORKDAYS(D5, D7,B5:B106)-1, 0)</f>
         <v>83</v>
       </c>
@@ -2840,22 +2840,22 @@
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
-      <c r="P9" s="82">
+      <c r="P9" s="63">
         <v>2</v>
       </c>
-      <c r="Q9" s="83">
+      <c r="Q9" s="64">
         <f>INDEX(H5:N8,P9, Q4)</f>
         <v>5</v>
       </c>
-      <c r="R9" s="84" t="str">
+      <c r="R9" s="65" t="str">
         <f>INDEX(E16:E23, Q9, 1)</f>
         <v>English</v>
       </c>
       <c r="S9" s="10"/>
-      <c r="T9" s="48" t="s">
+      <c r="T9" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="U9" s="58" t="s">
+      <c r="U9" s="91" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2866,35 +2866,35 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="45"/>
+      <c r="G10" s="81" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="95"/>
+      <c r="I10" s="95"/>
+      <c r="J10" s="95"/>
+      <c r="K10" s="95"/>
+      <c r="L10" s="95"/>
+      <c r="M10" s="95"/>
+      <c r="N10" s="82"/>
       <c r="O10" s="10"/>
-      <c r="P10" s="82">
+      <c r="P10" s="63">
         <v>3</v>
       </c>
-      <c r="Q10" s="83">
+      <c r="Q10" s="64">
         <f>INDEX(H5:N8,P10, Q4)</f>
         <v>6</v>
       </c>
-      <c r="R10" s="84" t="str">
+      <c r="R10" s="65" t="str">
         <f>INDEX(E16:E23, Q10, 1)</f>
         <v>Orchestra</v>
       </c>
       <c r="S10" s="10"/>
-      <c r="T10" s="49"/>
-      <c r="U10" s="59"/>
+      <c r="T10" s="80"/>
+      <c r="U10" s="92"/>
     </row>
     <row r="11" spans="1:21" ht="15.75" thickBot="1">
       <c r="A11" s="10"/>
@@ -2907,36 +2907,36 @@
         <v>4</v>
       </c>
       <c r="E11" s="35"/>
-      <c r="F11" s="62"/>
+      <c r="F11" s="43"/>
       <c r="G11" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="68" t="s">
-        <v>62</v>
-      </c>
-      <c r="I11" s="68" t="s">
+      <c r="H11" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="L11" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="J11" s="68" t="s">
-        <v>58</v>
-      </c>
-      <c r="K11" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="L11" s="68" t="s">
-        <v>57</v>
-      </c>
-      <c r="M11" s="68" t="s">
+      <c r="M11" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="N11" s="69" t="s">
-        <v>62</v>
+      <c r="N11" s="50" t="s">
+        <v>60</v>
       </c>
       <c r="O11" s="10"/>
       <c r="P11" s="29">
         <v>3.5</v>
       </c>
-      <c r="Q11" s="88">
+      <c r="Q11" s="69">
         <f>INDEX(H12:N15, 3, D11)</f>
         <v>10</v>
       </c>
@@ -2945,10 +2945,10 @@
         <v>Break</v>
       </c>
       <c r="S11" s="10"/>
-      <c r="T11" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="U11" s="58" t="s">
+      <c r="T11" s="79" t="s">
+        <v>45</v>
+      </c>
+      <c r="U11" s="91" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2960,46 +2960,46 @@
       <c r="C12" s="10"/>
       <c r="D12" s="37"/>
       <c r="E12" s="37"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="90">
+      <c r="F12" s="43"/>
+      <c r="G12" s="71">
         <v>0.5</v>
       </c>
-      <c r="H12" s="85">
+      <c r="H12" s="66">
         <v>0</v>
       </c>
-      <c r="I12" s="85">
+      <c r="I12" s="66">
         <v>9</v>
       </c>
-      <c r="J12" s="85">
+      <c r="J12" s="66">
         <v>13</v>
       </c>
-      <c r="K12" s="85">
+      <c r="K12" s="66">
         <v>14</v>
       </c>
-      <c r="L12" s="85">
+      <c r="L12" s="66">
         <v>13</v>
       </c>
-      <c r="M12" s="85">
+      <c r="M12" s="66">
         <v>9</v>
       </c>
-      <c r="N12" s="74">
+      <c r="N12" s="55">
         <v>0</v>
       </c>
       <c r="O12" s="10"/>
-      <c r="P12" s="82">
+      <c r="P12" s="63">
         <v>4</v>
       </c>
-      <c r="Q12" s="83">
+      <c r="Q12" s="64">
         <f>INDEX(H5:N8,P12, Q4)</f>
         <v>7</v>
       </c>
-      <c r="R12" s="84" t="str">
+      <c r="R12" s="65" t="str">
         <f>INDEX(E16:E23, Q12, 1)</f>
         <v>Physics</v>
       </c>
       <c r="S12" s="10"/>
-      <c r="T12" s="60"/>
-      <c r="U12" s="61"/>
+      <c r="T12" s="93"/>
+      <c r="U12" s="94"/>
     </row>
     <row r="13" spans="1:21" ht="15.75" thickBot="1">
       <c r="A13" s="10"/>
@@ -3007,40 +3007,40 @@
         <v>41712</v>
       </c>
       <c r="C13" s="10"/>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="45"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="90">
+      <c r="E13" s="82"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="71">
         <v>1.5</v>
       </c>
-      <c r="H13" s="85">
+      <c r="H13" s="66">
         <v>0</v>
       </c>
-      <c r="I13" s="85">
+      <c r="I13" s="66">
         <v>10</v>
       </c>
-      <c r="J13" s="85">
+      <c r="J13" s="66">
         <v>10</v>
       </c>
-      <c r="K13" s="85">
+      <c r="K13" s="66">
         <v>10</v>
       </c>
-      <c r="L13" s="85">
+      <c r="L13" s="66">
         <v>11</v>
       </c>
-      <c r="M13" s="85">
+      <c r="M13" s="66">
         <v>12</v>
       </c>
-      <c r="N13" s="74">
+      <c r="N13" s="55">
         <v>0</v>
       </c>
       <c r="O13" s="10"/>
       <c r="P13" s="31">
         <v>4.5</v>
       </c>
-      <c r="Q13" s="89">
+      <c r="Q13" s="70">
         <f>INDEX(H12:N15, 4, D11)</f>
         <v>9</v>
       </c>
@@ -3061,32 +3061,32 @@
       <c r="D14" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="65" t="s">
+      <c r="E14" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="63"/>
-      <c r="G14" s="90">
+      <c r="F14" s="44"/>
+      <c r="G14" s="71">
         <v>3.5</v>
       </c>
-      <c r="H14" s="85">
+      <c r="H14" s="66">
         <v>0</v>
       </c>
-      <c r="I14" s="85">
+      <c r="I14" s="66">
         <v>15</v>
       </c>
-      <c r="J14" s="85">
+      <c r="J14" s="66">
         <v>15</v>
       </c>
-      <c r="K14" s="85">
+      <c r="K14" s="66">
         <v>10</v>
       </c>
-      <c r="L14" s="85">
+      <c r="L14" s="66">
         <v>10</v>
       </c>
-      <c r="M14" s="85">
+      <c r="M14" s="66">
         <v>10</v>
       </c>
-      <c r="N14" s="74">
+      <c r="N14" s="55">
         <v>0</v>
       </c>
       <c r="O14" s="10"/>
@@ -3094,10 +3094,10 @@
       <c r="Q14" s="39"/>
       <c r="R14" s="40"/>
       <c r="S14" s="10"/>
-      <c r="T14" s="43" t="s">
+      <c r="T14" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="U14" s="45"/>
+      <c r="U14" s="82"/>
     </row>
     <row r="15" spans="1:21" ht="15.75" thickBot="1">
       <c r="A15" s="10"/>
@@ -3108,32 +3108,32 @@
       <c r="D15" s="22">
         <v>0</v>
       </c>
-      <c r="E15" s="86" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="63"/>
-      <c r="G15" s="91">
+      <c r="E15" s="67" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="44"/>
+      <c r="G15" s="72">
         <v>4.5</v>
       </c>
-      <c r="H15" s="92">
+      <c r="H15" s="73">
         <v>0</v>
       </c>
-      <c r="I15" s="92">
+      <c r="I15" s="73">
         <v>9</v>
       </c>
-      <c r="J15" s="92">
+      <c r="J15" s="73">
         <v>9</v>
       </c>
-      <c r="K15" s="92">
+      <c r="K15" s="73">
         <v>9</v>
       </c>
-      <c r="L15" s="92">
+      <c r="L15" s="73">
         <v>9</v>
       </c>
-      <c r="M15" s="92">
+      <c r="M15" s="73">
         <v>0</v>
       </c>
-      <c r="N15" s="75">
+      <c r="N15" s="56">
         <v>0</v>
       </c>
       <c r="O15" s="10"/>
@@ -3141,10 +3141,10 @@
       <c r="Q15" s="39"/>
       <c r="R15" s="40"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="50" t="s">
+      <c r="T15" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="U15" s="51"/>
+      <c r="U15" s="84"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="10"/>
@@ -3155,11 +3155,11 @@
       <c r="D16" s="22">
         <v>1</v>
       </c>
-      <c r="E16" s="66" t="s">
+      <c r="E16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="63"/>
-      <c r="G16" s="63"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
@@ -3172,8 +3172,8 @@
       <c r="Q16" s="39"/>
       <c r="R16" s="40"/>
       <c r="S16" s="10"/>
-      <c r="T16" s="52"/>
-      <c r="U16" s="53"/>
+      <c r="T16" s="85"/>
+      <c r="U16" s="86"/>
     </row>
     <row r="17" spans="1:21">
       <c r="A17" s="10"/>
@@ -3185,11 +3185,11 @@
         <f>D16+1</f>
         <v>2</v>
       </c>
-      <c r="E17" s="66" t="s">
+      <c r="E17" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
@@ -3202,10 +3202,10 @@
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
-      <c r="T17" s="54" t="s">
-        <v>47</v>
-      </c>
-      <c r="U17" s="55"/>
+      <c r="T17" s="87" t="s">
+        <v>62</v>
+      </c>
+      <c r="U17" s="88"/>
     </row>
     <row r="18" spans="1:21">
       <c r="A18" s="10"/>
@@ -3217,11 +3217,11 @@
         <f t="shared" ref="D18:D30" si="0">D17+1</f>
         <v>3</v>
       </c>
-      <c r="E18" s="66" t="s">
+      <c r="E18" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
@@ -3234,8 +3234,8 @@
       <c r="Q18" s="35"/>
       <c r="R18" s="36"/>
       <c r="S18" s="10"/>
-      <c r="T18" s="54"/>
-      <c r="U18" s="55"/>
+      <c r="T18" s="87"/>
+      <c r="U18" s="88"/>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1">
       <c r="A19" s="10"/>
@@ -3247,11 +3247,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E19" s="66" t="s">
+      <c r="E19" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="63"/>
-      <c r="G19" s="63"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
@@ -3264,8 +3264,8 @@
       <c r="Q19" s="37"/>
       <c r="R19" s="38"/>
       <c r="S19" s="10"/>
-      <c r="T19" s="56"/>
-      <c r="U19" s="57"/>
+      <c r="T19" s="89"/>
+      <c r="U19" s="90"/>
     </row>
     <row r="20" spans="1:21">
       <c r="A20" s="10"/>
@@ -3275,11 +3275,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E20" s="66" t="s">
+      <c r="E20" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
@@ -3303,7 +3303,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E21" s="66" t="s">
+      <c r="E21" s="47" t="s">
         <v>11</v>
       </c>
       <c r="F21" s="10"/>
@@ -3331,7 +3331,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="E22" s="66" t="s">
+      <c r="E22" s="47" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="10"/>
@@ -3359,7 +3359,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E23" s="70" t="s">
+      <c r="E23" s="51" t="s">
         <v>16</v>
       </c>
       <c r="F23" s="10"/>
@@ -3387,8 +3387,8 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="E24" s="71" t="s">
-        <v>48</v>
+      <c r="E24" s="52" t="s">
+        <v>46</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
@@ -3415,8 +3415,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E25" s="71" t="s">
-        <v>49</v>
+      <c r="E25" s="52" t="s">
+        <v>47</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
@@ -3443,8 +3443,8 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="E26" s="71" t="s">
-        <v>51</v>
+      <c r="E26" s="52" t="s">
+        <v>49</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
@@ -3471,8 +3471,8 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E27" s="71" t="s">
-        <v>54</v>
+      <c r="E27" s="52" t="s">
+        <v>52</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
@@ -3499,8 +3499,8 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="E28" s="71" t="s">
-        <v>52</v>
+      <c r="E28" s="52" t="s">
+        <v>50</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -3527,8 +3527,8 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="E29" s="71" t="s">
-        <v>53</v>
+      <c r="E29" s="52" t="s">
+        <v>51</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
@@ -3555,8 +3555,8 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="E30" s="67" t="s">
-        <v>50</v>
+      <c r="E30" s="48" t="s">
+        <v>48</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -5326,6 +5326,12 @@
   </sheetData>
   <sheetProtection password="C836" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
   <mergeCells count="15">
+    <mergeCell ref="G3:N3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="U7:U8"/>
     <mergeCell ref="G10:N10"/>
     <mergeCell ref="T17:U19"/>
     <mergeCell ref="T14:U14"/>
@@ -5335,12 +5341,6 @@
     <mergeCell ref="U9:U10"/>
     <mergeCell ref="T11:T12"/>
     <mergeCell ref="U11:U12"/>
-    <mergeCell ref="G3:N3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="T5:T6"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="U7:U8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Extended timing support to Macros
</commit_message>
<xml_diff>
--- a/WMS_Scheduler.xlsx
+++ b/WMS_Scheduler.xlsx
@@ -111,9 +111,6 @@
     <t>Instructions</t>
   </si>
   <si>
-    <t>2. Enter the date for the desired schedule in Fig. 4</t>
-  </si>
-  <si>
     <t>Date to Schedule</t>
   </si>
   <si>
@@ -166,9 +163,6 @@
   </si>
   <si>
     <t>Day Number</t>
-  </si>
-  <si>
-    <t>Empty</t>
   </si>
   <si>
     <t>S</t>
@@ -325,13 +319,19 @@
   <si>
     <t xml:space="preserve">4. Enter date of a Past A Day of Sem II in Fig. 3 (e.g 1/6/2014) </t>
   </si>
+  <si>
+    <t>2. Enter the date for the desired schedule in Fig. 3</t>
+  </si>
+  <si>
+    <t>Weekend</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -1091,35 +1091,26 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -1129,13 +1120,13 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1145,18 +1136,62 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1169,44 +1204,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1502,10 +1502,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:Y124"/>
+  <dimension ref="B1:Y123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1532,1147 +1532,1143 @@
     <col min="26" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25">
-      <c r="D1" s="9"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-    </row>
-    <row r="2" spans="2:25" ht="15.75" thickBot="1"/>
+    <row r="1" spans="2:25" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:25" ht="15.75" thickBot="1">
+      <c r="B2" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="74"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="77" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="79"/>
+      <c r="L2" s="77" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="79"/>
+    </row>
     <row r="3" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B3" s="87" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="54" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="55"/>
-      <c r="L3" s="54" t="s">
+      <c r="B3" s="75" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="76"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="89" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="86" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="87"/>
+      <c r="J3" s="88"/>
+      <c r="L3" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="56"/>
-      <c r="R3" s="55"/>
-    </row>
-    <row r="4" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B4" s="89" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="75" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="92" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="98"/>
-      <c r="J4" s="99"/>
-      <c r="L4" s="83" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="84"/>
-      <c r="N4" s="84"/>
-      <c r="O4" s="84"/>
-      <c r="P4" s="84"/>
-      <c r="Q4" s="84"/>
-      <c r="R4" s="85"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="92"/>
+      <c r="O3" s="92"/>
+      <c r="P3" s="92"/>
+      <c r="Q3" s="92"/>
+      <c r="R3" s="93"/>
+      <c r="X3" s="29"/>
+      <c r="Y3" s="29"/>
+    </row>
+    <row r="4" spans="2:25">
+      <c r="D4" s="71"/>
+      <c r="E4" s="94" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="95"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="80" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="81"/>
+      <c r="J4" s="82"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="95"/>
+      <c r="N4" s="95"/>
+      <c r="O4" s="95"/>
+      <c r="P4" s="95"/>
+      <c r="Q4" s="95"/>
+      <c r="R4" s="96"/>
       <c r="X4" s="29"/>
       <c r="Y4" s="29"/>
     </row>
     <row r="5" spans="2:25">
-      <c r="D5" s="74"/>
-      <c r="E5" s="78" t="s">
-        <v>77</v>
-      </c>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="91" t="s">
-        <v>73</v>
-      </c>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="76"/>
-      <c r="N5" s="76"/>
-      <c r="O5" s="76"/>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="76"/>
-      <c r="R5" s="79"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="102"/>
+      <c r="L5" s="94" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" s="95"/>
+      <c r="N5" s="95"/>
+      <c r="O5" s="95"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="95"/>
+      <c r="R5" s="96"/>
       <c r="X5" s="29"/>
       <c r="Y5" s="29"/>
     </row>
     <row r="6" spans="2:25">
-      <c r="D6" s="74"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="76"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="95"/>
-      <c r="I6" s="96"/>
-      <c r="J6" s="97"/>
-      <c r="L6" s="78" t="s">
-        <v>52</v>
-      </c>
-      <c r="M6" s="76"/>
-      <c r="N6" s="76"/>
-      <c r="O6" s="76"/>
-      <c r="P6" s="76"/>
-      <c r="Q6" s="76"/>
-      <c r="R6" s="79"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="94" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="95"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="80" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" s="81"/>
+      <c r="J6" s="82"/>
+      <c r="L6" s="94"/>
+      <c r="M6" s="95"/>
+      <c r="N6" s="95"/>
+      <c r="O6" s="95"/>
+      <c r="P6" s="95"/>
+      <c r="Q6" s="95"/>
+      <c r="R6" s="96"/>
       <c r="X6" s="29"/>
       <c r="Y6" s="29"/>
     </row>
-    <row r="7" spans="2:25">
-      <c r="D7" s="74"/>
-      <c r="E7" s="78" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="91" t="s">
-        <v>80</v>
-      </c>
-      <c r="I7" s="93"/>
-      <c r="J7" s="94"/>
-      <c r="L7" s="78"/>
-      <c r="M7" s="76"/>
-      <c r="N7" s="76"/>
-      <c r="O7" s="76"/>
-      <c r="P7" s="76"/>
-      <c r="Q7" s="76"/>
-      <c r="R7" s="79"/>
+    <row r="7" spans="2:25" ht="15.75" thickBot="1">
+      <c r="D7" s="71"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="102"/>
+      <c r="L7" s="97"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="98"/>
+      <c r="O7" s="98"/>
+      <c r="P7" s="98"/>
+      <c r="Q7" s="98"/>
+      <c r="R7" s="99"/>
       <c r="X7" s="29"/>
       <c r="Y7" s="29"/>
     </row>
     <row r="8" spans="2:25" ht="15.75" thickBot="1">
-      <c r="D8" s="74"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="95"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="97"/>
-      <c r="L8" s="80"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="81"/>
-      <c r="O8" s="81"/>
-      <c r="P8" s="81"/>
-      <c r="Q8" s="81"/>
-      <c r="R8" s="82"/>
-      <c r="X8" s="29"/>
-      <c r="Y8" s="29"/>
-    </row>
-    <row r="9" spans="2:25">
-      <c r="D9" s="74"/>
-      <c r="E9" s="78" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="91" t="s">
+      <c r="B8" s="77" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="79"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="94" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="95"/>
+      <c r="G8" s="95"/>
+      <c r="H8" s="80" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="81"/>
+      <c r="J8" s="82"/>
+    </row>
+    <row r="9" spans="2:25" ht="15.75" thickBot="1">
+      <c r="B9" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="94"/>
+      <c r="F9" s="95"/>
+      <c r="G9" s="95"/>
+      <c r="H9" s="100"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="102"/>
+    </row>
+    <row r="10" spans="2:25" ht="15.75" thickBot="1">
+      <c r="B10" s="18">
+        <v>0</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="94" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="95"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="80" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="81"/>
+      <c r="J10" s="82"/>
+      <c r="N10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q10" s="78"/>
+      <c r="R10" s="78"/>
+      <c r="S10" s="79"/>
+    </row>
+    <row r="11" spans="2:25" ht="15.75" thickBot="1">
+      <c r="B11" s="18">
+        <v>1</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="97"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="83"/>
+      <c r="I11" s="84"/>
+      <c r="J11" s="85"/>
+      <c r="N11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="P11" s="40" t="str">
+        <f>INDEX(F14:L14, 1, Q11)</f>
+        <v>D</v>
+      </c>
+      <c r="Q11" s="59">
+        <f>MOD(N16, 7)+1</f>
+        <v>4</v>
+      </c>
+      <c r="R11" s="70" t="s">
+        <v>72</v>
+      </c>
+      <c r="S11" s="69">
+        <f>N14</f>
+        <v>41582</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25" ht="15.75" thickBot="1">
+      <c r="B12" s="18">
+        <f>B11+1</f>
+        <v>2</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="N12" s="2">
+        <v>41501</v>
+      </c>
+      <c r="P12" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="R12" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="S12" s="65" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25" ht="15.75" thickBot="1">
+      <c r="B13" s="18">
+        <f t="shared" ref="B13:B25" si="0">B12+1</f>
+        <v>3</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="77" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="78"/>
+      <c r="I13" s="78"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="78"/>
+      <c r="L13" s="79"/>
+      <c r="N13" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94"/>
-    </row>
-    <row r="10" spans="2:25" ht="15.75" thickBot="1">
-      <c r="E10" s="78"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="95"/>
-      <c r="I10" s="96"/>
-      <c r="J10" s="97"/>
-    </row>
-    <row r="11" spans="2:25" ht="15.75" thickBot="1">
-      <c r="E11" s="78" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="91" t="s">
-        <v>29</v>
-      </c>
-      <c r="I11" s="93"/>
-      <c r="J11" s="94"/>
-      <c r="N11" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="P11" s="54" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q11" s="56"/>
-      <c r="R11" s="56"/>
-      <c r="S11" s="55"/>
-    </row>
-    <row r="12" spans="2:25" ht="15.75" thickBot="1">
-      <c r="E12" s="80"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="100"/>
-      <c r="I12" s="101"/>
-      <c r="J12" s="102"/>
-      <c r="N12" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="P12" s="40" t="str">
-        <f>INDEX(F15:L15, 1, Q12)</f>
-        <v>D</v>
-      </c>
-      <c r="Q12" s="62">
-        <f>MOD(N17, 7)+1</f>
+      <c r="O13" s="26"/>
+      <c r="P13" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="Q13" s="47">
+        <f>INDEX(F22:L25, 1, N18)</f>
+        <v>9</v>
+      </c>
+      <c r="R13" s="61" t="str">
+        <f>INDEX(C10:C25, Q13+1, 1)</f>
+        <v>Office Hours</v>
+      </c>
+      <c r="S13" s="66" t="str">
+        <f>INDEX(F29:L32, 1, N18)</f>
+        <v>8:00-8:30</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25">
+      <c r="B14" s="18">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="R12" s="73" t="s">
-        <v>74</v>
-      </c>
-      <c r="S12" s="72">
-        <f>N15</f>
+      <c r="C14" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="2">
         <v>41582</v>
       </c>
-    </row>
-    <row r="13" spans="2:25" ht="15.75" thickBot="1">
-      <c r="N13" s="2">
-        <v>41501</v>
-      </c>
-      <c r="P13" s="41" t="s">
+      <c r="O14" s="26"/>
+      <c r="P14" s="43">
         <v>1</v>
       </c>
-      <c r="Q13" s="42" t="s">
+      <c r="Q14" s="44">
+        <f>INDEX(F15:L18,P14, Q11)</f>
+        <v>6</v>
+      </c>
+      <c r="R14" s="62" t="str">
+        <f>INDEX(C11:C18, Q14, 1)</f>
+        <v>Orchestra</v>
+      </c>
+      <c r="S14" s="67" t="str">
+        <f>INDEX(F33:L36, P14, N18)</f>
+        <v>8:30-9:40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:25">
+      <c r="B15" s="18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="18">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <v>5</v>
+      </c>
+      <c r="H15" s="3">
         <v>2</v>
       </c>
-      <c r="R13" s="66" t="s">
+      <c r="I15" s="3">
+        <v>6</v>
+      </c>
+      <c r="J15" s="3">
+        <v>3</v>
+      </c>
+      <c r="K15" s="3">
+        <v>8</v>
+      </c>
+      <c r="L15" s="4">
         <v>4</v>
       </c>
-      <c r="S13" s="68" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B14" s="54" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="55"/>
-      <c r="E14" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="55"/>
-      <c r="N14" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="O14" s="26"/>
-      <c r="P14" s="22">
-        <v>0.5</v>
-      </c>
-      <c r="Q14" s="47">
-        <f>INDEX(F23:L26, 1, N19)</f>
-        <v>9</v>
-      </c>
-      <c r="R14" s="64" t="str">
-        <f>INDEX(C16:C31, Q14+1, 1)</f>
-        <v>Office Hours</v>
-      </c>
-      <c r="S14" s="69" t="str">
-        <f>INDEX(F30:L33, 1, N19)</f>
-        <v>8:00-8:30</v>
-      </c>
-    </row>
-    <row r="15" spans="2:25">
-      <c r="B15" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="K15" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="L15" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="N15" s="2">
-        <v>41582</v>
-      </c>
-      <c r="O15" s="26"/>
-      <c r="P15" s="43">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="44">
-        <f>INDEX(F16:L19,P15, Q12)</f>
-        <v>6</v>
-      </c>
-      <c r="R15" s="65" t="str">
-        <f>INDEX(C17:C24, Q15, 1)</f>
-        <v>Orchestra</v>
-      </c>
-      <c r="S15" s="70" t="str">
-        <f>INDEX(F34:L37, P15, N19)</f>
-        <v>8:30-9:40</v>
+      <c r="N15" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="O15" s="54"/>
+      <c r="P15" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="Q15" s="48">
+        <f>INDEX(F22:L25, 2, N18)</f>
+        <v>10</v>
+      </c>
+      <c r="R15" s="61" t="str">
+        <f>INDEX(C10:C25, Q15+1, 1)</f>
+        <v>Break</v>
+      </c>
+      <c r="S15" s="66" t="str">
+        <f>INDEX(F29:L32, 2, N18)</f>
+        <v>9:40-9:55</v>
       </c>
     </row>
     <row r="16" spans="2:25">
       <c r="B16" s="18">
-        <v>0</v>
-      </c>
-      <c r="C16" s="46" t="s">
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>10</v>
       </c>
       <c r="E16" s="18">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3">
+        <v>6</v>
+      </c>
+      <c r="H16" s="3">
+        <v>3</v>
+      </c>
+      <c r="I16" s="3">
+        <v>7</v>
+      </c>
+      <c r="J16" s="3">
+        <v>4</v>
+      </c>
+      <c r="K16" s="3">
         <v>1</v>
       </c>
-      <c r="F16" s="3">
-        <v>1</v>
-      </c>
-      <c r="G16" s="3">
+      <c r="L16" s="4">
         <v>5</v>
       </c>
-      <c r="H16" s="3">
+      <c r="N16" s="53">
+        <f>MAX(NETWORKDAYS(N12, N14,N22:N123)-1, 0)</f>
+        <v>52</v>
+      </c>
+      <c r="O16" s="54"/>
+      <c r="P16" s="43">
         <v>2</v>
       </c>
-      <c r="I16" s="3">
-        <v>6</v>
-      </c>
-      <c r="J16" s="3">
-        <v>3</v>
-      </c>
-      <c r="K16" s="3">
-        <v>8</v>
-      </c>
-      <c r="L16" s="4">
-        <v>4</v>
-      </c>
-      <c r="N16" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="O16" s="57"/>
-      <c r="P16" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="Q16" s="48">
-        <f>INDEX(F23:L26, 2, N19)</f>
-        <v>10</v>
-      </c>
-      <c r="R16" s="64" t="str">
-        <f>INDEX(C16:C31, Q16+1, 1)</f>
-        <v>Break</v>
-      </c>
-      <c r="S16" s="69" t="str">
-        <f>INDEX(F30:L33, 2, N19)</f>
-        <v>9:40-9:55</v>
+      <c r="Q16" s="44">
+        <f>INDEX(F15:L18,P16, Q11)</f>
+        <v>7</v>
+      </c>
+      <c r="R16" s="62" t="str">
+        <f>INDEX(C11:C18, Q16, 1)</f>
+        <v>Physics</v>
+      </c>
+      <c r="S16" s="67" t="str">
+        <f>INDEX(F33:L36, P16, N18)</f>
+        <v>9:55-11:05</v>
       </c>
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="18">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="18">
+        <v>3</v>
+      </c>
+      <c r="F17" s="3">
+        <v>3</v>
+      </c>
+      <c r="G17" s="3">
+        <v>8</v>
+      </c>
+      <c r="H17" s="3">
+        <v>4</v>
+      </c>
+      <c r="I17" s="3">
         <v>1</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="J17" s="3">
+        <v>5</v>
+      </c>
+      <c r="K17" s="3">
+        <v>2</v>
+      </c>
+      <c r="L17" s="4">
         <v>6</v>
       </c>
-      <c r="E17" s="18">
+      <c r="N17" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="O17" s="54"/>
+      <c r="P17" s="43">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="44">
+        <f>INDEX(F15:L18,P17, Q11)</f>
+        <v>1</v>
+      </c>
+      <c r="R17" s="62" t="str">
+        <f>INDEX(C11:C18, Q17, 1)</f>
+        <v>History</v>
+      </c>
+      <c r="S17" s="67" t="str">
+        <f>INDEX(F33:L36, P17, N18)</f>
+        <v>11:05-1:10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" ht="15.75" thickBot="1">
+      <c r="B18" s="18">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="20">
+        <v>4</v>
+      </c>
+      <c r="F18" s="5">
+        <v>4</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1</v>
+      </c>
+      <c r="H18" s="5">
+        <v>5</v>
+      </c>
+      <c r="I18" s="5">
         <v>2</v>
       </c>
-      <c r="F17" s="3">
+      <c r="J18" s="5">
+        <v>6</v>
+      </c>
+      <c r="K18" s="5">
+        <v>3</v>
+      </c>
+      <c r="L18" s="6">
+        <v>7</v>
+      </c>
+      <c r="N18" s="21">
+        <f>WEEKDAY(S11)</f>
         <v>2</v>
       </c>
-      <c r="G17" s="3">
-        <v>6</v>
-      </c>
-      <c r="H17" s="3">
-        <v>3</v>
-      </c>
-      <c r="I17" s="3">
-        <v>7</v>
-      </c>
-      <c r="J17" s="3">
-        <v>4</v>
-      </c>
-      <c r="K17" s="3">
-        <v>1</v>
-      </c>
-      <c r="L17" s="4">
-        <v>5</v>
-      </c>
-      <c r="N17" s="53">
-        <f>MAX(NETWORKDAYS(N13, N15,N23:N124)-1, 0)</f>
-        <v>52</v>
-      </c>
-      <c r="O17" s="57"/>
-      <c r="P17" s="43">
-        <v>2</v>
-      </c>
-      <c r="Q17" s="44">
-        <f>INDEX(F16:L19,P17, Q12)</f>
-        <v>7</v>
-      </c>
-      <c r="R17" s="65" t="str">
-        <f>INDEX(C17:C24, Q17, 1)</f>
-        <v>Physics</v>
-      </c>
-      <c r="S17" s="70" t="str">
-        <f>INDEX(F34:L37, P17, N19)</f>
-        <v>9:55-11:05</v>
-      </c>
-    </row>
-    <row r="18" spans="2:19">
-      <c r="B18" s="18">
-        <f>B17+1</f>
-        <v>2</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="18">
-        <v>3</v>
-      </c>
-      <c r="F18" s="3">
-        <v>3</v>
-      </c>
-      <c r="G18" s="3">
-        <v>8</v>
-      </c>
-      <c r="H18" s="3">
-        <v>4</v>
-      </c>
-      <c r="I18" s="3">
-        <v>1</v>
-      </c>
-      <c r="J18" s="3">
-        <v>5</v>
-      </c>
-      <c r="K18" s="3">
-        <v>2</v>
-      </c>
-      <c r="L18" s="4">
-        <v>6</v>
-      </c>
-      <c r="N18" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="O18" s="57"/>
-      <c r="P18" s="43">
-        <v>3</v>
-      </c>
-      <c r="Q18" s="44">
-        <f>INDEX(F16:L19,P18, Q12)</f>
-        <v>1</v>
-      </c>
-      <c r="R18" s="65" t="str">
-        <f>INDEX(C17:C24, Q18, 1)</f>
-        <v>History</v>
-      </c>
-      <c r="S18" s="70" t="str">
-        <f>INDEX(F34:L37, P18, N19)</f>
-        <v>11:05-1:10</v>
+      <c r="O18" s="54"/>
+      <c r="P18" s="22">
+        <v>3.5</v>
+      </c>
+      <c r="Q18" s="48">
+        <f>INDEX(F22:L25, 3, N18)</f>
+        <v>15</v>
+      </c>
+      <c r="R18" s="61" t="str">
+        <f>INDEX(C10:C25, Q18+1, 1)</f>
+        <v>ARTS/ADV</v>
+      </c>
+      <c r="S18" s="66" t="str">
+        <f>INDEX(F29:L32, 3, N18)</f>
+        <v>1:10-1:50</v>
       </c>
     </row>
     <row r="19" spans="2:19" ht="15.75" thickBot="1">
       <c r="B19" s="18">
-        <f t="shared" ref="B19:B31" si="0">B18+1</f>
-        <v>3</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="20">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="O19" s="28"/>
+      <c r="P19" s="43">
         <v>4</v>
       </c>
-      <c r="F19" s="5">
-        <v>4</v>
-      </c>
-      <c r="G19" s="5">
-        <v>1</v>
-      </c>
-      <c r="H19" s="5">
-        <v>5</v>
-      </c>
-      <c r="I19" s="5">
+      <c r="Q19" s="44">
+        <f>INDEX(F15:L18,P19, Q11)</f>
         <v>2</v>
       </c>
-      <c r="J19" s="5">
-        <v>6</v>
-      </c>
-      <c r="K19" s="5">
-        <v>3</v>
-      </c>
-      <c r="L19" s="6">
-        <v>7</v>
-      </c>
-      <c r="N19" s="21">
-        <f>WEEKDAY(S12)</f>
-        <v>2</v>
-      </c>
-      <c r="O19" s="57"/>
-      <c r="P19" s="22">
-        <v>3.5</v>
-      </c>
-      <c r="Q19" s="48">
-        <f>INDEX(F23:L26, 3, N19)</f>
-        <v>15</v>
-      </c>
-      <c r="R19" s="64" t="str">
-        <f>INDEX(C16:C31, Q19+1, 1)</f>
-        <v>ARTS/ADV</v>
-      </c>
-      <c r="S19" s="69" t="str">
-        <f>INDEX(F30:L33, 3, N19)</f>
-        <v>1:10-1:50</v>
+      <c r="R19" s="62" t="str">
+        <f>INDEX(C11:C18, Q19, 1)</f>
+        <v>Math</v>
+      </c>
+      <c r="S19" s="67" t="str">
+        <f>INDEX(F33:L36, P19, N18)</f>
+        <v>1:50-3:00</v>
       </c>
     </row>
     <row r="20" spans="2:19" ht="15.75" thickBot="1">
       <c r="B20" s="18">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="O20" s="28"/>
-      <c r="P20" s="43">
-        <v>4</v>
-      </c>
-      <c r="Q20" s="44">
-        <f>INDEX(F16:L19,P20, Q12)</f>
-        <v>2</v>
-      </c>
-      <c r="R20" s="65" t="str">
-        <f>INDEX(C17:C24, Q20, 1)</f>
-        <v>Math</v>
-      </c>
-      <c r="S20" s="70" t="str">
-        <f>INDEX(F34:L37, P20, N19)</f>
-        <v>1:50-3:00</v>
-      </c>
-    </row>
-    <row r="21" spans="2:19" ht="15.75" thickBot="1">
+        <v>10</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="77" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="78"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="78"/>
+      <c r="L20" s="79"/>
+      <c r="N20" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="O20" s="26"/>
+      <c r="P20" s="23">
+        <v>4.5</v>
+      </c>
+      <c r="Q20" s="49">
+        <f>INDEX(F22:L25, 4, N18)</f>
+        <v>9</v>
+      </c>
+      <c r="R20" s="64" t="str">
+        <f>INDEX(C10:C25, Q20+1, 1)</f>
+        <v>Office Hours</v>
+      </c>
+      <c r="S20" s="68" t="str">
+        <f>INDEX(F29:L32, 4, N18)</f>
+        <v>3:00-3:30</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19">
       <c r="B21" s="18">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21" s="56"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="56"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="56"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="55"/>
-      <c r="N21" s="11" t="s">
-        <v>25</v>
+        <v>11</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="J21" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="K21" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="L21" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="N21" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="O21" s="26"/>
-      <c r="P21" s="23">
-        <v>4.5</v>
-      </c>
-      <c r="Q21" s="49">
-        <f>INDEX(F23:L26, 4, N19)</f>
-        <v>9</v>
-      </c>
-      <c r="R21" s="67" t="str">
-        <f>INDEX(C16:C31, Q21+1, 1)</f>
-        <v>Office Hours</v>
-      </c>
-      <c r="S21" s="71" t="str">
-        <f>INDEX(F30:L33, 4, N19)</f>
-        <v>3:00-3:30</v>
-      </c>
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="18">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="G22" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="H22" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="I22" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="J22" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="K22" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="F22" s="45">
+        <v>0</v>
+      </c>
+      <c r="G22" s="45">
+        <v>9</v>
+      </c>
+      <c r="H22" s="45">
+        <v>13</v>
+      </c>
+      <c r="I22" s="45">
         <v>14</v>
       </c>
-      <c r="L22" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="N22" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="O22" s="26"/>
+      <c r="J22" s="45">
+        <v>13</v>
+      </c>
+      <c r="K22" s="45">
+        <v>9</v>
+      </c>
+      <c r="L22" s="38">
+        <v>0</v>
+      </c>
+      <c r="N22" s="7">
+        <v>41459</v>
+      </c>
+      <c r="O22" s="27"/>
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="18">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>40</v>
       </c>
       <c r="E23" s="50">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="F23" s="45">
         <v>0</v>
       </c>
       <c r="G23" s="45">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H23" s="45">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I23" s="45">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J23" s="45">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K23" s="45">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="L23" s="38">
         <v>0</v>
       </c>
       <c r="N23" s="7">
-        <v>41459</v>
+        <v>41519</v>
       </c>
       <c r="O23" s="27"/>
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="18">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C24" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="50">
+        <v>3.5</v>
+      </c>
+      <c r="F24" s="45">
+        <v>0</v>
+      </c>
+      <c r="G24" s="45">
         <v>15</v>
       </c>
-      <c r="E24" s="50">
-        <v>1.5</v>
-      </c>
-      <c r="F24" s="45">
-        <v>0</v>
-      </c>
-      <c r="G24" s="45">
-        <v>10</v>
-      </c>
       <c r="H24" s="45">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I24" s="45">
         <v>10</v>
       </c>
       <c r="J24" s="45">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K24" s="45">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L24" s="38">
         <v>0</v>
       </c>
       <c r="N24" s="7">
-        <v>41519</v>
+        <v>41561</v>
       </c>
       <c r="O24" s="27"/>
-    </row>
-    <row r="25" spans="2:19">
-      <c r="B25" s="18">
+      <c r="Q24" s="27"/>
+      <c r="S24" s="27"/>
+    </row>
+    <row r="25" spans="2:19" ht="15.75" thickBot="1">
+      <c r="B25" s="20">
         <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="51">
+        <v>4.5</v>
+      </c>
+      <c r="F25" s="52">
+        <v>0</v>
+      </c>
+      <c r="G25" s="52">
         <v>9</v>
       </c>
-      <c r="C25" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="50">
-        <v>3.5</v>
-      </c>
-      <c r="F25" s="45">
-        <v>0</v>
-      </c>
-      <c r="G25" s="45">
-        <v>15</v>
-      </c>
-      <c r="H25" s="45">
-        <v>15</v>
-      </c>
-      <c r="I25" s="45">
-        <v>10</v>
-      </c>
-      <c r="J25" s="45">
-        <v>10</v>
-      </c>
-      <c r="K25" s="45">
-        <v>10</v>
-      </c>
-      <c r="L25" s="38">
+      <c r="H25" s="52">
+        <v>9</v>
+      </c>
+      <c r="I25" s="52">
+        <v>9</v>
+      </c>
+      <c r="J25" s="52">
+        <v>9</v>
+      </c>
+      <c r="K25" s="52">
+        <v>0</v>
+      </c>
+      <c r="L25" s="39">
         <v>0</v>
       </c>
       <c r="N25" s="7">
-        <v>41561</v>
+        <v>41563</v>
       </c>
       <c r="O25" s="27"/>
       <c r="Q25" s="27"/>
       <c r="S25" s="27"/>
     </row>
     <row r="26" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B26" s="18">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C26" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="E26" s="51">
-        <v>4.5</v>
-      </c>
-      <c r="F26" s="52">
-        <v>0</v>
-      </c>
-      <c r="G26" s="52">
-        <v>9</v>
-      </c>
-      <c r="H26" s="52">
-        <v>9</v>
-      </c>
-      <c r="I26" s="52">
-        <v>9</v>
-      </c>
-      <c r="J26" s="52">
-        <v>9</v>
-      </c>
-      <c r="K26" s="52">
-        <v>0</v>
-      </c>
-      <c r="L26" s="39">
-        <v>0</v>
-      </c>
+      <c r="E26" s="30"/>
       <c r="N26" s="7">
-        <v>41563</v>
-      </c>
-      <c r="O26" s="27"/>
-      <c r="Q26" s="27"/>
+        <v>41565</v>
+      </c>
+      <c r="O26" s="28"/>
+      <c r="Q26" s="28"/>
       <c r="S26" s="27"/>
     </row>
     <row r="27" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B27" s="18">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C27" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="30"/>
+      <c r="E27" s="77" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="78"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="78"/>
+      <c r="I27" s="78"/>
+      <c r="J27" s="78"/>
+      <c r="K27" s="78"/>
+      <c r="L27" s="79"/>
       <c r="N27" s="7">
-        <v>41565</v>
-      </c>
-      <c r="O27" s="28"/>
-      <c r="Q27" s="28"/>
-      <c r="S27" s="27"/>
-    </row>
-    <row r="28" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B28" s="18">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C28" s="37" t="s">
+        <v>41575</v>
+      </c>
+      <c r="O27" s="26"/>
+      <c r="Q27" s="26"/>
+    </row>
+    <row r="28" spans="2:19">
+      <c r="E28" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="G28" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="56"/>
-      <c r="J28" s="56"/>
-      <c r="K28" s="56"/>
-      <c r="L28" s="55"/>
+      <c r="H28" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="J28" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="K28" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="L28" s="35" t="s">
+        <v>49</v>
+      </c>
       <c r="N28" s="7">
-        <v>41575</v>
+        <v>41603</v>
       </c>
       <c r="O28" s="26"/>
       <c r="Q28" s="26"/>
+      <c r="S28" s="25"/>
     </row>
     <row r="29" spans="2:19">
-      <c r="B29" s="18">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C29" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F29" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="G29" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="H29" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="I29" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="J29" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="K29" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="L29" s="35" t="s">
-        <v>51</v>
+      <c r="E29" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="F29" s="55">
+        <v>0</v>
+      </c>
+      <c r="G29" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="H29" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="I29" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="J29" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="K29" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="L29" s="56">
+        <v>0</v>
       </c>
       <c r="N29" s="7">
-        <v>41603</v>
-      </c>
-      <c r="O29" s="26"/>
-      <c r="Q29" s="26"/>
-      <c r="S29" s="25"/>
+        <v>41604</v>
+      </c>
+      <c r="O29" s="60"/>
+      <c r="Q29" s="60"/>
+      <c r="S29" s="26"/>
     </row>
     <row r="30" spans="2:19">
-      <c r="B30" s="18">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C30" s="37" t="s">
-        <v>42</v>
-      </c>
       <c r="E30" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="F30" s="58">
-        <v>0</v>
-      </c>
-      <c r="G30" s="58" t="s">
+        <v>1.5</v>
+      </c>
+      <c r="F30" s="55">
+        <v>0</v>
+      </c>
+      <c r="G30" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="H30" s="58" t="s">
-        <v>63</v>
-      </c>
-      <c r="I30" s="58" t="s">
+      <c r="H30" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="I30" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="J30" s="58" t="s">
-        <v>63</v>
-      </c>
-      <c r="K30" s="58" t="s">
+      <c r="J30" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="K30" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="L30" s="59">
+      <c r="L30" s="56">
         <v>0</v>
       </c>
       <c r="N30" s="7">
-        <v>41604</v>
-      </c>
-      <c r="O30" s="63"/>
-      <c r="Q30" s="63"/>
-      <c r="S30" s="26"/>
-    </row>
-    <row r="31" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B31" s="20">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C31" s="33" t="s">
-        <v>39</v>
-      </c>
+        <v>41605</v>
+      </c>
+      <c r="O30" s="60"/>
+      <c r="Q30" s="60"/>
+      <c r="S30" s="27"/>
+    </row>
+    <row r="31" spans="2:19">
       <c r="E31" s="18">
-        <v>1.5</v>
-      </c>
-      <c r="F31" s="58">
-        <v>0</v>
-      </c>
-      <c r="G31" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="H31" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="I31" s="58" t="s">
-        <v>66</v>
-      </c>
-      <c r="J31" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="K31" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="L31" s="59">
+        <v>3.5</v>
+      </c>
+      <c r="F31" s="55">
+        <v>0</v>
+      </c>
+      <c r="G31" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="H31" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="I31" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="J31" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="K31" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="L31" s="56">
         <v>0</v>
       </c>
       <c r="N31" s="7">
-        <v>41605</v>
-      </c>
-      <c r="O31" s="63"/>
-      <c r="Q31" s="63"/>
+        <v>41606</v>
+      </c>
+      <c r="O31" s="60"/>
+      <c r="Q31" s="60"/>
       <c r="S31" s="27"/>
     </row>
     <row r="32" spans="2:19">
       <c r="E32" s="18">
-        <v>3.5</v>
-      </c>
-      <c r="F32" s="58">
-        <v>0</v>
-      </c>
-      <c r="G32" s="58" t="s">
+        <v>4.5</v>
+      </c>
+      <c r="F32" s="55">
+        <v>0</v>
+      </c>
+      <c r="G32" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="H32" s="58" t="s">
+      <c r="H32" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="I32" s="58" t="s">
-        <v>69</v>
-      </c>
-      <c r="J32" s="58" t="s">
-        <v>69</v>
-      </c>
-      <c r="K32" s="58" t="s">
-        <v>71</v>
-      </c>
-      <c r="L32" s="59">
+      <c r="I32" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="J32" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="K32" s="55">
+        <v>0</v>
+      </c>
+      <c r="L32" s="56">
         <v>0</v>
       </c>
       <c r="N32" s="7">
-        <v>41606</v>
-      </c>
-      <c r="O32" s="63"/>
-      <c r="Q32" s="63"/>
+        <v>41607</v>
+      </c>
+      <c r="O32" s="60"/>
+      <c r="Q32" s="60"/>
       <c r="S32" s="27"/>
     </row>
-    <row r="33" spans="5:19">
+    <row r="33" spans="5:17">
       <c r="E33" s="18">
-        <v>4.5</v>
-      </c>
-      <c r="F33" s="58">
-        <v>0</v>
-      </c>
-      <c r="G33" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="H33" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="I33" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="J33" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="K33" s="58">
-        <v>0</v>
-      </c>
-      <c r="L33" s="59">
-        <v>0</v>
-      </c>
-      <c r="N33" s="7">
-        <v>41607</v>
-      </c>
-      <c r="O33" s="63"/>
-      <c r="Q33" s="63"/>
-      <c r="S33" s="27"/>
-    </row>
-    <row r="34" spans="5:19">
+        <v>1</v>
+      </c>
+      <c r="F33" s="55">
+        <v>0</v>
+      </c>
+      <c r="G33" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="H33" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I33" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="J33" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="K33" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="L33" s="56">
+        <v>0</v>
+      </c>
+      <c r="N33" s="7"/>
+      <c r="O33" s="60"/>
+      <c r="Q33" s="60"/>
+    </row>
+    <row r="34" spans="5:17">
       <c r="E34" s="18">
-        <v>1</v>
-      </c>
-      <c r="F34" s="58">
-        <v>0</v>
-      </c>
-      <c r="G34" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" s="55">
+        <v>0</v>
+      </c>
+      <c r="G34" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="H34" s="58" t="s">
+      <c r="H34" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="I34" s="58" t="s">
+      <c r="I34" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="J34" s="58" t="s">
+      <c r="J34" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="K34" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K34" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="L34" s="59">
+      <c r="L34" s="56">
         <v>0</v>
       </c>
       <c r="N34" s="7"/>
-      <c r="O34" s="63"/>
-      <c r="Q34" s="63"/>
-    </row>
-    <row r="35" spans="5:19">
+      <c r="O34" s="60"/>
+      <c r="Q34" s="60"/>
+    </row>
+    <row r="35" spans="5:17">
       <c r="E35" s="18">
-        <v>2</v>
-      </c>
-      <c r="F35" s="58">
-        <v>0</v>
-      </c>
-      <c r="G35" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="H35" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="I35" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="J35" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="K35" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="L35" s="59">
+        <v>3</v>
+      </c>
+      <c r="F35" s="55">
+        <v>0</v>
+      </c>
+      <c r="G35" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="H35" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I35" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="J35" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="K35" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="L35" s="56">
         <v>0</v>
       </c>
       <c r="N35" s="7"/>
-      <c r="O35" s="63"/>
-      <c r="Q35" s="63"/>
-    </row>
-    <row r="36" spans="5:19">
-      <c r="E36" s="18">
-        <v>3</v>
-      </c>
-      <c r="F36" s="58">
-        <v>0</v>
-      </c>
-      <c r="G36" s="58" t="s">
+      <c r="O35" s="60"/>
+      <c r="Q35" s="60"/>
+    </row>
+    <row r="36" spans="5:17" ht="15.75" thickBot="1">
+      <c r="E36" s="20">
+        <v>4</v>
+      </c>
+      <c r="F36" s="57">
+        <v>0</v>
+      </c>
+      <c r="G36" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="H36" s="58" t="s">
+      <c r="H36" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="I36" s="58" t="s">
-        <v>68</v>
-      </c>
-      <c r="J36" s="58" t="s">
-        <v>68</v>
-      </c>
-      <c r="K36" s="58" t="s">
+      <c r="I36" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="L36" s="59">
+      <c r="J36" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="K36" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="L36" s="58">
         <v>0</v>
       </c>
       <c r="N36" s="7"/>
-      <c r="O36" s="63"/>
-      <c r="Q36" s="63"/>
-    </row>
-    <row r="37" spans="5:19" ht="15.75" thickBot="1">
-      <c r="E37" s="20">
-        <v>4</v>
-      </c>
-      <c r="F37" s="60">
-        <v>0</v>
-      </c>
-      <c r="G37" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="H37" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="I37" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="J37" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="K37" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="L37" s="61">
-        <v>0</v>
-      </c>
+      <c r="O36" s="60"/>
+      <c r="Q36" s="60"/>
+    </row>
+    <row r="37" spans="5:17">
       <c r="N37" s="7"/>
-      <c r="O37" s="63"/>
-      <c r="Q37" s="63"/>
-    </row>
-    <row r="38" spans="5:19">
+    </row>
+    <row r="38" spans="5:17">
       <c r="N38" s="7"/>
     </row>
-    <row r="39" spans="5:19">
+    <row r="39" spans="5:17">
       <c r="N39" s="7"/>
     </row>
-    <row r="40" spans="5:19">
+    <row r="40" spans="5:17">
       <c r="N40" s="7"/>
     </row>
-    <row r="41" spans="5:19">
+    <row r="41" spans="5:17">
       <c r="N41" s="7"/>
     </row>
-    <row r="42" spans="5:19">
+    <row r="42" spans="5:17">
       <c r="N42" s="7"/>
     </row>
-    <row r="43" spans="5:19">
+    <row r="43" spans="5:17">
       <c r="N43" s="7"/>
     </row>
-    <row r="44" spans="5:19">
+    <row r="44" spans="5:17">
       <c r="N44" s="7"/>
     </row>
-    <row r="45" spans="5:19">
+    <row r="45" spans="5:17">
       <c r="N45" s="7"/>
     </row>
-    <row r="46" spans="5:19">
+    <row r="46" spans="5:17">
       <c r="N46" s="7"/>
     </row>
-    <row r="47" spans="5:19">
+    <row r="47" spans="5:17">
       <c r="N47" s="7"/>
     </row>
-    <row r="48" spans="5:19">
+    <row r="48" spans="5:17">
       <c r="N48" s="7"/>
     </row>
     <row r="49" spans="14:14">
@@ -2724,7 +2720,7 @@
       <c r="N64" s="7"/>
     </row>
     <row r="65" spans="14:14">
-      <c r="N65" s="7"/>
+      <c r="N65" s="1"/>
     </row>
     <row r="66" spans="14:14">
       <c r="N66" s="1"/>
@@ -2897,36 +2893,33 @@
     <row r="122" spans="14:14">
       <c r="N122" s="1"/>
     </row>
-    <row r="123" spans="14:14">
-      <c r="N123" s="1"/>
-    </row>
-    <row r="124" spans="14:14" ht="15.75" thickBot="1">
-      <c r="N124" s="8"/>
+    <row r="123" spans="14:14" ht="15.75" thickBot="1">
+      <c r="N123" s="8"/>
     </row>
   </sheetData>
   <sheetProtection password="C836" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
   <mergeCells count="21">
+    <mergeCell ref="E27:L27"/>
+    <mergeCell ref="H10:J11"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="L3:R4"/>
+    <mergeCell ref="L5:R7"/>
+    <mergeCell ref="E4:G5"/>
+    <mergeCell ref="H4:J5"/>
+    <mergeCell ref="E6:G7"/>
+    <mergeCell ref="E8:G9"/>
+    <mergeCell ref="E10:G11"/>
+    <mergeCell ref="H6:J7"/>
+    <mergeCell ref="H8:J9"/>
+    <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="P11:S11"/>
-    <mergeCell ref="E14:L14"/>
-    <mergeCell ref="E21:L21"/>
-    <mergeCell ref="E28:L28"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="H11:J12"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E3:J3"/>
-    <mergeCell ref="L4:R5"/>
-    <mergeCell ref="L6:R8"/>
-    <mergeCell ref="L3:R3"/>
-    <mergeCell ref="E5:G6"/>
-    <mergeCell ref="H5:J6"/>
-    <mergeCell ref="E7:G8"/>
-    <mergeCell ref="E9:G10"/>
-    <mergeCell ref="E11:G12"/>
-    <mergeCell ref="H7:J8"/>
-    <mergeCell ref="H9:J10"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="E13:L13"/>
+    <mergeCell ref="E20:L20"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="L2:R2"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2968,194 +2961,216 @@
   <sheetData>
     <row r="1" spans="2:25" ht="15.75" thickBot="1">
       <c r="D1" s="9"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
     </row>
     <row r="2" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B2" s="87" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="54" t="s">
+      <c r="B2" s="73" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="74"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="55"/>
-      <c r="L2" s="54" t="s">
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="79"/>
+      <c r="L2" s="77" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="79"/>
+    </row>
+    <row r="3" spans="2:25" ht="15.75" thickBot="1">
+      <c r="B3" s="75" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="76"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="89" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="86" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="87"/>
+      <c r="J3" s="88"/>
+      <c r="L3" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="55"/>
-    </row>
-    <row r="3" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B3" s="89" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="75" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="92" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="98"/>
-      <c r="J3" s="99"/>
-      <c r="L3" s="83" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="84"/>
-      <c r="N3" s="84"/>
-      <c r="O3" s="84"/>
-      <c r="P3" s="84"/>
-      <c r="Q3" s="84"/>
-      <c r="R3" s="85"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="92"/>
+      <c r="O3" s="92"/>
+      <c r="P3" s="92"/>
+      <c r="Q3" s="92"/>
+      <c r="R3" s="93"/>
       <c r="X3" s="29"/>
       <c r="Y3" s="29"/>
     </row>
     <row r="4" spans="2:25">
-      <c r="D4" s="74"/>
-      <c r="E4" s="78" t="s">
-        <v>77</v>
-      </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="91" t="s">
-        <v>73</v>
-      </c>
-      <c r="I4" s="93"/>
-      <c r="J4" s="94"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="76"/>
-      <c r="N4" s="76"/>
-      <c r="O4" s="76"/>
-      <c r="P4" s="76"/>
-      <c r="Q4" s="76"/>
-      <c r="R4" s="79"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="94" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="95"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="80" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="81"/>
+      <c r="J4" s="82"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="95"/>
+      <c r="N4" s="95"/>
+      <c r="O4" s="95"/>
+      <c r="P4" s="95"/>
+      <c r="Q4" s="95"/>
+      <c r="R4" s="96"/>
       <c r="X4" s="29"/>
       <c r="Y4" s="29"/>
     </row>
     <row r="5" spans="2:25">
-      <c r="D5" s="74"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="95"/>
-      <c r="I5" s="96"/>
-      <c r="J5" s="97"/>
-      <c r="L5" s="78" t="s">
-        <v>53</v>
-      </c>
-      <c r="M5" s="76"/>
-      <c r="N5" s="76"/>
-      <c r="O5" s="76"/>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="76"/>
-      <c r="R5" s="79"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="102"/>
+      <c r="L5" s="94" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" s="95"/>
+      <c r="N5" s="95"/>
+      <c r="O5" s="95"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="95"/>
+      <c r="R5" s="96"/>
       <c r="X5" s="29"/>
       <c r="Y5" s="29"/>
     </row>
     <row r="6" spans="2:25">
-      <c r="D6" s="74"/>
-      <c r="E6" s="78" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" s="76"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="91" t="s">
-        <v>80</v>
-      </c>
-      <c r="I6" s="93"/>
-      <c r="J6" s="94"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="76"/>
-      <c r="N6" s="76"/>
-      <c r="O6" s="76"/>
-      <c r="P6" s="76"/>
-      <c r="Q6" s="76"/>
-      <c r="R6" s="79"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="94" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="95"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="80" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" s="81"/>
+      <c r="J6" s="82"/>
+      <c r="L6" s="94"/>
+      <c r="M6" s="95"/>
+      <c r="N6" s="95"/>
+      <c r="O6" s="95"/>
+      <c r="P6" s="95"/>
+      <c r="Q6" s="95"/>
+      <c r="R6" s="96"/>
       <c r="X6" s="29"/>
       <c r="Y6" s="29"/>
     </row>
     <row r="7" spans="2:25" ht="15.75" thickBot="1">
-      <c r="D7" s="74"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="95"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="97"/>
-      <c r="L7" s="80"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="81"/>
-      <c r="O7" s="81"/>
-      <c r="P7" s="81"/>
-      <c r="Q7" s="81"/>
-      <c r="R7" s="82"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="102"/>
+      <c r="L7" s="97"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="98"/>
+      <c r="O7" s="98"/>
+      <c r="P7" s="98"/>
+      <c r="Q7" s="98"/>
+      <c r="R7" s="99"/>
       <c r="X7" s="29"/>
       <c r="Y7" s="29"/>
     </row>
-    <row r="8" spans="2:25">
-      <c r="D8" s="74"/>
-      <c r="E8" s="78" t="s">
+    <row r="8" spans="2:25" ht="15.75" thickBot="1">
+      <c r="B8" s="77" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="79"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="94" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="95"/>
+      <c r="G8" s="95"/>
+      <c r="H8" s="80" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="81"/>
+      <c r="J8" s="82"/>
+    </row>
+    <row r="9" spans="2:25" ht="15.75" thickBot="1">
+      <c r="B9" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="94"/>
+      <c r="F9" s="95"/>
+      <c r="G9" s="95"/>
+      <c r="H9" s="100"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="102"/>
+    </row>
+    <row r="10" spans="2:25" ht="15.75" thickBot="1">
+      <c r="B10" s="18">
+        <v>0</v>
+      </c>
+      <c r="C10" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="91" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="93"/>
-      <c r="J8" s="94"/>
-    </row>
-    <row r="9" spans="2:25" ht="15.75" thickBot="1">
-      <c r="E9" s="78"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="95"/>
-      <c r="I9" s="96"/>
-      <c r="J9" s="97"/>
-    </row>
-    <row r="10" spans="2:25" ht="15.75" thickBot="1">
-      <c r="E10" s="78" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="76"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="91" t="s">
+      <c r="E10" s="94" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="95"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="93"/>
-      <c r="J10" s="94"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="82"/>
       <c r="N10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="P10" s="54" t="s">
+      <c r="P10" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="56"/>
-      <c r="S10" s="55"/>
+      <c r="Q10" s="78"/>
+      <c r="R10" s="78"/>
+      <c r="S10" s="79"/>
     </row>
     <row r="11" spans="2:25" ht="15.75" thickBot="1">
-      <c r="E11" s="80"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="100"/>
-      <c r="I11" s="101"/>
-      <c r="J11" s="102"/>
+      <c r="B11" s="18">
+        <v>1</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="97"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="83"/>
+      <c r="I11" s="84"/>
+      <c r="J11" s="85"/>
       <c r="N11" s="14" t="s">
         <v>11</v>
       </c>
@@ -3163,19 +3178,26 @@
         <f>INDEX(F14:L14, 1, Q11)</f>
         <v>G</v>
       </c>
-      <c r="Q11" s="62">
+      <c r="Q11" s="59">
         <f>MOD(N16, 7)+1</f>
         <v>7</v>
       </c>
-      <c r="R11" s="73" t="s">
-        <v>74</v>
-      </c>
-      <c r="S11" s="72">
+      <c r="R11" s="70" t="s">
+        <v>72</v>
+      </c>
+      <c r="S11" s="69">
         <f>N14</f>
         <v>41773</v>
       </c>
     </row>
     <row r="12" spans="2:25" ht="15.75" thickBot="1">
+      <c r="B12" s="18">
+        <f>B11+1</f>
+        <v>2</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>5</v>
+      </c>
       <c r="N12" s="2">
         <v>41645</v>
       </c>
@@ -3185,30 +3207,33 @@
       <c r="Q12" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="R12" s="66" t="s">
+      <c r="R12" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="S12" s="68" t="s">
-        <v>75</v>
+      <c r="S12" s="65" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B13" s="54" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="55"/>
-      <c r="E13" s="54" t="s">
+      <c r="B13" s="18">
+        <f t="shared" ref="B13:B25" si="0">B12+1</f>
+        <v>3</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="55"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="78"/>
+      <c r="I13" s="78"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="78"/>
+      <c r="L13" s="79"/>
       <c r="N13" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O13" s="26"/>
       <c r="P13" s="22">
@@ -3218,21 +3243,22 @@
         <f>INDEX(F22:L25, 1, N18)</f>
         <v>14</v>
       </c>
-      <c r="R13" s="64" t="str">
-        <f>INDEX(C15:C30, Q13+1, 1)</f>
+      <c r="R13" s="61" t="str">
+        <f>INDEX(C10:C25, Q13+1, 1)</f>
         <v>FAC MTGS</v>
       </c>
-      <c r="S13" s="69" t="str">
+      <c r="S13" s="66" t="str">
         <f>INDEX(F29:L32, 1, N18)</f>
         <v>7:45-9:00</v>
       </c>
     </row>
     <row r="14" spans="2:25">
-      <c r="B14" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>3</v>
+      <c r="B14" s="18">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>8</v>
       </c>
       <c r="E14" s="24" t="s">
         <v>1</v>
@@ -3269,21 +3295,22 @@
         <f>INDEX(F15:L18,P14, Q11)</f>
         <v>4</v>
       </c>
-      <c r="R14" s="65" t="str">
-        <f>INDEX(C16:C23, Q14, 1)</f>
+      <c r="R14" s="62" t="str">
+        <f>INDEX(C11:C18, Q14, 1)</f>
         <v>Bible</v>
       </c>
-      <c r="S14" s="70" t="str">
+      <c r="S14" s="67" t="str">
         <f>INDEX(F33:L36, P14, N18)</f>
         <v>9:00-10:10</v>
       </c>
     </row>
     <row r="15" spans="2:25">
       <c r="B15" s="18">
-        <v>0</v>
-      </c>
-      <c r="C15" s="46" t="s">
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="E15" s="18">
         <v>1</v>
@@ -3312,7 +3339,7 @@
       <c r="N15" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="O15" s="57"/>
+      <c r="O15" s="54"/>
       <c r="P15" s="22">
         <v>1.5</v>
       </c>
@@ -3320,21 +3347,22 @@
         <f>INDEX(F22:L25, 2, N18)</f>
         <v>10</v>
       </c>
-      <c r="R15" s="64" t="str">
-        <f>INDEX(C15:C30, Q15+1, 1)</f>
+      <c r="R15" s="61" t="str">
+        <f>INDEX(C10:C25, Q15+1, 1)</f>
         <v>Break</v>
       </c>
-      <c r="S15" s="69" t="str">
+      <c r="S15" s="66" t="str">
         <f>INDEX(F29:L32, 2, N18)</f>
         <v>10:10-10:25</v>
       </c>
     </row>
     <row r="16" spans="2:25">
       <c r="B16" s="18">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E16" s="18">
         <v>2</v>
@@ -3364,7 +3392,7 @@
         <f>MAX(NETWORKDAYS(N12, N14,N22:N123)-1, 0)</f>
         <v>83</v>
       </c>
-      <c r="O16" s="57"/>
+      <c r="O16" s="54"/>
       <c r="P16" s="43">
         <v>2</v>
       </c>
@@ -3372,22 +3400,22 @@
         <f>INDEX(F15:L18,P16, Q11)</f>
         <v>5</v>
       </c>
-      <c r="R16" s="65" t="str">
-        <f>INDEX(C16:C23, Q16, 1)</f>
+      <c r="R16" s="62" t="str">
+        <f>INDEX(C11:C18, Q16, 1)</f>
         <v>English</v>
       </c>
-      <c r="S16" s="70" t="str">
+      <c r="S16" s="67" t="str">
         <f>INDEX(F33:L36, P16, N18)</f>
         <v>10:25-11:35</v>
       </c>
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="18">
-        <f>B16+1</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E17" s="18">
         <v>3</v>
@@ -3414,9 +3442,9 @@
         <v>6</v>
       </c>
       <c r="N17" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="O17" s="57"/>
+        <v>48</v>
+      </c>
+      <c r="O17" s="54"/>
       <c r="P17" s="43">
         <v>3</v>
       </c>
@@ -3424,22 +3452,22 @@
         <f>INDEX(F15:L18,P17, Q11)</f>
         <v>6</v>
       </c>
-      <c r="R17" s="65" t="str">
-        <f>INDEX(C16:C23, Q17, 1)</f>
+      <c r="R17" s="62" t="str">
+        <f>INDEX(C11:C18, Q17, 1)</f>
         <v>Orchestra</v>
       </c>
-      <c r="S17" s="70" t="str">
+      <c r="S17" s="67" t="str">
         <f>INDEX(F33:L36, P17, N18)</f>
         <v>11:35-1:40</v>
       </c>
     </row>
     <row r="18" spans="2:19" ht="15.75" thickBot="1">
       <c r="B18" s="18">
-        <f t="shared" ref="B18:B30" si="0">B17+1</f>
-        <v>3</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>15</v>
       </c>
       <c r="E18" s="20">
         <v>4</v>
@@ -3469,7 +3497,7 @@
         <f>WEEKDAY(S11)</f>
         <v>4</v>
       </c>
-      <c r="O18" s="57"/>
+      <c r="O18" s="54"/>
       <c r="P18" s="22">
         <v>3.5</v>
       </c>
@@ -3477,11 +3505,11 @@
         <f>INDEX(F22:L25, 3, N18)</f>
         <v>10</v>
       </c>
-      <c r="R18" s="64" t="str">
-        <f>INDEX(C15:C30, Q18+1, 1)</f>
+      <c r="R18" s="61" t="str">
+        <f>INDEX(C10:C25, Q18+1, 1)</f>
         <v>Break</v>
       </c>
-      <c r="S18" s="69" t="str">
+      <c r="S18" s="66" t="str">
         <f>INDEX(F29:L32, 3, N18)</f>
         <v>1:40-1:50</v>
       </c>
@@ -3489,10 +3517,10 @@
     <row r="19" spans="2:19" ht="15.75" thickBot="1">
       <c r="B19" s="18">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>36</v>
       </c>
       <c r="O19" s="28"/>
       <c r="P19" s="43">
@@ -3502,11 +3530,11 @@
         <f>INDEX(F15:L18,P19, Q11)</f>
         <v>7</v>
       </c>
-      <c r="R19" s="65" t="str">
-        <f>INDEX(C16:C23, Q19, 1)</f>
+      <c r="R19" s="62" t="str">
+        <f>INDEX(C11:C18, Q19, 1)</f>
         <v>Physics</v>
       </c>
-      <c r="S19" s="70" t="str">
+      <c r="S19" s="67" t="str">
         <f>INDEX(F33:L36, P19, N18)</f>
         <v>1:50-3:00</v>
       </c>
@@ -3514,21 +3542,21 @@
     <row r="20" spans="2:19" ht="15.75" thickBot="1">
       <c r="B20" s="18">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="55"/>
+        <v>10</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="77" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="78"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="78"/>
+      <c r="L20" s="79"/>
       <c r="N20" s="11" t="s">
         <v>25</v>
       </c>
@@ -3540,11 +3568,11 @@
         <f>INDEX(F22:L25, 4, N18)</f>
         <v>9</v>
       </c>
-      <c r="R20" s="67" t="str">
-        <f>INDEX(C15:C30, Q20+1, 1)</f>
+      <c r="R20" s="64" t="str">
+        <f>INDEX(C10:C25, Q20+1, 1)</f>
         <v>Office Hours</v>
       </c>
-      <c r="S20" s="71" t="str">
+      <c r="S20" s="68" t="str">
         <f>INDEX(F29:L32, 4, N18)</f>
         <v>3:00-3:30</v>
       </c>
@@ -3552,34 +3580,34 @@
     <row r="21" spans="2:19">
       <c r="B21" s="18">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>39</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G21" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="H21" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="I21" s="34" t="s">
+      <c r="J21" s="34" t="s">
         <v>45</v>
-      </c>
-      <c r="J21" s="34" t="s">
-        <v>46</v>
       </c>
       <c r="K21" s="34" t="s">
         <v>14</v>
       </c>
       <c r="L21" s="35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="N21" s="13" t="s">
         <v>0</v>
@@ -3589,10 +3617,10 @@
     <row r="22" spans="2:19">
       <c r="B22" s="18">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>42</v>
       </c>
       <c r="E22" s="50">
         <v>0.5</v>
@@ -3626,10 +3654,10 @@
     <row r="23" spans="2:19">
       <c r="B23" s="18">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>40</v>
       </c>
       <c r="E23" s="50">
         <v>1.5</v>
@@ -3663,10 +3691,10 @@
     <row r="24" spans="2:19">
       <c r="B24" s="18">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E24" s="50">
         <v>3.5</v>
@@ -3700,11 +3728,11 @@
       <c r="S24" s="27"/>
     </row>
     <row r="25" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B25" s="18">
+      <c r="B25" s="20">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C25" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="33" t="s">
         <v>38</v>
       </c>
       <c r="E25" s="51">
@@ -3739,13 +3767,6 @@
       <c r="S25" s="27"/>
     </row>
     <row r="26" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B26" s="18">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C26" s="37" t="s">
-        <v>40</v>
-      </c>
       <c r="E26" s="30"/>
       <c r="N26" s="7">
         <v>41708</v>
@@ -3755,23 +3776,16 @@
       <c r="S26" s="27"/>
     </row>
     <row r="27" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B27" s="18">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C27" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="F27" s="56"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="56"/>
-      <c r="J27" s="56"/>
-      <c r="K27" s="56"/>
-      <c r="L27" s="55"/>
+      <c r="E27" s="77" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="78"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="78"/>
+      <c r="I27" s="78"/>
+      <c r="J27" s="78"/>
+      <c r="K27" s="78"/>
+      <c r="L27" s="79"/>
       <c r="N27" s="7">
         <v>41709</v>
       </c>
@@ -3779,36 +3793,29 @@
       <c r="Q27" s="26"/>
     </row>
     <row r="28" spans="2:19">
-      <c r="B28" s="18">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C28" s="37" t="s">
-        <v>41</v>
-      </c>
       <c r="E28" s="15" t="s">
         <v>1</v>
       </c>
       <c r="F28" s="34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G28" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="H28" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="H28" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="I28" s="34" t="s">
+      <c r="J28" s="34" t="s">
         <v>45</v>
-      </c>
-      <c r="J28" s="34" t="s">
-        <v>46</v>
       </c>
       <c r="K28" s="34" t="s">
         <v>14</v>
       </c>
       <c r="L28" s="35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="N28" s="7">
         <v>41710</v>
@@ -3818,270 +3825,256 @@
       <c r="S28" s="25"/>
     </row>
     <row r="29" spans="2:19">
-      <c r="B29" s="18">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C29" s="37" t="s">
-        <v>42</v>
-      </c>
       <c r="E29" s="18">
         <v>0.5</v>
       </c>
-      <c r="F29" s="58">
-        <v>0</v>
-      </c>
-      <c r="G29" s="58" t="s">
-        <v>55</v>
-      </c>
-      <c r="H29" s="58" t="s">
-        <v>63</v>
-      </c>
-      <c r="I29" s="58" t="s">
-        <v>64</v>
-      </c>
-      <c r="J29" s="58" t="s">
-        <v>63</v>
-      </c>
-      <c r="K29" s="58" t="s">
-        <v>55</v>
-      </c>
-      <c r="L29" s="59">
+      <c r="F29" s="55">
+        <v>0</v>
+      </c>
+      <c r="G29" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="H29" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="I29" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="J29" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="K29" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="L29" s="56">
         <v>0</v>
       </c>
       <c r="N29" s="7">
         <v>41711</v>
       </c>
-      <c r="O29" s="63"/>
-      <c r="Q29" s="63"/>
+      <c r="O29" s="60"/>
+      <c r="Q29" s="60"/>
       <c r="S29" s="26"/>
     </row>
-    <row r="30" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B30" s="20">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>39</v>
-      </c>
+    <row r="30" spans="2:19">
       <c r="E30" s="18">
         <v>1.5</v>
       </c>
-      <c r="F30" s="58">
-        <v>0</v>
-      </c>
-      <c r="G30" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="H30" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="I30" s="58" t="s">
-        <v>66</v>
-      </c>
-      <c r="J30" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="K30" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="L30" s="59">
+      <c r="F30" s="55">
+        <v>0</v>
+      </c>
+      <c r="G30" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="H30" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="I30" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="J30" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="K30" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="L30" s="56">
         <v>0</v>
       </c>
       <c r="N30" s="7">
         <v>41712</v>
       </c>
-      <c r="O30" s="63"/>
-      <c r="Q30" s="63"/>
+      <c r="O30" s="60"/>
+      <c r="Q30" s="60"/>
       <c r="S30" s="27"/>
     </row>
     <row r="31" spans="2:19">
       <c r="E31" s="18">
         <v>3.5</v>
       </c>
-      <c r="F31" s="58">
-        <v>0</v>
-      </c>
-      <c r="G31" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="H31" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="I31" s="58" t="s">
+      <c r="F31" s="55">
+        <v>0</v>
+      </c>
+      <c r="G31" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="H31" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="I31" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="J31" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="K31" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="J31" s="58" t="s">
-        <v>69</v>
-      </c>
-      <c r="K31" s="58" t="s">
-        <v>71</v>
-      </c>
-      <c r="L31" s="59">
+      <c r="L31" s="56">
         <v>0</v>
       </c>
       <c r="N31" s="7">
         <v>41713</v>
       </c>
-      <c r="O31" s="63"/>
-      <c r="Q31" s="63"/>
+      <c r="O31" s="60"/>
+      <c r="Q31" s="60"/>
       <c r="S31" s="27"/>
     </row>
     <row r="32" spans="2:19">
       <c r="E32" s="18">
         <v>4.5</v>
       </c>
-      <c r="F32" s="58">
-        <v>0</v>
-      </c>
-      <c r="G32" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="H32" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="I32" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="J32" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="K32" s="58">
-        <v>0</v>
-      </c>
-      <c r="L32" s="59">
+      <c r="F32" s="55">
+        <v>0</v>
+      </c>
+      <c r="G32" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="H32" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="I32" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="J32" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="K32" s="55">
+        <v>0</v>
+      </c>
+      <c r="L32" s="56">
         <v>0</v>
       </c>
       <c r="N32" s="7">
         <v>41714</v>
       </c>
-      <c r="O32" s="63"/>
-      <c r="Q32" s="63"/>
+      <c r="O32" s="60"/>
+      <c r="Q32" s="60"/>
       <c r="S32" s="27"/>
     </row>
     <row r="33" spans="5:17">
       <c r="E33" s="18">
         <v>1</v>
       </c>
-      <c r="F33" s="58">
-        <v>0</v>
-      </c>
-      <c r="G33" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="H33" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="I33" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="J33" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="K33" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="L33" s="59">
+      <c r="F33" s="55">
+        <v>0</v>
+      </c>
+      <c r="G33" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="H33" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I33" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="J33" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="K33" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="L33" s="56">
         <v>0</v>
       </c>
       <c r="N33" s="7">
         <v>41747</v>
       </c>
-      <c r="O33" s="63"/>
-      <c r="Q33" s="63"/>
+      <c r="O33" s="60"/>
+      <c r="Q33" s="60"/>
     </row>
     <row r="34" spans="5:17">
       <c r="E34" s="18">
         <v>2</v>
       </c>
-      <c r="F34" s="58">
-        <v>0</v>
-      </c>
-      <c r="G34" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="H34" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="I34" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="J34" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="K34" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="L34" s="59">
+      <c r="F34" s="55">
+        <v>0</v>
+      </c>
+      <c r="G34" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="H34" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="I34" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="J34" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="K34" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="L34" s="56">
         <v>0</v>
       </c>
       <c r="N34" s="7">
         <v>41748</v>
       </c>
-      <c r="O34" s="63"/>
-      <c r="Q34" s="63"/>
+      <c r="O34" s="60"/>
+      <c r="Q34" s="60"/>
     </row>
     <row r="35" spans="5:17">
       <c r="E35" s="18">
         <v>3</v>
       </c>
-      <c r="F35" s="58">
-        <v>0</v>
-      </c>
-      <c r="G35" s="58" t="s">
-        <v>59</v>
-      </c>
-      <c r="H35" s="58" t="s">
-        <v>59</v>
-      </c>
-      <c r="I35" s="58" t="s">
-        <v>68</v>
-      </c>
-      <c r="J35" s="58" t="s">
-        <v>68</v>
-      </c>
-      <c r="K35" s="58" t="s">
-        <v>59</v>
-      </c>
-      <c r="L35" s="59">
+      <c r="F35" s="55">
+        <v>0</v>
+      </c>
+      <c r="G35" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="H35" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I35" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="J35" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="K35" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="L35" s="56">
         <v>0</v>
       </c>
       <c r="N35" s="7">
         <v>41749</v>
       </c>
-      <c r="O35" s="63"/>
-      <c r="Q35" s="63"/>
+      <c r="O35" s="60"/>
+      <c r="Q35" s="60"/>
     </row>
     <row r="36" spans="5:17" ht="15.75" thickBot="1">
       <c r="E36" s="20">
         <v>4</v>
       </c>
-      <c r="F36" s="60">
-        <v>0</v>
-      </c>
-      <c r="G36" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="H36" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="I36" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="J36" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="K36" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="L36" s="61">
+      <c r="F36" s="57">
+        <v>0</v>
+      </c>
+      <c r="G36" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="H36" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="I36" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="J36" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="K36" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="L36" s="58">
         <v>0</v>
       </c>
       <c r="N36" s="7">
         <v>41750</v>
       </c>
-      <c r="O36" s="63"/>
-      <c r="Q36" s="63"/>
+      <c r="O36" s="60"/>
+      <c r="Q36" s="60"/>
     </row>
     <row r="37" spans="5:17">
       <c r="N37" s="7"/>
@@ -4345,19 +4338,9 @@
       <c r="N123" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection password="C836" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="C836" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
   <mergeCells count="21">
-    <mergeCell ref="P10:S10"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E13:L13"/>
-    <mergeCell ref="E20:L20"/>
-    <mergeCell ref="E27:L27"/>
-    <mergeCell ref="E6:G7"/>
-    <mergeCell ref="H6:J7"/>
-    <mergeCell ref="E8:G9"/>
-    <mergeCell ref="H8:J9"/>
-    <mergeCell ref="E10:G11"/>
-    <mergeCell ref="H10:J11"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:J2"/>
     <mergeCell ref="L2:R2"/>
@@ -4368,6 +4351,16 @@
     <mergeCell ref="E4:G5"/>
     <mergeCell ref="H4:J5"/>
     <mergeCell ref="L5:R7"/>
+    <mergeCell ref="E6:G7"/>
+    <mergeCell ref="H6:J7"/>
+    <mergeCell ref="E8:G9"/>
+    <mergeCell ref="H8:J9"/>
+    <mergeCell ref="E10:G11"/>
+    <mergeCell ref="H10:J11"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="E13:L13"/>
+    <mergeCell ref="E20:L20"/>
+    <mergeCell ref="E27:L27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added support for naming the days of the week
</commit_message>
<xml_diff>
--- a/WMS_Scheduler.xlsx
+++ b/WMS_Scheduler.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="81">
   <si>
     <t>Holidays</t>
   </si>
@@ -294,9 +294,6 @@
       </rPr>
       <t xml:space="preserve"> Areas</t>
     </r>
-  </si>
-  <si>
-    <t>Day</t>
   </si>
   <si>
     <t>Time</t>
@@ -1137,18 +1134,6 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1207,6 +1192,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1534,155 +1531,155 @@
   <sheetData>
     <row r="1" spans="2:25" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="74"/>
+      <c r="C2" s="100"/>
       <c r="D2" s="71"/>
-      <c r="E2" s="77" t="s">
+      <c r="E2" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="79"/>
-      <c r="L2" s="77" t="s">
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="75"/>
+      <c r="L2" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="79"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="75"/>
     </row>
     <row r="3" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="76"/>
+      <c r="C3" s="102"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="89" t="s">
+      <c r="E3" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="86" t="s">
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="87"/>
-      <c r="J3" s="88"/>
-      <c r="L3" s="91" t="s">
+      <c r="I3" s="83"/>
+      <c r="J3" s="84"/>
+      <c r="L3" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="92"/>
-      <c r="N3" s="92"/>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="93"/>
+      <c r="M3" s="88"/>
+      <c r="N3" s="88"/>
+      <c r="O3" s="88"/>
+      <c r="P3" s="88"/>
+      <c r="Q3" s="88"/>
+      <c r="R3" s="89"/>
       <c r="X3" s="29"/>
       <c r="Y3" s="29"/>
     </row>
     <row r="4" spans="2:25">
       <c r="D4" s="71"/>
-      <c r="E4" s="94" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" s="95"/>
-      <c r="G4" s="95"/>
-      <c r="H4" s="80" t="s">
+      <c r="E4" s="90" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="I4" s="81"/>
-      <c r="J4" s="82"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="95"/>
-      <c r="N4" s="95"/>
-      <c r="O4" s="95"/>
-      <c r="P4" s="95"/>
-      <c r="Q4" s="95"/>
-      <c r="R4" s="96"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="78"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="91"/>
+      <c r="Q4" s="91"/>
+      <c r="R4" s="92"/>
       <c r="X4" s="29"/>
       <c r="Y4" s="29"/>
     </row>
     <row r="5" spans="2:25">
       <c r="D5" s="71"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="101"/>
-      <c r="J5" s="102"/>
-      <c r="L5" s="94" t="s">
+      <c r="E5" s="90"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="96"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="98"/>
+      <c r="L5" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="M5" s="95"/>
-      <c r="N5" s="95"/>
-      <c r="O5" s="95"/>
-      <c r="P5" s="95"/>
-      <c r="Q5" s="95"/>
-      <c r="R5" s="96"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="91"/>
+      <c r="O5" s="91"/>
+      <c r="P5" s="91"/>
+      <c r="Q5" s="91"/>
+      <c r="R5" s="92"/>
       <c r="X5" s="29"/>
       <c r="Y5" s="29"/>
     </row>
     <row r="6" spans="2:25">
       <c r="D6" s="71"/>
-      <c r="E6" s="94" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="80" t="s">
-        <v>78</v>
-      </c>
-      <c r="I6" s="81"/>
-      <c r="J6" s="82"/>
-      <c r="L6" s="94"/>
-      <c r="M6" s="95"/>
-      <c r="N6" s="95"/>
-      <c r="O6" s="95"/>
-      <c r="P6" s="95"/>
-      <c r="Q6" s="95"/>
-      <c r="R6" s="96"/>
+      <c r="E6" s="90" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="76" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="77"/>
+      <c r="J6" s="78"/>
+      <c r="L6" s="90"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+      <c r="O6" s="91"/>
+      <c r="P6" s="91"/>
+      <c r="Q6" s="91"/>
+      <c r="R6" s="92"/>
       <c r="X6" s="29"/>
       <c r="Y6" s="29"/>
     </row>
     <row r="7" spans="2:25" ht="15.75" thickBot="1">
       <c r="D7" s="71"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="102"/>
-      <c r="L7" s="97"/>
-      <c r="M7" s="98"/>
-      <c r="N7" s="98"/>
-      <c r="O7" s="98"/>
-      <c r="P7" s="98"/>
-      <c r="Q7" s="98"/>
-      <c r="R7" s="99"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="91"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="97"/>
+      <c r="J7" s="98"/>
+      <c r="L7" s="93"/>
+      <c r="M7" s="94"/>
+      <c r="N7" s="94"/>
+      <c r="O7" s="94"/>
+      <c r="P7" s="94"/>
+      <c r="Q7" s="94"/>
+      <c r="R7" s="95"/>
       <c r="X7" s="29"/>
       <c r="Y7" s="29"/>
     </row>
     <row r="8" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="79"/>
+      <c r="C8" s="75"/>
       <c r="D8" s="71"/>
-      <c r="E8" s="94" t="s">
-        <v>76</v>
-      </c>
-      <c r="F8" s="95"/>
-      <c r="G8" s="95"/>
-      <c r="H8" s="80" t="s">
-        <v>80</v>
-      </c>
-      <c r="I8" s="81"/>
-      <c r="J8" s="82"/>
+      <c r="E8" s="90" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="91"/>
+      <c r="G8" s="91"/>
+      <c r="H8" s="76" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" s="77"/>
+      <c r="J8" s="78"/>
     </row>
     <row r="9" spans="2:25" ht="15.75" thickBot="1">
       <c r="B9" s="15" t="s">
@@ -1691,39 +1688,39 @@
       <c r="C9" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="94"/>
-      <c r="F9" s="95"/>
-      <c r="G9" s="95"/>
-      <c r="H9" s="100"/>
-      <c r="I9" s="101"/>
-      <c r="J9" s="102"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="91"/>
+      <c r="G9" s="91"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="98"/>
     </row>
     <row r="10" spans="2:25" ht="15.75" thickBot="1">
       <c r="B10" s="18">
         <v>0</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" s="94" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" s="95"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="80" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="90" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
+      <c r="H10" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="81"/>
-      <c r="J10" s="82"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="78"/>
       <c r="N10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="P10" s="77" t="s">
+      <c r="P10" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="Q10" s="78"/>
-      <c r="R10" s="78"/>
-      <c r="S10" s="79"/>
+      <c r="Q10" s="74"/>
+      <c r="R10" s="74"/>
+      <c r="S10" s="75"/>
     </row>
     <row r="11" spans="2:25" ht="15.75" thickBot="1">
       <c r="B11" s="18">
@@ -1732,29 +1729,30 @@
       <c r="C11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="97"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
-      <c r="H11" s="83"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="85"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="81"/>
       <c r="N11" s="14" t="s">
         <v>11</v>
       </c>
       <c r="P11" s="40" t="str">
         <f>INDEX(F14:L14, 1, Q11)</f>
-        <v>D</v>
+        <v>G</v>
       </c>
       <c r="Q11" s="59">
         <f>MOD(N16, 7)+1</f>
-        <v>4</v>
-      </c>
-      <c r="R11" s="70" t="s">
-        <v>72</v>
+        <v>7</v>
+      </c>
+      <c r="R11" s="70" t="str">
+        <f>CHOOSE(N18, "Sunday", "Monday", "Tuesday", "Wednesday", "Thursday", "Friday", "Saturday")</f>
+        <v>Friday</v>
       </c>
       <c r="S11" s="69">
         <f>N14</f>
-        <v>41582</v>
+        <v>41509</v>
       </c>
     </row>
     <row r="12" spans="2:25" ht="15.75" thickBot="1">
@@ -1778,7 +1776,7 @@
         <v>4</v>
       </c>
       <c r="S12" s="65" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="2:25" ht="15.75" thickBot="1">
@@ -1789,16 +1787,16 @@
       <c r="C13" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="77" t="s">
+      <c r="E13" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78"/>
-      <c r="L13" s="79"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="74"/>
+      <c r="L13" s="75"/>
       <c r="N13" s="19" t="s">
         <v>31</v>
       </c>
@@ -1852,7 +1850,7 @@
         <v>20</v>
       </c>
       <c r="N14" s="2">
-        <v>41582</v>
+        <v>41509</v>
       </c>
       <c r="O14" s="26"/>
       <c r="P14" s="43">
@@ -1860,11 +1858,11 @@
       </c>
       <c r="Q14" s="44">
         <f>INDEX(F15:L18,P14, Q11)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="R14" s="62" t="str">
         <f>INDEX(C11:C18, Q14, 1)</f>
-        <v>Orchestra</v>
+        <v>Bible</v>
       </c>
       <c r="S14" s="67" t="str">
         <f>INDEX(F33:L36, P14, N18)</f>
@@ -1912,11 +1910,11 @@
       </c>
       <c r="Q15" s="48">
         <f>INDEX(F22:L25, 2, N18)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="R15" s="61" t="str">
         <f>INDEX(C10:C25, Q15+1, 1)</f>
-        <v>Break</v>
+        <v>ADV</v>
       </c>
       <c r="S15" s="66" t="str">
         <f>INDEX(F29:L32, 2, N18)</f>
@@ -1957,7 +1955,7 @@
       </c>
       <c r="N16" s="53">
         <f>MAX(NETWORKDAYS(N12, N14,N22:N123)-1, 0)</f>
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="O16" s="54"/>
       <c r="P16" s="43">
@@ -1965,11 +1963,11 @@
       </c>
       <c r="Q16" s="44">
         <f>INDEX(F15:L18,P16, Q11)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R16" s="62" t="str">
         <f>INDEX(C11:C18, Q16, 1)</f>
-        <v>Physics</v>
+        <v>English</v>
       </c>
       <c r="S16" s="67" t="str">
         <f>INDEX(F33:L36, P16, N18)</f>
@@ -2017,11 +2015,11 @@
       </c>
       <c r="Q17" s="44">
         <f>INDEX(F15:L18,P17, Q11)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="R17" s="62" t="str">
         <f>INDEX(C11:C18, Q17, 1)</f>
-        <v>History</v>
+        <v>Orchestra</v>
       </c>
       <c r="S17" s="67" t="str">
         <f>INDEX(F33:L36, P17, N18)</f>
@@ -2062,7 +2060,7 @@
       </c>
       <c r="N18" s="21">
         <f>WEEKDAY(S11)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="O18" s="54"/>
       <c r="P18" s="22">
@@ -2070,15 +2068,15 @@
       </c>
       <c r="Q18" s="48">
         <f>INDEX(F22:L25, 3, N18)</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="R18" s="61" t="str">
         <f>INDEX(C10:C25, Q18+1, 1)</f>
-        <v>ARTS/ADV</v>
+        <v>Break</v>
       </c>
       <c r="S18" s="66" t="str">
         <f>INDEX(F29:L32, 3, N18)</f>
-        <v>1:10-1:50</v>
+        <v>1:10-1:20</v>
       </c>
     </row>
     <row r="19" spans="2:19" ht="15.75" thickBot="1">
@@ -2095,15 +2093,15 @@
       </c>
       <c r="Q19" s="44">
         <f>INDEX(F15:L18,P19, Q11)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="R19" s="62" t="str">
         <f>INDEX(C11:C18, Q19, 1)</f>
-        <v>Math</v>
+        <v>Physics</v>
       </c>
       <c r="S19" s="67" t="str">
         <f>INDEX(F33:L36, P19, N18)</f>
-        <v>1:50-3:00</v>
+        <v>1:20-2:30</v>
       </c>
     </row>
     <row r="20" spans="2:19" ht="15.75" thickBot="1">
@@ -2114,16 +2112,16 @@
       <c r="C20" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="77" t="s">
+      <c r="E20" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="78"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="78"/>
-      <c r="J20" s="78"/>
-      <c r="K20" s="78"/>
-      <c r="L20" s="79"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="74"/>
+      <c r="J20" s="74"/>
+      <c r="K20" s="74"/>
+      <c r="L20" s="75"/>
       <c r="N20" s="11" t="s">
         <v>25</v>
       </c>
@@ -2133,15 +2131,15 @@
       </c>
       <c r="Q20" s="49">
         <f>INDEX(F22:L25, 4, N18)</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="R20" s="64" t="str">
         <f>INDEX(C10:C25, Q20+1, 1)</f>
-        <v>Office Hours</v>
-      </c>
-      <c r="S20" s="68" t="str">
+        <v>Weekend</v>
+      </c>
+      <c r="S20" s="68">
         <f>INDEX(F29:L32, 4, N18)</f>
-        <v>3:00-3:30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:19">
@@ -2343,16 +2341,16 @@
       <c r="S26" s="27"/>
     </row>
     <row r="27" spans="2:19" ht="15.75" thickBot="1">
-      <c r="E27" s="77" t="s">
+      <c r="E27" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="78"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="78"/>
-      <c r="I27" s="78"/>
-      <c r="J27" s="78"/>
-      <c r="K27" s="78"/>
-      <c r="L27" s="79"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
+      <c r="K27" s="74"/>
+      <c r="L27" s="75"/>
       <c r="N27" s="7">
         <v>41575</v>
       </c>
@@ -2899,6 +2897,14 @@
   </sheetData>
   <sheetProtection password="C836" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
   <mergeCells count="21">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="E13:L13"/>
+    <mergeCell ref="E20:L20"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="L2:R2"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="E27:L27"/>
     <mergeCell ref="H10:J11"/>
     <mergeCell ref="H3:J3"/>
@@ -2912,14 +2918,6 @@
     <mergeCell ref="E10:G11"/>
     <mergeCell ref="H6:J7"/>
     <mergeCell ref="H8:J9"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="P10:S10"/>
-    <mergeCell ref="E13:L13"/>
-    <mergeCell ref="E20:L20"/>
-    <mergeCell ref="E2:J2"/>
-    <mergeCell ref="L2:R2"/>
-    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2967,155 +2965,155 @@
       <c r="J1" s="72"/>
     </row>
     <row r="2" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="99" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="74"/>
+      <c r="C2" s="100"/>
       <c r="D2" s="71"/>
-      <c r="E2" s="77" t="s">
+      <c r="E2" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="79"/>
-      <c r="L2" s="77" t="s">
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="75"/>
+      <c r="L2" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="79"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="75"/>
     </row>
     <row r="3" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="76"/>
+      <c r="C3" s="102"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="89" t="s">
+      <c r="E3" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="86" t="s">
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="87"/>
-      <c r="J3" s="88"/>
-      <c r="L3" s="91" t="s">
+      <c r="I3" s="83"/>
+      <c r="J3" s="84"/>
+      <c r="L3" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="92"/>
-      <c r="N3" s="92"/>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="93"/>
+      <c r="M3" s="88"/>
+      <c r="N3" s="88"/>
+      <c r="O3" s="88"/>
+      <c r="P3" s="88"/>
+      <c r="Q3" s="88"/>
+      <c r="R3" s="89"/>
       <c r="X3" s="29"/>
       <c r="Y3" s="29"/>
     </row>
     <row r="4" spans="2:25">
       <c r="D4" s="71"/>
-      <c r="E4" s="94" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" s="95"/>
-      <c r="G4" s="95"/>
-      <c r="H4" s="80" t="s">
+      <c r="E4" s="90" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="I4" s="81"/>
-      <c r="J4" s="82"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="95"/>
-      <c r="N4" s="95"/>
-      <c r="O4" s="95"/>
-      <c r="P4" s="95"/>
-      <c r="Q4" s="95"/>
-      <c r="R4" s="96"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="78"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="91"/>
+      <c r="Q4" s="91"/>
+      <c r="R4" s="92"/>
       <c r="X4" s="29"/>
       <c r="Y4" s="29"/>
     </row>
     <row r="5" spans="2:25">
       <c r="D5" s="71"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="101"/>
-      <c r="J5" s="102"/>
-      <c r="L5" s="94" t="s">
+      <c r="E5" s="90"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="96"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="98"/>
+      <c r="L5" s="90" t="s">
         <v>51</v>
       </c>
-      <c r="M5" s="95"/>
-      <c r="N5" s="95"/>
-      <c r="O5" s="95"/>
-      <c r="P5" s="95"/>
-      <c r="Q5" s="95"/>
-      <c r="R5" s="96"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="91"/>
+      <c r="O5" s="91"/>
+      <c r="P5" s="91"/>
+      <c r="Q5" s="91"/>
+      <c r="R5" s="92"/>
       <c r="X5" s="29"/>
       <c r="Y5" s="29"/>
     </row>
     <row r="6" spans="2:25">
       <c r="D6" s="71"/>
-      <c r="E6" s="94" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="80" t="s">
-        <v>78</v>
-      </c>
-      <c r="I6" s="81"/>
-      <c r="J6" s="82"/>
-      <c r="L6" s="94"/>
-      <c r="M6" s="95"/>
-      <c r="N6" s="95"/>
-      <c r="O6" s="95"/>
-      <c r="P6" s="95"/>
-      <c r="Q6" s="95"/>
-      <c r="R6" s="96"/>
+      <c r="E6" s="90" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="76" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="77"/>
+      <c r="J6" s="78"/>
+      <c r="L6" s="90"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+      <c r="O6" s="91"/>
+      <c r="P6" s="91"/>
+      <c r="Q6" s="91"/>
+      <c r="R6" s="92"/>
       <c r="X6" s="29"/>
       <c r="Y6" s="29"/>
     </row>
     <row r="7" spans="2:25" ht="15.75" thickBot="1">
       <c r="D7" s="71"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="102"/>
-      <c r="L7" s="97"/>
-      <c r="M7" s="98"/>
-      <c r="N7" s="98"/>
-      <c r="O7" s="98"/>
-      <c r="P7" s="98"/>
-      <c r="Q7" s="98"/>
-      <c r="R7" s="99"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="91"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="97"/>
+      <c r="J7" s="98"/>
+      <c r="L7" s="93"/>
+      <c r="M7" s="94"/>
+      <c r="N7" s="94"/>
+      <c r="O7" s="94"/>
+      <c r="P7" s="94"/>
+      <c r="Q7" s="94"/>
+      <c r="R7" s="95"/>
       <c r="X7" s="29"/>
       <c r="Y7" s="29"/>
     </row>
     <row r="8" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="79"/>
+      <c r="C8" s="75"/>
       <c r="D8" s="71"/>
-      <c r="E8" s="94" t="s">
+      <c r="E8" s="90" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="91"/>
+      <c r="G8" s="91"/>
+      <c r="H8" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="95"/>
-      <c r="G8" s="95"/>
-      <c r="H8" s="80" t="s">
-        <v>80</v>
-      </c>
-      <c r="I8" s="81"/>
-      <c r="J8" s="82"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="78"/>
     </row>
     <row r="9" spans="2:25" ht="15.75" thickBot="1">
       <c r="B9" s="15" t="s">
@@ -3124,39 +3122,39 @@
       <c r="C9" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="94"/>
-      <c r="F9" s="95"/>
-      <c r="G9" s="95"/>
-      <c r="H9" s="100"/>
-      <c r="I9" s="101"/>
-      <c r="J9" s="102"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="91"/>
+      <c r="G9" s="91"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="98"/>
     </row>
     <row r="10" spans="2:25" ht="15.75" thickBot="1">
       <c r="B10" s="18">
         <v>0</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" s="94" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" s="95"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="80" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="90" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
+      <c r="H10" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="81"/>
-      <c r="J10" s="82"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="78"/>
       <c r="N10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="P10" s="77" t="s">
+      <c r="P10" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="Q10" s="78"/>
-      <c r="R10" s="78"/>
-      <c r="S10" s="79"/>
+      <c r="Q10" s="74"/>
+      <c r="R10" s="74"/>
+      <c r="S10" s="75"/>
     </row>
     <row r="11" spans="2:25" ht="15.75" thickBot="1">
       <c r="B11" s="18">
@@ -3165,12 +3163,12 @@
       <c r="C11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="97"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
-      <c r="H11" s="83"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="85"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="81"/>
       <c r="N11" s="14" t="s">
         <v>11</v>
       </c>
@@ -3182,8 +3180,9 @@
         <f>MOD(N16, 7)+1</f>
         <v>7</v>
       </c>
-      <c r="R11" s="70" t="s">
-        <v>72</v>
+      <c r="R11" s="70" t="str">
+        <f>CHOOSE(N18, "Sunday", "Monday", "Tuesday", "Wednesday", "Thursday", "Friday", "Saturday")</f>
+        <v>Wednesday</v>
       </c>
       <c r="S11" s="69">
         <f>N14</f>
@@ -3211,7 +3210,7 @@
         <v>4</v>
       </c>
       <c r="S12" s="65" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="2:25" ht="15.75" thickBot="1">
@@ -3222,16 +3221,16 @@
       <c r="C13" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="77" t="s">
+      <c r="E13" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78"/>
-      <c r="L13" s="79"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="74"/>
+      <c r="L13" s="75"/>
       <c r="N13" s="19" t="s">
         <v>31</v>
       </c>
@@ -3547,16 +3546,16 @@
       <c r="C20" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="77" t="s">
+      <c r="E20" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="78"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="78"/>
-      <c r="J20" s="78"/>
-      <c r="K20" s="78"/>
-      <c r="L20" s="79"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="74"/>
+      <c r="J20" s="74"/>
+      <c r="K20" s="74"/>
+      <c r="L20" s="75"/>
       <c r="N20" s="11" t="s">
         <v>25</v>
       </c>
@@ -3776,16 +3775,16 @@
       <c r="S26" s="27"/>
     </row>
     <row r="27" spans="2:19" ht="15.75" thickBot="1">
-      <c r="E27" s="77" t="s">
+      <c r="E27" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="78"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="78"/>
-      <c r="I27" s="78"/>
-      <c r="J27" s="78"/>
-      <c r="K27" s="78"/>
-      <c r="L27" s="79"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
+      <c r="K27" s="74"/>
+      <c r="L27" s="75"/>
       <c r="N27" s="7">
         <v>41709</v>
       </c>
@@ -4340,6 +4339,12 @@
   </sheetData>
   <sheetProtection password="C836" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
   <mergeCells count="21">
+    <mergeCell ref="E27:L27"/>
+    <mergeCell ref="E10:G11"/>
+    <mergeCell ref="H10:J11"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="E13:L13"/>
+    <mergeCell ref="E20:L20"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:J2"/>
@@ -4355,12 +4360,6 @@
     <mergeCell ref="H6:J7"/>
     <mergeCell ref="E8:G9"/>
     <mergeCell ref="H8:J9"/>
-    <mergeCell ref="E10:G11"/>
-    <mergeCell ref="H10:J11"/>
-    <mergeCell ref="P10:S10"/>
-    <mergeCell ref="E13:L13"/>
-    <mergeCell ref="E20:L20"/>
-    <mergeCell ref="E27:L27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated instructions, added Helper Buttons (Today and Reset)
</commit_message>
<xml_diff>
--- a/WMS_Scheduler.xlsx
+++ b/WMS_Scheduler.xlsx
@@ -299,28 +299,28 @@
     <t>Time</t>
   </si>
   <si>
-    <t>2. Fill out your rot. schedule in Fig. 2 (Using 8 as a Free period)</t>
-  </si>
-  <si>
-    <t>1. Fill out your course names in Fig. 1 (8 represents your Frees)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. Enter date of a Past A Day of Sem I in Fig. 3 (e.g 8/15/2013) </t>
-  </si>
-  <si>
-    <t>3. Make sure all the holidays are correctly marked in Fig. 4</t>
-  </si>
-  <si>
-    <t>1. Use the LATEST A day (before Date to Schedule) in Fig. 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. Enter date of a Past A Day of Sem II in Fig. 3 (e.g 1/6/2014) </t>
-  </si>
-  <si>
     <t>2. Enter the date for the desired schedule in Fig. 3</t>
   </si>
   <si>
     <t>Weekend</t>
+  </si>
+  <si>
+    <t>4. Make sure all the holidays are correctly marked in Fig. 4</t>
+  </si>
+  <si>
+    <t>1. Fill out course names in Fig. 1 (8 represents your Frees)</t>
+  </si>
+  <si>
+    <t>2. Fill out Fig. 2 with the period numbers from your rotational schedule (1-7). Then use 8 to represent any frees. Do include lab frees. For example: If you have 5th free, then all the 5's should be replaced with 8's.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Enter date of a Past "A" Day of Sem I in Fig. 3 (e.g 8/15/2013) </t>
+  </si>
+  <si>
+    <t>1. Use the LATEST "A" day (before Date to Schedule) in Fig. 3</t>
+  </si>
+  <si>
+    <t>3. Enter date of a Past "A" Day of Sem II in Fig. 3 (e.g 1/6/2014)</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -859,19 +859,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -888,14 +875,23 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -904,9 +900,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -917,16 +911,56 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -935,7 +969,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1134,6 +1168,9 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1143,66 +1180,119 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1531,196 +1621,212 @@
   <sheetData>
     <row r="1" spans="2:25" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="104" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="100"/>
+      <c r="C2" s="105"/>
       <c r="D2" s="71"/>
-      <c r="E2" s="73" t="s">
+      <c r="E2" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="75"/>
-      <c r="L2" s="73" t="s">
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="94"/>
+      <c r="N2" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74"/>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="74"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
       <c r="R2" s="75"/>
-    </row>
-    <row r="3" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B3" s="101" t="s">
+      <c r="S2" s="76"/>
+      <c r="T2" s="29"/>
+    </row>
+    <row r="3" spans="2:25" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B3" s="106" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="102"/>
+      <c r="C3" s="107"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="85" t="s">
+      <c r="E3" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="82" t="s">
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="83"/>
-      <c r="J3" s="84"/>
-      <c r="L3" s="87" t="s">
+      <c r="K3" s="96"/>
+      <c r="L3" s="97"/>
+      <c r="N3" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
-      <c r="P3" s="88"/>
-      <c r="Q3" s="88"/>
-      <c r="R3" s="89"/>
+      <c r="O3" s="78"/>
+      <c r="P3" s="78"/>
+      <c r="Q3" s="78"/>
+      <c r="R3" s="78"/>
+      <c r="S3" s="79"/>
+      <c r="T3" s="73"/>
       <c r="X3" s="29"/>
       <c r="Y3" s="29"/>
     </row>
-    <row r="4" spans="2:25">
+    <row r="4" spans="2:25" ht="15" customHeight="1">
       <c r="D4" s="71"/>
-      <c r="E4" s="90" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="76" t="s">
+      <c r="E4" s="98" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="108" t="s">
         <v>71</v>
       </c>
-      <c r="I4" s="77"/>
-      <c r="J4" s="78"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="91"/>
-      <c r="N4" s="91"/>
-      <c r="O4" s="91"/>
-      <c r="P4" s="91"/>
-      <c r="Q4" s="91"/>
-      <c r="R4" s="92"/>
+      <c r="K4" s="84"/>
+      <c r="L4" s="85"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="82"/>
+      <c r="T4" s="73"/>
       <c r="X4" s="29"/>
       <c r="Y4" s="29"/>
     </row>
-    <row r="5" spans="2:25">
+    <row r="5" spans="2:25" ht="15" customHeight="1">
       <c r="D5" s="71"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="98"/>
-      <c r="L5" s="90" t="s">
+      <c r="E5" s="100" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="109"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="82"/>
+      <c r="N5" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="M5" s="91"/>
-      <c r="N5" s="91"/>
-      <c r="O5" s="91"/>
-      <c r="P5" s="91"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="92"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="84"/>
+      <c r="Q5" s="84"/>
+      <c r="R5" s="84"/>
+      <c r="S5" s="85"/>
+      <c r="T5" s="73"/>
       <c r="X5" s="29"/>
       <c r="Y5" s="29"/>
     </row>
-    <row r="6" spans="2:25">
+    <row r="6" spans="2:25" ht="15" customHeight="1">
       <c r="D6" s="71"/>
-      <c r="E6" s="90" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="91"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="76" t="s">
-        <v>77</v>
-      </c>
-      <c r="I6" s="77"/>
-      <c r="J6" s="78"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
-      <c r="O6" s="91"/>
-      <c r="P6" s="91"/>
-      <c r="Q6" s="91"/>
-      <c r="R6" s="92"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="101"/>
+      <c r="G6" s="101"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="101"/>
+      <c r="J6" s="99" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" s="99"/>
+      <c r="L6" s="110"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="87"/>
+      <c r="S6" s="88"/>
+      <c r="T6" s="73"/>
       <c r="X6" s="29"/>
       <c r="Y6" s="29"/>
     </row>
     <row r="7" spans="2:25" ht="15.75" thickBot="1">
       <c r="D7" s="71"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="91"/>
-      <c r="G7" s="91"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="97"/>
-      <c r="J7" s="98"/>
-      <c r="L7" s="93"/>
-      <c r="M7" s="94"/>
-      <c r="N7" s="94"/>
-      <c r="O7" s="94"/>
-      <c r="P7" s="94"/>
-      <c r="Q7" s="94"/>
-      <c r="R7" s="95"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="101"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="99"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="110"/>
+      <c r="N7" s="89"/>
+      <c r="O7" s="90"/>
+      <c r="P7" s="90"/>
+      <c r="Q7" s="90"/>
+      <c r="R7" s="90"/>
+      <c r="S7" s="91"/>
+      <c r="T7" s="73"/>
       <c r="X7" s="29"/>
       <c r="Y7" s="29"/>
     </row>
-    <row r="8" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B8" s="73" t="s">
+    <row r="8" spans="2:25" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B8" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="75"/>
+      <c r="C8" s="76"/>
       <c r="D8" s="71"/>
-      <c r="E8" s="90" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="91"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="76" t="s">
-        <v>79</v>
-      </c>
-      <c r="I8" s="77"/>
-      <c r="J8" s="78"/>
-    </row>
-    <row r="9" spans="2:25" ht="15.75" thickBot="1">
+      <c r="E8" s="100"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101"/>
+      <c r="I8" s="101"/>
+      <c r="J8" s="111" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8" s="111"/>
+      <c r="L8" s="112"/>
+    </row>
+    <row r="9" spans="2:25" ht="15.75" customHeight="1" thickBot="1">
       <c r="B9" s="15" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="90"/>
-      <c r="F9" s="91"/>
-      <c r="G9" s="91"/>
-      <c r="H9" s="96"/>
-      <c r="I9" s="97"/>
-      <c r="J9" s="98"/>
-    </row>
-    <row r="10" spans="2:25" ht="15.75" thickBot="1">
+      <c r="E9" s="98" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="99"/>
+      <c r="G9" s="99"/>
+      <c r="H9" s="99"/>
+      <c r="I9" s="99"/>
+      <c r="J9" s="111"/>
+      <c r="K9" s="111"/>
+      <c r="L9" s="112"/>
+    </row>
+    <row r="10" spans="2:25" ht="15.75" customHeight="1" thickBot="1">
       <c r="B10" s="18">
         <v>0</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="90" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="91"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="98"/>
+      <c r="F10" s="99"/>
+      <c r="G10" s="99"/>
+      <c r="H10" s="99"/>
+      <c r="I10" s="99"/>
+      <c r="J10" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="77"/>
-      <c r="J10" s="78"/>
+      <c r="K10" s="99"/>
+      <c r="L10" s="110"/>
       <c r="N10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="P10" s="73" t="s">
+      <c r="P10" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="74"/>
-      <c r="S10" s="75"/>
+      <c r="Q10" s="75"/>
+      <c r="R10" s="75"/>
+      <c r="S10" s="76"/>
     </row>
     <row r="11" spans="2:25" ht="15.75" thickBot="1">
       <c r="B11" s="18">
@@ -1729,12 +1835,16 @@
       <c r="C11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="93"/>
-      <c r="F11" s="94"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="81"/>
+      <c r="E11" s="102" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="103"/>
+      <c r="G11" s="103"/>
+      <c r="H11" s="103"/>
+      <c r="I11" s="103"/>
+      <c r="J11" s="113"/>
+      <c r="K11" s="113"/>
+      <c r="L11" s="114"/>
       <c r="N11" s="14" t="s">
         <v>11</v>
       </c>
@@ -1787,16 +1897,16 @@
       <c r="C13" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="73" t="s">
+      <c r="E13" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="74"/>
-      <c r="K13" s="74"/>
-      <c r="L13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="76"/>
       <c r="N13" s="19" t="s">
         <v>31</v>
       </c>
@@ -1884,7 +1994,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H15" s="3">
         <v>2</v>
@@ -1896,7 +2006,7 @@
         <v>3</v>
       </c>
       <c r="K15" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L15" s="4">
         <v>4</v>
@@ -1951,7 +2061,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N16" s="53">
         <f>MAX(NETWORKDAYS(N12, N14,N22:N123)-1, 0)</f>
@@ -1963,11 +2073,11 @@
       </c>
       <c r="Q16" s="44">
         <f>INDEX(F15:L18,P16, Q11)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="R16" s="62" t="str">
         <f>INDEX(C11:C18, Q16, 1)</f>
-        <v>English</v>
+        <v>Free</v>
       </c>
       <c r="S16" s="67" t="str">
         <f>INDEX(F33:L36, P16, N18)</f>
@@ -1989,7 +2099,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H17" s="3">
         <v>4</v>
@@ -1998,7 +2108,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K17" s="3">
         <v>2</v>
@@ -2044,7 +2154,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I18" s="5">
         <v>2</v>
@@ -2112,16 +2222,16 @@
       <c r="C20" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="73" t="s">
+      <c r="E20" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="74"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="75"/>
+      <c r="F20" s="75"/>
+      <c r="G20" s="75"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="75"/>
+      <c r="J20" s="75"/>
+      <c r="K20" s="75"/>
+      <c r="L20" s="76"/>
       <c r="N20" s="11" t="s">
         <v>25</v>
       </c>
@@ -2341,16 +2451,16 @@
       <c r="S26" s="27"/>
     </row>
     <row r="27" spans="2:19" ht="15.75" thickBot="1">
-      <c r="E27" s="73" t="s">
+      <c r="E27" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="74"/>
-      <c r="I27" s="74"/>
-      <c r="J27" s="74"/>
-      <c r="K27" s="74"/>
-      <c r="L27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="75"/>
+      <c r="J27" s="75"/>
+      <c r="K27" s="75"/>
+      <c r="L27" s="76"/>
       <c r="N27" s="7">
         <v>41575</v>
       </c>
@@ -2897,27 +3007,27 @@
   </sheetData>
   <sheetProtection password="C836" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
   <mergeCells count="21">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
     <mergeCell ref="P10:S10"/>
     <mergeCell ref="E13:L13"/>
     <mergeCell ref="E20:L20"/>
-    <mergeCell ref="E2:J2"/>
-    <mergeCell ref="L2:R2"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="J4:L5"/>
+    <mergeCell ref="J6:L7"/>
+    <mergeCell ref="J8:L9"/>
+    <mergeCell ref="J10:L11"/>
+    <mergeCell ref="E9:I10"/>
+    <mergeCell ref="E11:I11"/>
     <mergeCell ref="E27:L27"/>
-    <mergeCell ref="H10:J11"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="L3:R4"/>
-    <mergeCell ref="L5:R7"/>
-    <mergeCell ref="E4:G5"/>
-    <mergeCell ref="H4:J5"/>
-    <mergeCell ref="E6:G7"/>
-    <mergeCell ref="E8:G9"/>
-    <mergeCell ref="E10:G11"/>
-    <mergeCell ref="H6:J7"/>
-    <mergeCell ref="H8:J9"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="N3:S4"/>
+    <mergeCell ref="N5:S7"/>
+    <mergeCell ref="E2:L2"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="E5:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2965,210 +3075,230 @@
       <c r="J1" s="72"/>
     </row>
     <row r="2" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="100"/>
+      <c r="C2" s="105"/>
       <c r="D2" s="71"/>
-      <c r="E2" s="73" t="s">
+      <c r="E2" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="75"/>
-      <c r="L2" s="73" t="s">
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="94"/>
+      <c r="N2" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74"/>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="74"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
       <c r="R2" s="75"/>
-    </row>
-    <row r="3" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B3" s="101" t="s">
+      <c r="S2" s="76"/>
+      <c r="T2" s="29"/>
+    </row>
+    <row r="3" spans="2:25" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B3" s="106" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="102"/>
+      <c r="C3" s="107"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="85" t="s">
+      <c r="E3" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="82" t="s">
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="83"/>
-      <c r="J3" s="84"/>
-      <c r="L3" s="87" t="s">
+      <c r="K3" s="96"/>
+      <c r="L3" s="97"/>
+      <c r="N3" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
-      <c r="P3" s="88"/>
-      <c r="Q3" s="88"/>
-      <c r="R3" s="89"/>
+      <c r="O3" s="78"/>
+      <c r="P3" s="78"/>
+      <c r="Q3" s="78"/>
+      <c r="R3" s="78"/>
+      <c r="S3" s="79"/>
+      <c r="T3" s="73"/>
       <c r="X3" s="29"/>
       <c r="Y3" s="29"/>
     </row>
-    <row r="4" spans="2:25">
+    <row r="4" spans="2:25" ht="15" customHeight="1">
       <c r="D4" s="71"/>
-      <c r="E4" s="90" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="76" t="s">
+      <c r="E4" s="98" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="108" t="s">
         <v>71</v>
       </c>
-      <c r="I4" s="77"/>
-      <c r="J4" s="78"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="91"/>
-      <c r="N4" s="91"/>
-      <c r="O4" s="91"/>
-      <c r="P4" s="91"/>
-      <c r="Q4" s="91"/>
-      <c r="R4" s="92"/>
+      <c r="K4" s="84"/>
+      <c r="L4" s="85"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="82"/>
+      <c r="T4" s="73"/>
       <c r="X4" s="29"/>
       <c r="Y4" s="29"/>
     </row>
-    <row r="5" spans="2:25">
+    <row r="5" spans="2:25" ht="15" customHeight="1">
       <c r="D5" s="71"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="98"/>
-      <c r="L5" s="90" t="s">
+      <c r="E5" s="100" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="109"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="82"/>
+      <c r="N5" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="M5" s="91"/>
-      <c r="N5" s="91"/>
-      <c r="O5" s="91"/>
-      <c r="P5" s="91"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="92"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="84"/>
+      <c r="Q5" s="84"/>
+      <c r="R5" s="84"/>
+      <c r="S5" s="85"/>
+      <c r="T5" s="73"/>
       <c r="X5" s="29"/>
       <c r="Y5" s="29"/>
     </row>
-    <row r="6" spans="2:25">
+    <row r="6" spans="2:25" ht="15" customHeight="1">
       <c r="D6" s="71"/>
-      <c r="E6" s="90" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="91"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="76" t="s">
-        <v>77</v>
-      </c>
-      <c r="I6" s="77"/>
-      <c r="J6" s="78"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
-      <c r="O6" s="91"/>
-      <c r="P6" s="91"/>
-      <c r="Q6" s="91"/>
-      <c r="R6" s="92"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="101"/>
+      <c r="G6" s="101"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="101"/>
+      <c r="J6" s="99" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" s="99"/>
+      <c r="L6" s="110"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="87"/>
+      <c r="S6" s="88"/>
+      <c r="T6" s="73"/>
       <c r="X6" s="29"/>
       <c r="Y6" s="29"/>
     </row>
     <row r="7" spans="2:25" ht="15.75" thickBot="1">
       <c r="D7" s="71"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="91"/>
-      <c r="G7" s="91"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="97"/>
-      <c r="J7" s="98"/>
-      <c r="L7" s="93"/>
-      <c r="M7" s="94"/>
-      <c r="N7" s="94"/>
-      <c r="O7" s="94"/>
-      <c r="P7" s="94"/>
-      <c r="Q7" s="94"/>
-      <c r="R7" s="95"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="101"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="99"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="110"/>
+      <c r="N7" s="89"/>
+      <c r="O7" s="90"/>
+      <c r="P7" s="90"/>
+      <c r="Q7" s="90"/>
+      <c r="R7" s="90"/>
+      <c r="S7" s="91"/>
+      <c r="T7" s="73"/>
       <c r="X7" s="29"/>
       <c r="Y7" s="29"/>
     </row>
-    <row r="8" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B8" s="73" t="s">
+    <row r="8" spans="2:25" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B8" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="75"/>
+      <c r="C8" s="76"/>
       <c r="D8" s="71"/>
-      <c r="E8" s="90" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="91"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="76" t="s">
-        <v>79</v>
-      </c>
-      <c r="I8" s="77"/>
-      <c r="J8" s="78"/>
-    </row>
-    <row r="9" spans="2:25" ht="15.75" thickBot="1">
+      <c r="E8" s="100"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101"/>
+      <c r="I8" s="101"/>
+      <c r="J8" s="111" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8" s="111"/>
+      <c r="L8" s="112"/>
+    </row>
+    <row r="9" spans="2:25" ht="15.75" customHeight="1" thickBot="1">
       <c r="B9" s="15" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="90"/>
-      <c r="F9" s="91"/>
-      <c r="G9" s="91"/>
-      <c r="H9" s="96"/>
-      <c r="I9" s="97"/>
-      <c r="J9" s="98"/>
-    </row>
-    <row r="10" spans="2:25" ht="15.75" thickBot="1">
+      <c r="E9" s="98" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="99"/>
+      <c r="G9" s="99"/>
+      <c r="H9" s="99"/>
+      <c r="I9" s="99"/>
+      <c r="J9" s="111"/>
+      <c r="K9" s="111"/>
+      <c r="L9" s="112"/>
+    </row>
+    <row r="10" spans="2:25" ht="15.75" customHeight="1" thickBot="1">
       <c r="B10" s="18">
         <v>0</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="90" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="91"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="98"/>
+      <c r="F10" s="99"/>
+      <c r="G10" s="99"/>
+      <c r="H10" s="99"/>
+      <c r="I10" s="99"/>
+      <c r="J10" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="77"/>
-      <c r="J10" s="78"/>
+      <c r="K10" s="99"/>
+      <c r="L10" s="110"/>
       <c r="N10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="P10" s="73" t="s">
+      <c r="P10" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="74"/>
-      <c r="S10" s="75"/>
-    </row>
-    <row r="11" spans="2:25" ht="15.75" thickBot="1">
+      <c r="Q10" s="75"/>
+      <c r="R10" s="75"/>
+      <c r="S10" s="76"/>
+    </row>
+    <row r="11" spans="2:25" ht="15.75" customHeight="1" thickBot="1">
       <c r="B11" s="18">
         <v>1</v>
       </c>
       <c r="C11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="93"/>
-      <c r="F11" s="94"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="81"/>
+      <c r="E11" s="102" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="103"/>
+      <c r="G11" s="103"/>
+      <c r="H11" s="103"/>
+      <c r="I11" s="103"/>
+      <c r="J11" s="113"/>
+      <c r="K11" s="113"/>
+      <c r="L11" s="114"/>
       <c r="N11" s="14" t="s">
         <v>11</v>
       </c>
@@ -3221,16 +3351,16 @@
       <c r="C13" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="73" t="s">
+      <c r="E13" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="74"/>
-      <c r="K13" s="74"/>
-      <c r="L13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="76"/>
       <c r="N13" s="19" t="s">
         <v>31</v>
       </c>
@@ -3318,7 +3448,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H15" s="3">
         <v>2</v>
@@ -3330,7 +3460,7 @@
         <v>3</v>
       </c>
       <c r="K15" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L15" s="4">
         <v>4</v>
@@ -3385,7 +3515,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N16" s="53">
         <f>MAX(NETWORKDAYS(N12, N14,N22:N123)-1, 0)</f>
@@ -3397,11 +3527,11 @@
       </c>
       <c r="Q16" s="44">
         <f>INDEX(F15:L18,P16, Q11)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="R16" s="62" t="str">
         <f>INDEX(C11:C18, Q16, 1)</f>
-        <v>English</v>
+        <v>Free</v>
       </c>
       <c r="S16" s="67" t="str">
         <f>INDEX(F33:L36, P16, N18)</f>
@@ -3423,7 +3553,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H17" s="3">
         <v>4</v>
@@ -3432,7 +3562,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K17" s="3">
         <v>2</v>
@@ -3478,7 +3608,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I18" s="5">
         <v>2</v>
@@ -3546,16 +3676,16 @@
       <c r="C20" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="73" t="s">
+      <c r="E20" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="74"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="75"/>
+      <c r="F20" s="75"/>
+      <c r="G20" s="75"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="75"/>
+      <c r="J20" s="75"/>
+      <c r="K20" s="75"/>
+      <c r="L20" s="76"/>
       <c r="N20" s="11" t="s">
         <v>25</v>
       </c>
@@ -3775,16 +3905,16 @@
       <c r="S26" s="27"/>
     </row>
     <row r="27" spans="2:19" ht="15.75" thickBot="1">
-      <c r="E27" s="73" t="s">
+      <c r="E27" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="74"/>
-      <c r="I27" s="74"/>
-      <c r="J27" s="74"/>
-      <c r="K27" s="74"/>
-      <c r="L27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="75"/>
+      <c r="J27" s="75"/>
+      <c r="K27" s="75"/>
+      <c r="L27" s="76"/>
       <c r="N27" s="7">
         <v>41709</v>
       </c>
@@ -4339,27 +4469,27 @@
   </sheetData>
   <sheetProtection password="C836" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
   <mergeCells count="21">
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
     <mergeCell ref="E27:L27"/>
-    <mergeCell ref="E10:G11"/>
-    <mergeCell ref="H10:J11"/>
     <mergeCell ref="P10:S10"/>
     <mergeCell ref="E13:L13"/>
     <mergeCell ref="E20:L20"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:J2"/>
-    <mergeCell ref="L2:R2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="L3:R4"/>
-    <mergeCell ref="E4:G5"/>
-    <mergeCell ref="H4:J5"/>
-    <mergeCell ref="L5:R7"/>
-    <mergeCell ref="E6:G7"/>
-    <mergeCell ref="H6:J7"/>
-    <mergeCell ref="E8:G9"/>
-    <mergeCell ref="H8:J9"/>
+    <mergeCell ref="N5:S7"/>
+    <mergeCell ref="E2:L2"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="J4:L5"/>
+    <mergeCell ref="E5:I8"/>
+    <mergeCell ref="J6:L7"/>
+    <mergeCell ref="J8:L9"/>
+    <mergeCell ref="E9:I10"/>
+    <mergeCell ref="J10:L11"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="N3:S4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated instructions, added Example schedules
</commit_message>
<xml_diff>
--- a/WMS_Scheduler.xlsx
+++ b/WMS_Scheduler.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="84">
   <si>
     <t>Holidays</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Disclaimers</t>
   </si>
   <si>
-    <t>1. This calculates your schedule on the assumption that it is always rolling from the PAD, except for weekends and holidays.</t>
-  </si>
-  <si>
     <t>WMS Scheduler I</t>
   </si>
   <si>
@@ -166,12 +163,6 @@
   </si>
   <si>
     <t>S</t>
-  </si>
-  <si>
-    <t>2. All the break / holiday dates from the Calendar have been added, except for wms exam days. This Scheduler works only for Semester I. See "Sheet2" (below) for the Semester II Scheduler.</t>
-  </si>
-  <si>
-    <t>2. All the break / holiday dates from the Calendar have been added, except for wms exam days. This Scheduler works only for Semester II. See "Sheet1" (below) for the Semester I Scheduler.</t>
   </si>
   <si>
     <t>Weekly Timings</t>
@@ -299,28 +290,285 @@
     <t>Time</t>
   </si>
   <si>
-    <t>2. Enter the date for the desired schedule in Fig. 3</t>
-  </si>
-  <si>
     <t>Weekend</t>
   </si>
   <si>
     <t>4. Make sure all the holidays are correctly marked in Fig. 4</t>
   </si>
   <si>
-    <t>1. Fill out course names in Fig. 1 (8 represents your Frees)</t>
-  </si>
-  <si>
-    <t>2. Fill out Fig. 2 with the period numbers from your rotational schedule (1-7). Then use 8 to represent any frees. Do include lab frees. For example: If you have 5th free, then all the 5's should be replaced with 8's.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. Enter date of a Past "A" Day of Sem I in Fig. 3 (e.g 8/15/2013) </t>
-  </si>
-  <si>
-    <t>1. Use the LATEST "A" day (before Date to Schedule) in Fig. 3</t>
-  </si>
-  <si>
-    <t>3. Enter date of a Past "A" Day of Sem II in Fig. 3 (e.g 1/6/2014)</t>
+    <r>
+      <t xml:space="preserve">1. Use the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LATEST "A" day</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (before Date to Schedule) in Fig. 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. Enter the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>date for the desired schedule</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in Fig. 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3. Enter </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">date of a Past "A" Day </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">of Sem I in Fig. 3 (e.g 8/15/2013) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. All the break / holiday dates from the Calendar have been added, except for wms exam days. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>This Scheduler works only for Semester I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. See "Sheet2" (below) for the Semester II Scheduler.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. This calculates your schedule on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assumption that it is always rolling from the PAD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, except for weekends and holidays.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3. Enter </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">date of a Past "A" Day </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">of Sem II in Fig. 3 (e.g 1/6/2014) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Fill out </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>course names</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in Fig. 1 (8 represents your Frees)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. All the break / holiday dates from the Calendar have been added, except for wms exam days. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>This Scheduler works only for Semester II.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> See "Sheet1" (below) for the Semester I Scheduler.</t>
+    </r>
+  </si>
+  <si>
+    <t>Fig. 2.1 (Example: 5th Free)</t>
+  </si>
+  <si>
+    <t>Fig. 2.3 (Example: 5th Free AND 7th Lab Frees on B and F days)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. Fill out Fig. 2 with the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>period numbers from your rotational schedule (1-7).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Then use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8 to represent any frees.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Make sure to include lab frees. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>See Fig 2.1 through Fig 2.3 (below Fig. 2) for examples.</t>
+    </r>
+  </si>
+  <si>
+    <t>Fig. 2.2 (Example: 7th Lab Frees on B and F days)</t>
   </si>
 </sst>
 </file>
@@ -384,7 +632,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -421,6 +669,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="44">
     <border>
@@ -969,7 +1223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1180,6 +1434,63 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1192,21 +1503,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1243,56 +1542,44 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1621,21 +1908,21 @@
   <sheetData>
     <row r="1" spans="2:25" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B2" s="104" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="105"/>
+      <c r="B2" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="93"/>
       <c r="D2" s="71"/>
-      <c r="E2" s="92" t="s">
+      <c r="E2" s="107" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="94"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
+      <c r="K2" s="108"/>
+      <c r="L2" s="109"/>
       <c r="N2" s="74" t="s">
         <v>32</v>
       </c>
@@ -1647,50 +1934,50 @@
       <c r="T2" s="29"/>
     </row>
     <row r="3" spans="2:25" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="107"/>
+      <c r="C3" s="95"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96" t="s">
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="96"/>
-      <c r="L3" s="97"/>
-      <c r="N3" s="77" t="s">
-        <v>33</v>
-      </c>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="78"/>
-      <c r="R3" s="78"/>
-      <c r="S3" s="79"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="112"/>
+      <c r="N3" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="O3" s="97"/>
+      <c r="P3" s="97"/>
+      <c r="Q3" s="97"/>
+      <c r="R3" s="97"/>
+      <c r="S3" s="98"/>
       <c r="T3" s="73"/>
       <c r="X3" s="29"/>
       <c r="Y3" s="29"/>
     </row>
     <row r="4" spans="2:25" ht="15" customHeight="1">
       <c r="D4" s="71"/>
-      <c r="E4" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="108" t="s">
-        <v>71</v>
-      </c>
-      <c r="K4" s="84"/>
-      <c r="L4" s="85"/>
-      <c r="N4" s="80"/>
+      <c r="E4" s="89" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="78"/>
+      <c r="L4" s="79"/>
+      <c r="N4" s="99"/>
       <c r="O4" s="81"/>
       <c r="P4" s="81"/>
       <c r="Q4" s="81"/>
@@ -1702,66 +1989,66 @@
     </row>
     <row r="5" spans="2:25" ht="15" customHeight="1">
       <c r="D5" s="71"/>
-      <c r="E5" s="100" t="s">
-        <v>77</v>
-      </c>
-      <c r="F5" s="101"/>
-      <c r="G5" s="101"/>
-      <c r="H5" s="101"/>
-      <c r="I5" s="101"/>
-      <c r="J5" s="109"/>
+      <c r="E5" s="113" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="114"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="114"/>
+      <c r="I5" s="114"/>
+      <c r="J5" s="80"/>
       <c r="K5" s="81"/>
       <c r="L5" s="82"/>
-      <c r="N5" s="83" t="s">
-        <v>50</v>
-      </c>
-      <c r="O5" s="84"/>
-      <c r="P5" s="84"/>
-      <c r="Q5" s="84"/>
-      <c r="R5" s="84"/>
-      <c r="S5" s="85"/>
+      <c r="N5" s="100" t="s">
+        <v>75</v>
+      </c>
+      <c r="O5" s="78"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="78"/>
+      <c r="S5" s="79"/>
       <c r="T5" s="73"/>
       <c r="X5" s="29"/>
       <c r="Y5" s="29"/>
     </row>
     <row r="6" spans="2:25" ht="15" customHeight="1">
       <c r="D6" s="71"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="101"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="101"/>
-      <c r="I6" s="101"/>
-      <c r="J6" s="99" t="s">
-        <v>79</v>
-      </c>
-      <c r="K6" s="99"/>
-      <c r="L6" s="110"/>
-      <c r="N6" s="86"/>
-      <c r="O6" s="87"/>
-      <c r="P6" s="87"/>
-      <c r="Q6" s="87"/>
-      <c r="R6" s="87"/>
-      <c r="S6" s="88"/>
+      <c r="E6" s="113"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="114"/>
+      <c r="H6" s="114"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="83" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" s="83"/>
+      <c r="L6" s="84"/>
+      <c r="N6" s="101"/>
+      <c r="O6" s="102"/>
+      <c r="P6" s="102"/>
+      <c r="Q6" s="102"/>
+      <c r="R6" s="102"/>
+      <c r="S6" s="103"/>
       <c r="T6" s="73"/>
       <c r="X6" s="29"/>
       <c r="Y6" s="29"/>
     </row>
     <row r="7" spans="2:25" ht="15.75" thickBot="1">
       <c r="D7" s="71"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="99"/>
-      <c r="K7" s="99"/>
-      <c r="L7" s="110"/>
-      <c r="N7" s="89"/>
-      <c r="O7" s="90"/>
-      <c r="P7" s="90"/>
-      <c r="Q7" s="90"/>
-      <c r="R7" s="90"/>
-      <c r="S7" s="91"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="114"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="84"/>
+      <c r="N7" s="104"/>
+      <c r="O7" s="105"/>
+      <c r="P7" s="105"/>
+      <c r="Q7" s="105"/>
+      <c r="R7" s="105"/>
+      <c r="S7" s="106"/>
       <c r="T7" s="73"/>
       <c r="X7" s="29"/>
       <c r="Y7" s="29"/>
@@ -1772,16 +2059,16 @@
       </c>
       <c r="C8" s="76"/>
       <c r="D8" s="71"/>
-      <c r="E8" s="100"/>
-      <c r="F8" s="101"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="101"/>
-      <c r="I8" s="101"/>
-      <c r="J8" s="111" t="s">
+      <c r="E8" s="113"/>
+      <c r="F8" s="114"/>
+      <c r="G8" s="114"/>
+      <c r="H8" s="114"/>
+      <c r="I8" s="114"/>
+      <c r="J8" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="K8" s="111"/>
-      <c r="L8" s="112"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="86"/>
     </row>
     <row r="9" spans="2:25" ht="15.75" customHeight="1" thickBot="1">
       <c r="B9" s="15" t="s">
@@ -1790,34 +2077,34 @@
       <c r="C9" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" s="99"/>
-      <c r="G9" s="99"/>
-      <c r="H9" s="99"/>
-      <c r="I9" s="99"/>
-      <c r="J9" s="111"/>
-      <c r="K9" s="111"/>
-      <c r="L9" s="112"/>
+      <c r="E9" s="89" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="85"/>
+      <c r="L9" s="86"/>
     </row>
     <row r="10" spans="2:25" ht="15.75" customHeight="1" thickBot="1">
       <c r="B10" s="18">
         <v>0</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="E10" s="98"/>
-      <c r="F10" s="99"/>
-      <c r="G10" s="99"/>
-      <c r="H10" s="99"/>
-      <c r="I10" s="99"/>
-      <c r="J10" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="89"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="K10" s="99"/>
-      <c r="L10" s="110"/>
+      <c r="K10" s="83"/>
+      <c r="L10" s="84"/>
       <c r="N10" s="12" t="s">
         <v>24</v>
       </c>
@@ -1835,16 +2122,16 @@
       <c r="C11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="102" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" s="103"/>
-      <c r="G11" s="103"/>
-      <c r="H11" s="103"/>
-      <c r="I11" s="103"/>
-      <c r="J11" s="113"/>
-      <c r="K11" s="113"/>
-      <c r="L11" s="114"/>
+      <c r="E11" s="90" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="91"/>
+      <c r="G11" s="91"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="91"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="88"/>
       <c r="N11" s="14" t="s">
         <v>11</v>
       </c>
@@ -1886,7 +2173,7 @@
         <v>4</v>
       </c>
       <c r="S12" s="65" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="2:25" ht="15.75" thickBot="1">
@@ -1915,7 +2202,7 @@
         <v>0.5</v>
       </c>
       <c r="Q13" s="47">
-        <f>INDEX(F22:L25, 1, N18)</f>
+        <f>INDEX(F43:L46, 1, N18)</f>
         <v>9</v>
       </c>
       <c r="R13" s="61" t="str">
@@ -1923,7 +2210,7 @@
         <v>Office Hours</v>
       </c>
       <c r="S13" s="66" t="str">
-        <f>INDEX(F29:L32, 1, N18)</f>
+        <f>INDEX(F50:L53, 1, N18)</f>
         <v>8:00-8:30</v>
       </c>
     </row>
@@ -1975,7 +2262,7 @@
         <v>Bible</v>
       </c>
       <c r="S14" s="67" t="str">
-        <f>INDEX(F33:L36, P14, N18)</f>
+        <f>INDEX(F54:L57, P14, N18)</f>
         <v>8:30-9:40</v>
       </c>
     </row>
@@ -1994,7 +2281,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H15" s="3">
         <v>2</v>
@@ -2019,7 +2306,7 @@
         <v>1.5</v>
       </c>
       <c r="Q15" s="48">
-        <f>INDEX(F22:L25, 2, N18)</f>
+        <f>INDEX(F43:L46, 2, N18)</f>
         <v>12</v>
       </c>
       <c r="R15" s="61" t="str">
@@ -2027,7 +2314,7 @@
         <v>ADV</v>
       </c>
       <c r="S15" s="66" t="str">
-        <f>INDEX(F29:L32, 2, N18)</f>
+        <f>INDEX(F50:L53, 2, N18)</f>
         <v>9:40-9:55</v>
       </c>
     </row>
@@ -2061,7 +2348,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N16" s="53">
         <f>MAX(NETWORKDAYS(N12, N14,N22:N123)-1, 0)</f>
@@ -2073,14 +2360,14 @@
       </c>
       <c r="Q16" s="44">
         <f>INDEX(F15:L18,P16, Q11)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="R16" s="62" t="str">
         <f>INDEX(C11:C18, Q16, 1)</f>
-        <v>Free</v>
+        <v>English</v>
       </c>
       <c r="S16" s="67" t="str">
-        <f>INDEX(F33:L36, P16, N18)</f>
+        <f>INDEX(F54:L57, P16, N18)</f>
         <v>9:55-11:05</v>
       </c>
     </row>
@@ -2108,7 +2395,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K17" s="3">
         <v>2</v>
@@ -2117,7 +2404,7 @@
         <v>6</v>
       </c>
       <c r="N17" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O17" s="54"/>
       <c r="P17" s="43">
@@ -2132,7 +2419,7 @@
         <v>Orchestra</v>
       </c>
       <c r="S17" s="67" t="str">
-        <f>INDEX(F33:L36, P17, N18)</f>
+        <f>INDEX(F54:L57, P17, N18)</f>
         <v>11:05-1:10</v>
       </c>
     </row>
@@ -2154,7 +2441,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I18" s="5">
         <v>2</v>
@@ -2177,7 +2464,7 @@
         <v>3.5</v>
       </c>
       <c r="Q18" s="48">
-        <f>INDEX(F22:L25, 3, N18)</f>
+        <f>INDEX(F43:L46, 3, N18)</f>
         <v>10</v>
       </c>
       <c r="R18" s="61" t="str">
@@ -2185,7 +2472,7 @@
         <v>Break</v>
       </c>
       <c r="S18" s="66" t="str">
-        <f>INDEX(F29:L32, 3, N18)</f>
+        <f>INDEX(F50:L53, 3, N18)</f>
         <v>1:10-1:20</v>
       </c>
     </row>
@@ -2195,7 +2482,7 @@
         <v>9</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O19" s="28"/>
       <c r="P19" s="43">
@@ -2210,7 +2497,7 @@
         <v>Physics</v>
       </c>
       <c r="S19" s="67" t="str">
-        <f>INDEX(F33:L36, P19, N18)</f>
+        <f>INDEX(F54:L57, P19, N18)</f>
         <v>1:20-2:30</v>
       </c>
     </row>
@@ -2220,10 +2507,10 @@
         <v>10</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E20" s="74" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="F20" s="75"/>
       <c r="G20" s="75"/>
@@ -2240,7 +2527,7 @@
         <v>4.5</v>
       </c>
       <c r="Q20" s="49">
-        <f>INDEX(F22:L25, 4, N18)</f>
+        <f>INDEX(F43:L46, 4, N18)</f>
         <v>0</v>
       </c>
       <c r="R20" s="64" t="str">
@@ -2248,7 +2535,7 @@
         <v>Weekend</v>
       </c>
       <c r="S20" s="68">
-        <f>INDEX(F29:L32, 4, N18)</f>
+        <f>INDEX(F50:L53, 4, N18)</f>
         <v>0</v>
       </c>
     </row>
@@ -2258,31 +2545,31 @@
         <v>11</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="G21" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="H21" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="I21" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="J21" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="K21" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="115" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="116" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="116" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="116" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="116" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="116" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="L21" s="35" t="s">
-        <v>49</v>
+      <c r="L21" s="117" t="s">
+        <v>20</v>
       </c>
       <c r="N21" s="13" t="s">
         <v>0</v>
@@ -2295,31 +2582,31 @@
         <v>12</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="50">
-        <v>0.5</v>
-      </c>
-      <c r="F22" s="45">
-        <v>0</v>
-      </c>
-      <c r="G22" s="45">
-        <v>9</v>
-      </c>
-      <c r="H22" s="45">
-        <v>13</v>
-      </c>
-      <c r="I22" s="45">
-        <v>14</v>
-      </c>
-      <c r="J22" s="45">
-        <v>13</v>
-      </c>
-      <c r="K22" s="45">
-        <v>9</v>
-      </c>
-      <c r="L22" s="38">
-        <v>0</v>
+        <v>41</v>
+      </c>
+      <c r="E22" s="43">
+        <v>1</v>
+      </c>
+      <c r="F22" s="118">
+        <v>1</v>
+      </c>
+      <c r="G22" s="123">
+        <v>8</v>
+      </c>
+      <c r="H22" s="118">
+        <v>2</v>
+      </c>
+      <c r="I22" s="118">
+        <v>6</v>
+      </c>
+      <c r="J22" s="118">
+        <v>3</v>
+      </c>
+      <c r="K22" s="118">
+        <v>7</v>
+      </c>
+      <c r="L22" s="119">
+        <v>4</v>
       </c>
       <c r="N22" s="7">
         <v>41459</v>
@@ -2332,31 +2619,31 @@
         <v>13</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="50">
-        <v>1.5</v>
-      </c>
-      <c r="F23" s="45">
-        <v>0</v>
-      </c>
-      <c r="G23" s="45">
-        <v>10</v>
-      </c>
-      <c r="H23" s="45">
-        <v>10</v>
-      </c>
-      <c r="I23" s="45">
-        <v>10</v>
-      </c>
-      <c r="J23" s="45">
-        <v>11</v>
-      </c>
-      <c r="K23" s="45">
-        <v>12</v>
-      </c>
-      <c r="L23" s="38">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="E23" s="43">
+        <v>2</v>
+      </c>
+      <c r="F23" s="118">
+        <v>2</v>
+      </c>
+      <c r="G23" s="118">
+        <v>6</v>
+      </c>
+      <c r="H23" s="118">
+        <v>3</v>
+      </c>
+      <c r="I23" s="118">
+        <v>7</v>
+      </c>
+      <c r="J23" s="118">
+        <v>4</v>
+      </c>
+      <c r="K23" s="118">
+        <v>1</v>
+      </c>
+      <c r="L23" s="124">
+        <v>8</v>
       </c>
       <c r="N23" s="7">
         <v>41519</v>
@@ -2369,31 +2656,31 @@
         <v>14</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="50">
-        <v>3.5</v>
-      </c>
-      <c r="F24" s="45">
-        <v>0</v>
-      </c>
-      <c r="G24" s="45">
-        <v>15</v>
-      </c>
-      <c r="H24" s="45">
-        <v>15</v>
-      </c>
-      <c r="I24" s="45">
-        <v>10</v>
-      </c>
-      <c r="J24" s="45">
-        <v>10</v>
-      </c>
-      <c r="K24" s="45">
-        <v>10</v>
-      </c>
-      <c r="L24" s="38">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="E24" s="43">
+        <v>3</v>
+      </c>
+      <c r="F24" s="118">
+        <v>3</v>
+      </c>
+      <c r="G24" s="118">
+        <v>7</v>
+      </c>
+      <c r="H24" s="118">
+        <v>4</v>
+      </c>
+      <c r="I24" s="118">
+        <v>1</v>
+      </c>
+      <c r="J24" s="123">
+        <v>8</v>
+      </c>
+      <c r="K24" s="118">
+        <v>2</v>
+      </c>
+      <c r="L24" s="119">
+        <v>6</v>
       </c>
       <c r="N24" s="7">
         <v>41561</v>
@@ -2408,31 +2695,31 @@
         <v>15</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="E25" s="51">
-        <v>4.5</v>
-      </c>
-      <c r="F25" s="52">
-        <v>0</v>
-      </c>
-      <c r="G25" s="52">
-        <v>9</v>
-      </c>
-      <c r="H25" s="52">
-        <v>9</v>
-      </c>
-      <c r="I25" s="52">
-        <v>9</v>
-      </c>
-      <c r="J25" s="52">
-        <v>9</v>
-      </c>
-      <c r="K25" s="52">
-        <v>0</v>
-      </c>
-      <c r="L25" s="39">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="E25" s="120">
+        <v>4</v>
+      </c>
+      <c r="F25" s="121">
+        <v>4</v>
+      </c>
+      <c r="G25" s="121">
+        <v>1</v>
+      </c>
+      <c r="H25" s="125">
+        <v>8</v>
+      </c>
+      <c r="I25" s="121">
+        <v>2</v>
+      </c>
+      <c r="J25" s="121">
+        <v>6</v>
+      </c>
+      <c r="K25" s="121">
+        <v>3</v>
+      </c>
+      <c r="L25" s="122">
+        <v>7</v>
       </c>
       <c r="N25" s="7">
         <v>41563</v>
@@ -2442,7 +2729,7 @@
       <c r="S25" s="27"/>
     </row>
     <row r="26" spans="2:19" ht="15.75" thickBot="1">
-      <c r="E26" s="30"/>
+      <c r="E26" s="28"/>
       <c r="N26" s="7">
         <v>41565</v>
       </c>
@@ -2452,7 +2739,7 @@
     </row>
     <row r="27" spans="2:19" ht="15.75" thickBot="1">
       <c r="E27" s="74" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="F27" s="75"/>
       <c r="G27" s="75"/>
@@ -2468,29 +2755,29 @@
       <c r="Q27" s="26"/>
     </row>
     <row r="28" spans="2:19">
-      <c r="E28" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F28" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="G28" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="H28" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="I28" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="J28" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="K28" s="34" t="s">
+      <c r="E28" s="115" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="116" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="116" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="116" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" s="116" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="116" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="L28" s="35" t="s">
-        <v>49</v>
+      <c r="L28" s="117" t="s">
+        <v>20</v>
       </c>
       <c r="N28" s="7">
         <v>41603</v>
@@ -2500,29 +2787,29 @@
       <c r="S28" s="25"/>
     </row>
     <row r="29" spans="2:19">
-      <c r="E29" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="F29" s="55">
-        <v>0</v>
-      </c>
-      <c r="G29" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="H29" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="I29" s="55" t="s">
-        <v>62</v>
-      </c>
-      <c r="J29" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="K29" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="L29" s="56">
-        <v>0</v>
+      <c r="E29" s="43">
+        <v>1</v>
+      </c>
+      <c r="F29" s="118">
+        <v>1</v>
+      </c>
+      <c r="G29" s="118">
+        <v>5</v>
+      </c>
+      <c r="H29" s="118">
+        <v>2</v>
+      </c>
+      <c r="I29" s="118">
+        <v>6</v>
+      </c>
+      <c r="J29" s="118">
+        <v>3</v>
+      </c>
+      <c r="K29" s="123">
+        <v>8</v>
+      </c>
+      <c r="L29" s="119">
+        <v>4</v>
       </c>
       <c r="N29" s="7">
         <v>41604</v>
@@ -2532,29 +2819,29 @@
       <c r="S29" s="26"/>
     </row>
     <row r="30" spans="2:19">
-      <c r="E30" s="18">
-        <v>1.5</v>
-      </c>
-      <c r="F30" s="55">
-        <v>0</v>
-      </c>
-      <c r="G30" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="H30" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="I30" s="55" t="s">
-        <v>64</v>
-      </c>
-      <c r="J30" s="55" t="s">
-        <v>68</v>
-      </c>
-      <c r="K30" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="L30" s="56">
-        <v>0</v>
+      <c r="E30" s="43">
+        <v>2</v>
+      </c>
+      <c r="F30" s="118">
+        <v>2</v>
+      </c>
+      <c r="G30" s="118">
+        <v>6</v>
+      </c>
+      <c r="H30" s="118">
+        <v>3</v>
+      </c>
+      <c r="I30" s="118">
+        <v>7</v>
+      </c>
+      <c r="J30" s="118">
+        <v>4</v>
+      </c>
+      <c r="K30" s="118">
+        <v>1</v>
+      </c>
+      <c r="L30" s="119">
+        <v>5</v>
       </c>
       <c r="N30" s="7">
         <v>41605</v>
@@ -2564,29 +2851,29 @@
       <c r="S30" s="27"/>
     </row>
     <row r="31" spans="2:19">
-      <c r="E31" s="18">
-        <v>3.5</v>
-      </c>
-      <c r="F31" s="55">
-        <v>0</v>
-      </c>
-      <c r="G31" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="H31" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="I31" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="J31" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="K31" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="L31" s="56">
-        <v>0</v>
+      <c r="E31" s="43">
+        <v>3</v>
+      </c>
+      <c r="F31" s="118">
+        <v>3</v>
+      </c>
+      <c r="G31" s="123">
+        <v>8</v>
+      </c>
+      <c r="H31" s="118">
+        <v>4</v>
+      </c>
+      <c r="I31" s="118">
+        <v>1</v>
+      </c>
+      <c r="J31" s="118">
+        <v>5</v>
+      </c>
+      <c r="K31" s="118">
+        <v>2</v>
+      </c>
+      <c r="L31" s="119">
+        <v>6</v>
       </c>
       <c r="N31" s="7">
         <v>41606</v>
@@ -2595,30 +2882,30 @@
       <c r="Q31" s="60"/>
       <c r="S31" s="27"/>
     </row>
-    <row r="32" spans="2:19">
-      <c r="E32" s="18">
-        <v>4.5</v>
-      </c>
-      <c r="F32" s="55">
-        <v>0</v>
-      </c>
-      <c r="G32" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="H32" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="I32" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="J32" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="K32" s="55">
-        <v>0</v>
-      </c>
-      <c r="L32" s="56">
-        <v>0</v>
+    <row r="32" spans="2:19" ht="15.75" thickBot="1">
+      <c r="E32" s="120">
+        <v>4</v>
+      </c>
+      <c r="F32" s="121">
+        <v>4</v>
+      </c>
+      <c r="G32" s="121">
+        <v>1</v>
+      </c>
+      <c r="H32" s="121">
+        <v>5</v>
+      </c>
+      <c r="I32" s="121">
+        <v>2</v>
+      </c>
+      <c r="J32" s="121">
+        <v>6</v>
+      </c>
+      <c r="K32" s="121">
+        <v>3</v>
+      </c>
+      <c r="L32" s="122">
+        <v>7</v>
       </c>
       <c r="N32" s="7">
         <v>41607</v>
@@ -2627,204 +2914,596 @@
       <c r="Q32" s="60"/>
       <c r="S32" s="27"/>
     </row>
-    <row r="33" spans="5:17">
-      <c r="E33" s="18">
-        <v>1</v>
-      </c>
-      <c r="F33" s="55">
-        <v>0</v>
-      </c>
-      <c r="G33" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="H33" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="I33" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J33" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="K33" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="L33" s="56">
-        <v>0</v>
-      </c>
+    <row r="33" spans="5:17" ht="15.75" thickBot="1">
+      <c r="E33" s="28"/>
       <c r="N33" s="7"/>
       <c r="O33" s="60"/>
       <c r="Q33" s="60"/>
     </row>
-    <row r="34" spans="5:17">
-      <c r="E34" s="18">
-        <v>2</v>
-      </c>
-      <c r="F34" s="55">
-        <v>0</v>
-      </c>
-      <c r="G34" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="H34" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="I34" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="J34" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="K34" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="L34" s="56">
-        <v>0</v>
-      </c>
+    <row r="34" spans="5:17" ht="15.75" thickBot="1">
+      <c r="E34" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="F34" s="75"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="75"/>
+      <c r="I34" s="75"/>
+      <c r="J34" s="75"/>
+      <c r="K34" s="75"/>
+      <c r="L34" s="76"/>
       <c r="N34" s="7"/>
       <c r="O34" s="60"/>
       <c r="Q34" s="60"/>
     </row>
     <row r="35" spans="5:17">
-      <c r="E35" s="18">
-        <v>3</v>
-      </c>
-      <c r="F35" s="55">
-        <v>0</v>
-      </c>
-      <c r="G35" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="H35" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="I35" s="55" t="s">
-        <v>66</v>
-      </c>
-      <c r="J35" s="55" t="s">
-        <v>66</v>
-      </c>
-      <c r="K35" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="L35" s="56">
-        <v>0</v>
+      <c r="E35" s="115" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" s="116" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="116" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="116" t="s">
+        <v>17</v>
+      </c>
+      <c r="I35" s="116" t="s">
+        <v>18</v>
+      </c>
+      <c r="J35" s="116" t="s">
+        <v>19</v>
+      </c>
+      <c r="K35" s="116" t="s">
+        <v>14</v>
+      </c>
+      <c r="L35" s="117" t="s">
+        <v>20</v>
       </c>
       <c r="N35" s="7"/>
       <c r="O35" s="60"/>
       <c r="Q35" s="60"/>
     </row>
-    <row r="36" spans="5:17" ht="15.75" thickBot="1">
-      <c r="E36" s="20">
+    <row r="36" spans="5:17">
+      <c r="E36" s="43">
+        <v>1</v>
+      </c>
+      <c r="F36" s="118">
+        <v>1</v>
+      </c>
+      <c r="G36" s="123">
+        <v>8</v>
+      </c>
+      <c r="H36" s="118">
+        <v>2</v>
+      </c>
+      <c r="I36" s="118">
+        <v>6</v>
+      </c>
+      <c r="J36" s="118">
+        <v>3</v>
+      </c>
+      <c r="K36" s="123">
+        <v>8</v>
+      </c>
+      <c r="L36" s="119">
         <v>4</v>
-      </c>
-      <c r="F36" s="57">
-        <v>0</v>
-      </c>
-      <c r="G36" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="H36" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="I36" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="J36" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="K36" s="57" t="s">
-        <v>70</v>
-      </c>
-      <c r="L36" s="58">
-        <v>0</v>
       </c>
       <c r="N36" s="7"/>
       <c r="O36" s="60"/>
       <c r="Q36" s="60"/>
     </row>
     <row r="37" spans="5:17">
+      <c r="E37" s="43">
+        <v>2</v>
+      </c>
+      <c r="F37" s="118">
+        <v>2</v>
+      </c>
+      <c r="G37" s="118">
+        <v>6</v>
+      </c>
+      <c r="H37" s="118">
+        <v>3</v>
+      </c>
+      <c r="I37" s="118">
+        <v>7</v>
+      </c>
+      <c r="J37" s="118">
+        <v>4</v>
+      </c>
+      <c r="K37" s="118">
+        <v>1</v>
+      </c>
+      <c r="L37" s="124">
+        <v>8</v>
+      </c>
       <c r="N37" s="7"/>
     </row>
     <row r="38" spans="5:17">
+      <c r="E38" s="43">
+        <v>3</v>
+      </c>
+      <c r="F38" s="118">
+        <v>3</v>
+      </c>
+      <c r="G38" s="123">
+        <v>8</v>
+      </c>
+      <c r="H38" s="118">
+        <v>4</v>
+      </c>
+      <c r="I38" s="118">
+        <v>1</v>
+      </c>
+      <c r="J38" s="123">
+        <v>8</v>
+      </c>
+      <c r="K38" s="118">
+        <v>2</v>
+      </c>
+      <c r="L38" s="119">
+        <v>6</v>
+      </c>
       <c r="N38" s="7"/>
     </row>
-    <row r="39" spans="5:17">
+    <row r="39" spans="5:17" ht="15.75" thickBot="1">
+      <c r="E39" s="120">
+        <v>4</v>
+      </c>
+      <c r="F39" s="121">
+        <v>4</v>
+      </c>
+      <c r="G39" s="121">
+        <v>1</v>
+      </c>
+      <c r="H39" s="125">
+        <v>8</v>
+      </c>
+      <c r="I39" s="121">
+        <v>2</v>
+      </c>
+      <c r="J39" s="121">
+        <v>6</v>
+      </c>
+      <c r="K39" s="121">
+        <v>3</v>
+      </c>
+      <c r="L39" s="122">
+        <v>7</v>
+      </c>
       <c r="N39" s="7"/>
     </row>
-    <row r="40" spans="5:17">
+    <row r="40" spans="5:17" ht="15.75" thickBot="1">
       <c r="N40" s="7"/>
     </row>
-    <row r="41" spans="5:17">
+    <row r="41" spans="5:17" ht="15.75" thickBot="1">
+      <c r="E41" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" s="75"/>
+      <c r="G41" s="75"/>
+      <c r="H41" s="75"/>
+      <c r="I41" s="75"/>
+      <c r="J41" s="75"/>
+      <c r="K41" s="75"/>
+      <c r="L41" s="76"/>
       <c r="N41" s="7"/>
     </row>
     <row r="42" spans="5:17">
+      <c r="E42" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F42" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="G42" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="H42" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="I42" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="J42" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="K42" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="L42" s="35" t="s">
+        <v>48</v>
+      </c>
       <c r="N42" s="7"/>
     </row>
     <row r="43" spans="5:17">
+      <c r="E43" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="F43" s="45">
+        <v>0</v>
+      </c>
+      <c r="G43" s="45">
+        <v>9</v>
+      </c>
+      <c r="H43" s="45">
+        <v>13</v>
+      </c>
+      <c r="I43" s="45">
+        <v>14</v>
+      </c>
+      <c r="J43" s="45">
+        <v>13</v>
+      </c>
+      <c r="K43" s="45">
+        <v>9</v>
+      </c>
+      <c r="L43" s="38">
+        <v>0</v>
+      </c>
       <c r="N43" s="7"/>
     </row>
     <row r="44" spans="5:17">
+      <c r="E44" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="F44" s="45">
+        <v>0</v>
+      </c>
+      <c r="G44" s="45">
+        <v>10</v>
+      </c>
+      <c r="H44" s="45">
+        <v>10</v>
+      </c>
+      <c r="I44" s="45">
+        <v>10</v>
+      </c>
+      <c r="J44" s="45">
+        <v>11</v>
+      </c>
+      <c r="K44" s="45">
+        <v>12</v>
+      </c>
+      <c r="L44" s="38">
+        <v>0</v>
+      </c>
       <c r="N44" s="7"/>
     </row>
     <row r="45" spans="5:17">
+      <c r="E45" s="50">
+        <v>3.5</v>
+      </c>
+      <c r="F45" s="45">
+        <v>0</v>
+      </c>
+      <c r="G45" s="45">
+        <v>15</v>
+      </c>
+      <c r="H45" s="45">
+        <v>15</v>
+      </c>
+      <c r="I45" s="45">
+        <v>10</v>
+      </c>
+      <c r="J45" s="45">
+        <v>10</v>
+      </c>
+      <c r="K45" s="45">
+        <v>10</v>
+      </c>
+      <c r="L45" s="38">
+        <v>0</v>
+      </c>
       <c r="N45" s="7"/>
     </row>
-    <row r="46" spans="5:17">
+    <row r="46" spans="5:17" ht="15.75" thickBot="1">
+      <c r="E46" s="51">
+        <v>4.5</v>
+      </c>
+      <c r="F46" s="52">
+        <v>0</v>
+      </c>
+      <c r="G46" s="52">
+        <v>9</v>
+      </c>
+      <c r="H46" s="52">
+        <v>9</v>
+      </c>
+      <c r="I46" s="52">
+        <v>9</v>
+      </c>
+      <c r="J46" s="52">
+        <v>9</v>
+      </c>
+      <c r="K46" s="52">
+        <v>0</v>
+      </c>
+      <c r="L46" s="39">
+        <v>0</v>
+      </c>
       <c r="N46" s="7"/>
     </row>
-    <row r="47" spans="5:17">
+    <row r="47" spans="5:17" ht="15.75" thickBot="1">
+      <c r="E47" s="30"/>
       <c r="N47" s="7"/>
     </row>
-    <row r="48" spans="5:17">
+    <row r="48" spans="5:17" ht="15.75" thickBot="1">
+      <c r="E48" s="74" t="s">
+        <v>49</v>
+      </c>
+      <c r="F48" s="75"/>
+      <c r="G48" s="75"/>
+      <c r="H48" s="75"/>
+      <c r="I48" s="75"/>
+      <c r="J48" s="75"/>
+      <c r="K48" s="75"/>
+      <c r="L48" s="76"/>
       <c r="N48" s="7"/>
     </row>
-    <row r="49" spans="14:14">
+    <row r="49" spans="5:14">
+      <c r="E49" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F49" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="G49" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="H49" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="I49" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="J49" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="K49" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="L49" s="35" t="s">
+        <v>48</v>
+      </c>
       <c r="N49" s="7"/>
     </row>
-    <row r="50" spans="14:14">
+    <row r="50" spans="5:14">
+      <c r="E50" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="F50" s="55">
+        <v>0</v>
+      </c>
+      <c r="G50" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="H50" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="I50" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="J50" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="K50" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="L50" s="56">
+        <v>0</v>
+      </c>
       <c r="N50" s="7"/>
     </row>
-    <row r="51" spans="14:14">
+    <row r="51" spans="5:14">
+      <c r="E51" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="F51" s="55">
+        <v>0</v>
+      </c>
+      <c r="G51" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="H51" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="I51" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="J51" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="K51" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="L51" s="56">
+        <v>0</v>
+      </c>
       <c r="N51" s="7"/>
     </row>
-    <row r="52" spans="14:14">
+    <row r="52" spans="5:14">
+      <c r="E52" s="18">
+        <v>3.5</v>
+      </c>
+      <c r="F52" s="55">
+        <v>0</v>
+      </c>
+      <c r="G52" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="H52" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="I52" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="J52" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="K52" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="L52" s="56">
+        <v>0</v>
+      </c>
       <c r="N52" s="7"/>
     </row>
-    <row r="53" spans="14:14">
+    <row r="53" spans="5:14">
+      <c r="E53" s="18">
+        <v>4.5</v>
+      </c>
+      <c r="F53" s="55">
+        <v>0</v>
+      </c>
+      <c r="G53" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="H53" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I53" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="J53" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="K53" s="55">
+        <v>0</v>
+      </c>
+      <c r="L53" s="56">
+        <v>0</v>
+      </c>
       <c r="N53" s="7"/>
     </row>
-    <row r="54" spans="14:14">
+    <row r="54" spans="5:14">
+      <c r="E54" s="18">
+        <v>1</v>
+      </c>
+      <c r="F54" s="55">
+        <v>0</v>
+      </c>
+      <c r="G54" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="H54" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="I54" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="J54" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="K54" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="L54" s="56">
+        <v>0</v>
+      </c>
       <c r="N54" s="7"/>
     </row>
-    <row r="55" spans="14:14">
+    <row r="55" spans="5:14">
+      <c r="E55" s="18">
+        <v>2</v>
+      </c>
+      <c r="F55" s="55">
+        <v>0</v>
+      </c>
+      <c r="G55" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="H55" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="I55" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="J55" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="K55" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="L55" s="56">
+        <v>0</v>
+      </c>
       <c r="N55" s="7"/>
     </row>
-    <row r="56" spans="14:14">
+    <row r="56" spans="5:14">
+      <c r="E56" s="18">
+        <v>3</v>
+      </c>
+      <c r="F56" s="55">
+        <v>0</v>
+      </c>
+      <c r="G56" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="H56" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I56" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="J56" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="K56" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="L56" s="56">
+        <v>0</v>
+      </c>
       <c r="N56" s="7"/>
     </row>
-    <row r="57" spans="14:14">
+    <row r="57" spans="5:14" ht="15.75" thickBot="1">
+      <c r="E57" s="20">
+        <v>4</v>
+      </c>
+      <c r="F57" s="57">
+        <v>0</v>
+      </c>
+      <c r="G57" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="H57" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="I57" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="J57" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="K57" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="L57" s="58">
+        <v>0</v>
+      </c>
       <c r="N57" s="7"/>
     </row>
-    <row r="58" spans="14:14">
+    <row r="58" spans="5:14">
       <c r="N58" s="7"/>
     </row>
-    <row r="59" spans="14:14">
+    <row r="59" spans="5:14">
       <c r="N59" s="7"/>
     </row>
-    <row r="60" spans="14:14">
+    <row r="60" spans="5:14">
       <c r="N60" s="7"/>
     </row>
-    <row r="61" spans="14:14">
+    <row r="61" spans="5:14">
       <c r="N61" s="7"/>
     </row>
-    <row r="62" spans="14:14">
+    <row r="62" spans="5:14">
       <c r="N62" s="7"/>
     </row>
-    <row r="63" spans="14:14">
+    <row r="63" spans="5:14">
       <c r="N63" s="7"/>
     </row>
-    <row r="64" spans="14:14">
+    <row r="64" spans="5:14">
       <c r="N64" s="7"/>
     </row>
     <row r="65" spans="14:14">
@@ -3006,17 +3685,10 @@
     </row>
   </sheetData>
   <sheetProtection password="C836" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
-  <mergeCells count="21">
-    <mergeCell ref="P10:S10"/>
-    <mergeCell ref="E13:L13"/>
-    <mergeCell ref="E20:L20"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="J4:L5"/>
-    <mergeCell ref="J6:L7"/>
-    <mergeCell ref="J8:L9"/>
-    <mergeCell ref="J10:L11"/>
-    <mergeCell ref="E9:I10"/>
-    <mergeCell ref="E11:I11"/>
+  <mergeCells count="24">
+    <mergeCell ref="E34:L34"/>
+    <mergeCell ref="E41:L41"/>
+    <mergeCell ref="E48:L48"/>
     <mergeCell ref="E27:L27"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -3028,6 +3700,16 @@
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="E4:I4"/>
     <mergeCell ref="E5:I8"/>
+    <mergeCell ref="E20:L20"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="E13:L13"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="J4:L5"/>
+    <mergeCell ref="J6:L7"/>
+    <mergeCell ref="J8:L9"/>
+    <mergeCell ref="J10:L11"/>
+    <mergeCell ref="E9:I10"/>
+    <mergeCell ref="E11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3075,21 +3757,21 @@
       <c r="J1" s="72"/>
     </row>
     <row r="2" spans="2:25" ht="15.75" thickBot="1">
-      <c r="B2" s="104" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="105"/>
+      <c r="B2" s="92" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="93"/>
       <c r="D2" s="71"/>
-      <c r="E2" s="92" t="s">
+      <c r="E2" s="107" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="94"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
+      <c r="K2" s="108"/>
+      <c r="L2" s="109"/>
       <c r="N2" s="74" t="s">
         <v>32</v>
       </c>
@@ -3101,50 +3783,50 @@
       <c r="T2" s="29"/>
     </row>
     <row r="3" spans="2:25" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="107"/>
+      <c r="C3" s="95"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96" t="s">
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="96"/>
-      <c r="L3" s="97"/>
-      <c r="N3" s="77" t="s">
-        <v>33</v>
-      </c>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="78"/>
-      <c r="R3" s="78"/>
-      <c r="S3" s="79"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="112"/>
+      <c r="N3" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="O3" s="97"/>
+      <c r="P3" s="97"/>
+      <c r="Q3" s="97"/>
+      <c r="R3" s="97"/>
+      <c r="S3" s="98"/>
       <c r="T3" s="73"/>
       <c r="X3" s="29"/>
       <c r="Y3" s="29"/>
     </row>
     <row r="4" spans="2:25" ht="15" customHeight="1">
       <c r="D4" s="71"/>
-      <c r="E4" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="108" t="s">
-        <v>71</v>
-      </c>
-      <c r="K4" s="84"/>
-      <c r="L4" s="85"/>
-      <c r="N4" s="80"/>
+      <c r="E4" s="89" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="78"/>
+      <c r="L4" s="79"/>
+      <c r="N4" s="99"/>
       <c r="O4" s="81"/>
       <c r="P4" s="81"/>
       <c r="Q4" s="81"/>
@@ -3156,66 +3838,66 @@
     </row>
     <row r="5" spans="2:25" ht="15" customHeight="1">
       <c r="D5" s="71"/>
-      <c r="E5" s="100" t="s">
-        <v>77</v>
-      </c>
-      <c r="F5" s="101"/>
-      <c r="G5" s="101"/>
-      <c r="H5" s="101"/>
-      <c r="I5" s="101"/>
-      <c r="J5" s="109"/>
+      <c r="E5" s="113" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="114"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="114"/>
+      <c r="I5" s="114"/>
+      <c r="J5" s="80"/>
       <c r="K5" s="81"/>
       <c r="L5" s="82"/>
-      <c r="N5" s="83" t="s">
-        <v>51</v>
-      </c>
-      <c r="O5" s="84"/>
-      <c r="P5" s="84"/>
-      <c r="Q5" s="84"/>
-      <c r="R5" s="84"/>
-      <c r="S5" s="85"/>
+      <c r="N5" s="100" t="s">
+        <v>79</v>
+      </c>
+      <c r="O5" s="78"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="78"/>
+      <c r="S5" s="79"/>
       <c r="T5" s="73"/>
       <c r="X5" s="29"/>
       <c r="Y5" s="29"/>
     </row>
     <row r="6" spans="2:25" ht="15" customHeight="1">
       <c r="D6" s="71"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="101"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="101"/>
-      <c r="I6" s="101"/>
-      <c r="J6" s="99" t="s">
-        <v>79</v>
-      </c>
-      <c r="K6" s="99"/>
-      <c r="L6" s="110"/>
-      <c r="N6" s="86"/>
-      <c r="O6" s="87"/>
-      <c r="P6" s="87"/>
-      <c r="Q6" s="87"/>
-      <c r="R6" s="87"/>
-      <c r="S6" s="88"/>
+      <c r="E6" s="113"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="114"/>
+      <c r="H6" s="114"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="83" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" s="83"/>
+      <c r="L6" s="84"/>
+      <c r="N6" s="101"/>
+      <c r="O6" s="102"/>
+      <c r="P6" s="102"/>
+      <c r="Q6" s="102"/>
+      <c r="R6" s="102"/>
+      <c r="S6" s="103"/>
       <c r="T6" s="73"/>
       <c r="X6" s="29"/>
       <c r="Y6" s="29"/>
     </row>
     <row r="7" spans="2:25" ht="15.75" thickBot="1">
       <c r="D7" s="71"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="99"/>
-      <c r="K7" s="99"/>
-      <c r="L7" s="110"/>
-      <c r="N7" s="89"/>
-      <c r="O7" s="90"/>
-      <c r="P7" s="90"/>
-      <c r="Q7" s="90"/>
-      <c r="R7" s="90"/>
-      <c r="S7" s="91"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="114"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="84"/>
+      <c r="N7" s="104"/>
+      <c r="O7" s="105"/>
+      <c r="P7" s="105"/>
+      <c r="Q7" s="105"/>
+      <c r="R7" s="105"/>
+      <c r="S7" s="106"/>
       <c r="T7" s="73"/>
       <c r="X7" s="29"/>
       <c r="Y7" s="29"/>
@@ -3226,16 +3908,16 @@
       </c>
       <c r="C8" s="76"/>
       <c r="D8" s="71"/>
-      <c r="E8" s="100"/>
-      <c r="F8" s="101"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="101"/>
-      <c r="I8" s="101"/>
-      <c r="J8" s="111" t="s">
+      <c r="E8" s="113"/>
+      <c r="F8" s="114"/>
+      <c r="G8" s="114"/>
+      <c r="H8" s="114"/>
+      <c r="I8" s="114"/>
+      <c r="J8" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="K8" s="111"/>
-      <c r="L8" s="112"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="86"/>
     </row>
     <row r="9" spans="2:25" ht="15.75" customHeight="1" thickBot="1">
       <c r="B9" s="15" t="s">
@@ -3244,34 +3926,34 @@
       <c r="C9" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="98" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9" s="99"/>
-      <c r="G9" s="99"/>
-      <c r="H9" s="99"/>
-      <c r="I9" s="99"/>
-      <c r="J9" s="111"/>
-      <c r="K9" s="111"/>
-      <c r="L9" s="112"/>
+      <c r="E9" s="89" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="85"/>
+      <c r="L9" s="86"/>
     </row>
     <row r="10" spans="2:25" ht="15.75" customHeight="1" thickBot="1">
       <c r="B10" s="18">
         <v>0</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="E10" s="98"/>
-      <c r="F10" s="99"/>
-      <c r="G10" s="99"/>
-      <c r="H10" s="99"/>
-      <c r="I10" s="99"/>
-      <c r="J10" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="89"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="K10" s="99"/>
-      <c r="L10" s="110"/>
+      <c r="K10" s="83"/>
+      <c r="L10" s="84"/>
       <c r="N10" s="12" t="s">
         <v>24</v>
       </c>
@@ -3289,16 +3971,16 @@
       <c r="C11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="102" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" s="103"/>
-      <c r="G11" s="103"/>
-      <c r="H11" s="103"/>
-      <c r="I11" s="103"/>
-      <c r="J11" s="113"/>
-      <c r="K11" s="113"/>
-      <c r="L11" s="114"/>
+      <c r="E11" s="90" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="91"/>
+      <c r="G11" s="91"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="91"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="88"/>
       <c r="N11" s="14" t="s">
         <v>11</v>
       </c>
@@ -3340,7 +4022,7 @@
         <v>4</v>
       </c>
       <c r="S12" s="65" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="2:25" ht="15.75" thickBot="1">
@@ -3369,7 +4051,7 @@
         <v>0.5</v>
       </c>
       <c r="Q13" s="47">
-        <f>INDEX(F22:L25, 1, N18)</f>
+        <f>INDEX(F43:L46, 1, N18)</f>
         <v>14</v>
       </c>
       <c r="R13" s="61" t="str">
@@ -3377,7 +4059,7 @@
         <v>FAC MTGS</v>
       </c>
       <c r="S13" s="66" t="str">
-        <f>INDEX(F29:L32, 1, N18)</f>
+        <f>INDEX(F50:L53, 1, N18)</f>
         <v>7:45-9:00</v>
       </c>
     </row>
@@ -3429,7 +4111,7 @@
         <v>Bible</v>
       </c>
       <c r="S14" s="67" t="str">
-        <f>INDEX(F33:L36, P14, N18)</f>
+        <f>INDEX(F54:L57, P14, N18)</f>
         <v>9:00-10:10</v>
       </c>
     </row>
@@ -3448,7 +4130,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H15" s="3">
         <v>2</v>
@@ -3473,7 +4155,7 @@
         <v>1.5</v>
       </c>
       <c r="Q15" s="48">
-        <f>INDEX(F22:L25, 2, N18)</f>
+        <f>INDEX(F43:L46, 2, N18)</f>
         <v>10</v>
       </c>
       <c r="R15" s="61" t="str">
@@ -3481,7 +4163,7 @@
         <v>Break</v>
       </c>
       <c r="S15" s="66" t="str">
-        <f>INDEX(F29:L32, 2, N18)</f>
+        <f>INDEX(F50:L53, 2, N18)</f>
         <v>10:10-10:25</v>
       </c>
     </row>
@@ -3515,7 +4197,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N16" s="53">
         <f>MAX(NETWORKDAYS(N12, N14,N22:N123)-1, 0)</f>
@@ -3527,14 +4209,14 @@
       </c>
       <c r="Q16" s="44">
         <f>INDEX(F15:L18,P16, Q11)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="R16" s="62" t="str">
         <f>INDEX(C11:C18, Q16, 1)</f>
-        <v>Free</v>
+        <v>English</v>
       </c>
       <c r="S16" s="67" t="str">
-        <f>INDEX(F33:L36, P16, N18)</f>
+        <f>INDEX(F54:L57, P16, N18)</f>
         <v>10:25-11:35</v>
       </c>
     </row>
@@ -3562,7 +4244,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K17" s="3">
         <v>2</v>
@@ -3571,7 +4253,7 @@
         <v>6</v>
       </c>
       <c r="N17" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O17" s="54"/>
       <c r="P17" s="43">
@@ -3586,7 +4268,7 @@
         <v>Orchestra</v>
       </c>
       <c r="S17" s="67" t="str">
-        <f>INDEX(F33:L36, P17, N18)</f>
+        <f>INDEX(F54:L57, P17, N18)</f>
         <v>11:35-1:40</v>
       </c>
     </row>
@@ -3608,7 +4290,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I18" s="5">
         <v>2</v>
@@ -3631,7 +4313,7 @@
         <v>3.5</v>
       </c>
       <c r="Q18" s="48">
-        <f>INDEX(F22:L25, 3, N18)</f>
+        <f>INDEX(F43:L46, 3, N18)</f>
         <v>10</v>
       </c>
       <c r="R18" s="61" t="str">
@@ -3639,7 +4321,7 @@
         <v>Break</v>
       </c>
       <c r="S18" s="66" t="str">
-        <f>INDEX(F29:L32, 3, N18)</f>
+        <f>INDEX(F50:L53, 3, N18)</f>
         <v>1:40-1:50</v>
       </c>
     </row>
@@ -3649,7 +4331,7 @@
         <v>9</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O19" s="28"/>
       <c r="P19" s="43">
@@ -3664,7 +4346,7 @@
         <v>Physics</v>
       </c>
       <c r="S19" s="67" t="str">
-        <f>INDEX(F33:L36, P19, N18)</f>
+        <f>INDEX(F54:L57, P19, N18)</f>
         <v>1:50-3:00</v>
       </c>
     </row>
@@ -3674,10 +4356,10 @@
         <v>10</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E20" s="74" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="F20" s="75"/>
       <c r="G20" s="75"/>
@@ -3694,7 +4376,7 @@
         <v>4.5</v>
       </c>
       <c r="Q20" s="49">
-        <f>INDEX(F22:L25, 4, N18)</f>
+        <f>INDEX(F43:L46, 4, N18)</f>
         <v>9</v>
       </c>
       <c r="R20" s="64" t="str">
@@ -3702,7 +4384,7 @@
         <v>Office Hours</v>
       </c>
       <c r="S20" s="68" t="str">
-        <f>INDEX(F29:L32, 4, N18)</f>
+        <f>INDEX(F50:L53, 4, N18)</f>
         <v>3:00-3:30</v>
       </c>
     </row>
@@ -3712,31 +4394,31 @@
         <v>11</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="G21" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="H21" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="I21" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="J21" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="K21" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="115" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="116" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="116" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="116" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="116" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="116" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="L21" s="35" t="s">
-        <v>49</v>
+      <c r="L21" s="117" t="s">
+        <v>20</v>
       </c>
       <c r="N21" s="13" t="s">
         <v>0</v>
@@ -3749,31 +4431,31 @@
         <v>12</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="50">
-        <v>0.5</v>
-      </c>
-      <c r="F22" s="45">
-        <v>0</v>
-      </c>
-      <c r="G22" s="45">
-        <v>9</v>
-      </c>
-      <c r="H22" s="45">
-        <v>13</v>
-      </c>
-      <c r="I22" s="45">
-        <v>14</v>
-      </c>
-      <c r="J22" s="45">
-        <v>13</v>
-      </c>
-      <c r="K22" s="45">
-        <v>9</v>
-      </c>
-      <c r="L22" s="38">
-        <v>0</v>
+        <v>41</v>
+      </c>
+      <c r="E22" s="43">
+        <v>1</v>
+      </c>
+      <c r="F22" s="118">
+        <v>1</v>
+      </c>
+      <c r="G22" s="123">
+        <v>8</v>
+      </c>
+      <c r="H22" s="118">
+        <v>2</v>
+      </c>
+      <c r="I22" s="118">
+        <v>6</v>
+      </c>
+      <c r="J22" s="118">
+        <v>3</v>
+      </c>
+      <c r="K22" s="118">
+        <v>7</v>
+      </c>
+      <c r="L22" s="119">
+        <v>4</v>
       </c>
       <c r="N22" s="7">
         <v>41659</v>
@@ -3786,31 +4468,31 @@
         <v>13</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="50">
-        <v>1.5</v>
-      </c>
-      <c r="F23" s="45">
-        <v>0</v>
-      </c>
-      <c r="G23" s="45">
-        <v>10</v>
-      </c>
-      <c r="H23" s="45">
-        <v>10</v>
-      </c>
-      <c r="I23" s="45">
-        <v>10</v>
-      </c>
-      <c r="J23" s="45">
-        <v>11</v>
-      </c>
-      <c r="K23" s="45">
-        <v>12</v>
-      </c>
-      <c r="L23" s="38">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="E23" s="43">
+        <v>2</v>
+      </c>
+      <c r="F23" s="118">
+        <v>2</v>
+      </c>
+      <c r="G23" s="118">
+        <v>6</v>
+      </c>
+      <c r="H23" s="118">
+        <v>3</v>
+      </c>
+      <c r="I23" s="118">
+        <v>7</v>
+      </c>
+      <c r="J23" s="118">
+        <v>4</v>
+      </c>
+      <c r="K23" s="118">
+        <v>1</v>
+      </c>
+      <c r="L23" s="124">
+        <v>8</v>
       </c>
       <c r="N23" s="7">
         <v>41687</v>
@@ -3823,31 +4505,31 @@
         <v>14</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="50">
-        <v>3.5</v>
-      </c>
-      <c r="F24" s="45">
-        <v>0</v>
-      </c>
-      <c r="G24" s="45">
-        <v>15</v>
-      </c>
-      <c r="H24" s="45">
-        <v>15</v>
-      </c>
-      <c r="I24" s="45">
-        <v>10</v>
-      </c>
-      <c r="J24" s="45">
-        <v>10</v>
-      </c>
-      <c r="K24" s="45">
-        <v>10</v>
-      </c>
-      <c r="L24" s="38">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="E24" s="43">
+        <v>3</v>
+      </c>
+      <c r="F24" s="118">
+        <v>3</v>
+      </c>
+      <c r="G24" s="118">
+        <v>7</v>
+      </c>
+      <c r="H24" s="118">
+        <v>4</v>
+      </c>
+      <c r="I24" s="118">
+        <v>1</v>
+      </c>
+      <c r="J24" s="123">
+        <v>8</v>
+      </c>
+      <c r="K24" s="118">
+        <v>2</v>
+      </c>
+      <c r="L24" s="119">
+        <v>6</v>
       </c>
       <c r="N24" s="7">
         <v>41706</v>
@@ -3862,31 +4544,31 @@
         <v>15</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="E25" s="51">
-        <v>4.5</v>
-      </c>
-      <c r="F25" s="52">
-        <v>0</v>
-      </c>
-      <c r="G25" s="52">
-        <v>9</v>
-      </c>
-      <c r="H25" s="52">
-        <v>9</v>
-      </c>
-      <c r="I25" s="52">
-        <v>9</v>
-      </c>
-      <c r="J25" s="52">
-        <v>9</v>
-      </c>
-      <c r="K25" s="52">
-        <v>0</v>
-      </c>
-      <c r="L25" s="39">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="E25" s="120">
+        <v>4</v>
+      </c>
+      <c r="F25" s="121">
+        <v>4</v>
+      </c>
+      <c r="G25" s="121">
+        <v>1</v>
+      </c>
+      <c r="H25" s="125">
+        <v>8</v>
+      </c>
+      <c r="I25" s="121">
+        <v>2</v>
+      </c>
+      <c r="J25" s="121">
+        <v>6</v>
+      </c>
+      <c r="K25" s="121">
+        <v>3</v>
+      </c>
+      <c r="L25" s="122">
+        <v>7</v>
       </c>
       <c r="N25" s="7">
         <v>41707</v>
@@ -3896,7 +4578,7 @@
       <c r="S25" s="27"/>
     </row>
     <row r="26" spans="2:19" ht="15.75" thickBot="1">
-      <c r="E26" s="30"/>
+      <c r="E26" s="28"/>
       <c r="N26" s="7">
         <v>41708</v>
       </c>
@@ -3906,7 +4588,7 @@
     </row>
     <row r="27" spans="2:19" ht="15.75" thickBot="1">
       <c r="E27" s="74" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="F27" s="75"/>
       <c r="G27" s="75"/>
@@ -3922,29 +4604,29 @@
       <c r="Q27" s="26"/>
     </row>
     <row r="28" spans="2:19">
-      <c r="E28" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F28" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="G28" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="H28" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="I28" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="J28" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="K28" s="34" t="s">
+      <c r="E28" s="115" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="116" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="116" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="116" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" s="116" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="116" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="L28" s="35" t="s">
-        <v>49</v>
+      <c r="L28" s="117" t="s">
+        <v>20</v>
       </c>
       <c r="N28" s="7">
         <v>41710</v>
@@ -3954,29 +4636,29 @@
       <c r="S28" s="25"/>
     </row>
     <row r="29" spans="2:19">
-      <c r="E29" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="F29" s="55">
-        <v>0</v>
-      </c>
-      <c r="G29" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="H29" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="I29" s="55" t="s">
-        <v>62</v>
-      </c>
-      <c r="J29" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="K29" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="L29" s="56">
-        <v>0</v>
+      <c r="E29" s="43">
+        <v>1</v>
+      </c>
+      <c r="F29" s="118">
+        <v>1</v>
+      </c>
+      <c r="G29" s="118">
+        <v>5</v>
+      </c>
+      <c r="H29" s="118">
+        <v>2</v>
+      </c>
+      <c r="I29" s="118">
+        <v>6</v>
+      </c>
+      <c r="J29" s="118">
+        <v>3</v>
+      </c>
+      <c r="K29" s="123">
+        <v>8</v>
+      </c>
+      <c r="L29" s="119">
+        <v>4</v>
       </c>
       <c r="N29" s="7">
         <v>41711</v>
@@ -3986,29 +4668,29 @@
       <c r="S29" s="26"/>
     </row>
     <row r="30" spans="2:19">
-      <c r="E30" s="18">
-        <v>1.5</v>
-      </c>
-      <c r="F30" s="55">
-        <v>0</v>
-      </c>
-      <c r="G30" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="H30" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="I30" s="55" t="s">
-        <v>64</v>
-      </c>
-      <c r="J30" s="55" t="s">
-        <v>68</v>
-      </c>
-      <c r="K30" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="L30" s="56">
-        <v>0</v>
+      <c r="E30" s="43">
+        <v>2</v>
+      </c>
+      <c r="F30" s="118">
+        <v>2</v>
+      </c>
+      <c r="G30" s="118">
+        <v>6</v>
+      </c>
+      <c r="H30" s="118">
+        <v>3</v>
+      </c>
+      <c r="I30" s="118">
+        <v>7</v>
+      </c>
+      <c r="J30" s="118">
+        <v>4</v>
+      </c>
+      <c r="K30" s="118">
+        <v>1</v>
+      </c>
+      <c r="L30" s="119">
+        <v>5</v>
       </c>
       <c r="N30" s="7">
         <v>41712</v>
@@ -4018,29 +4700,29 @@
       <c r="S30" s="27"/>
     </row>
     <row r="31" spans="2:19">
-      <c r="E31" s="18">
-        <v>3.5</v>
-      </c>
-      <c r="F31" s="55">
-        <v>0</v>
-      </c>
-      <c r="G31" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="H31" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="I31" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="J31" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="K31" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="L31" s="56">
-        <v>0</v>
+      <c r="E31" s="43">
+        <v>3</v>
+      </c>
+      <c r="F31" s="118">
+        <v>3</v>
+      </c>
+      <c r="G31" s="123">
+        <v>8</v>
+      </c>
+      <c r="H31" s="118">
+        <v>4</v>
+      </c>
+      <c r="I31" s="118">
+        <v>1</v>
+      </c>
+      <c r="J31" s="118">
+        <v>5</v>
+      </c>
+      <c r="K31" s="118">
+        <v>2</v>
+      </c>
+      <c r="L31" s="119">
+        <v>6</v>
       </c>
       <c r="N31" s="7">
         <v>41713</v>
@@ -4049,30 +4731,30 @@
       <c r="Q31" s="60"/>
       <c r="S31" s="27"/>
     </row>
-    <row r="32" spans="2:19">
-      <c r="E32" s="18">
-        <v>4.5</v>
-      </c>
-      <c r="F32" s="55">
-        <v>0</v>
-      </c>
-      <c r="G32" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="H32" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="I32" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="J32" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="K32" s="55">
-        <v>0</v>
-      </c>
-      <c r="L32" s="56">
-        <v>0</v>
+    <row r="32" spans="2:19" ht="15.75" thickBot="1">
+      <c r="E32" s="120">
+        <v>4</v>
+      </c>
+      <c r="F32" s="121">
+        <v>4</v>
+      </c>
+      <c r="G32" s="121">
+        <v>1</v>
+      </c>
+      <c r="H32" s="121">
+        <v>5</v>
+      </c>
+      <c r="I32" s="121">
+        <v>2</v>
+      </c>
+      <c r="J32" s="121">
+        <v>6</v>
+      </c>
+      <c r="K32" s="121">
+        <v>3</v>
+      </c>
+      <c r="L32" s="122">
+        <v>7</v>
       </c>
       <c r="N32" s="7">
         <v>41714</v>
@@ -4081,62 +4763,25 @@
       <c r="Q32" s="60"/>
       <c r="S32" s="27"/>
     </row>
-    <row r="33" spans="5:17">
-      <c r="E33" s="18">
-        <v>1</v>
-      </c>
-      <c r="F33" s="55">
-        <v>0</v>
-      </c>
-      <c r="G33" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="H33" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="I33" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="J33" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="K33" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="L33" s="56">
-        <v>0</v>
-      </c>
+    <row r="33" spans="5:17" ht="15.75" thickBot="1">
+      <c r="E33" s="28"/>
       <c r="N33" s="7">
         <v>41747</v>
       </c>
       <c r="O33" s="60"/>
       <c r="Q33" s="60"/>
     </row>
-    <row r="34" spans="5:17">
-      <c r="E34" s="18">
-        <v>2</v>
-      </c>
-      <c r="F34" s="55">
-        <v>0</v>
-      </c>
-      <c r="G34" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="H34" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="I34" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="J34" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="K34" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="L34" s="56">
-        <v>0</v>
-      </c>
+    <row r="34" spans="5:17" ht="15.75" thickBot="1">
+      <c r="E34" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="F34" s="75"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="75"/>
+      <c r="I34" s="75"/>
+      <c r="J34" s="75"/>
+      <c r="K34" s="75"/>
+      <c r="L34" s="76"/>
       <c r="N34" s="7">
         <v>41748</v>
       </c>
@@ -4144,29 +4789,29 @@
       <c r="Q34" s="60"/>
     </row>
     <row r="35" spans="5:17">
-      <c r="E35" s="18">
-        <v>3</v>
-      </c>
-      <c r="F35" s="55">
-        <v>0</v>
-      </c>
-      <c r="G35" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="H35" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="I35" s="55" t="s">
-        <v>66</v>
-      </c>
-      <c r="J35" s="55" t="s">
-        <v>66</v>
-      </c>
-      <c r="K35" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="L35" s="56">
-        <v>0</v>
+      <c r="E35" s="115" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" s="116" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="116" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="116" t="s">
+        <v>17</v>
+      </c>
+      <c r="I35" s="116" t="s">
+        <v>18</v>
+      </c>
+      <c r="J35" s="116" t="s">
+        <v>19</v>
+      </c>
+      <c r="K35" s="116" t="s">
+        <v>14</v>
+      </c>
+      <c r="L35" s="117" t="s">
+        <v>20</v>
       </c>
       <c r="N35" s="7">
         <v>41749</v>
@@ -4174,30 +4819,30 @@
       <c r="O35" s="60"/>
       <c r="Q35" s="60"/>
     </row>
-    <row r="36" spans="5:17" ht="15.75" thickBot="1">
-      <c r="E36" s="20">
+    <row r="36" spans="5:17">
+      <c r="E36" s="43">
+        <v>1</v>
+      </c>
+      <c r="F36" s="118">
+        <v>1</v>
+      </c>
+      <c r="G36" s="123">
+        <v>8</v>
+      </c>
+      <c r="H36" s="118">
+        <v>2</v>
+      </c>
+      <c r="I36" s="118">
+        <v>6</v>
+      </c>
+      <c r="J36" s="118">
+        <v>3</v>
+      </c>
+      <c r="K36" s="123">
+        <v>8</v>
+      </c>
+      <c r="L36" s="119">
         <v>4</v>
-      </c>
-      <c r="F36" s="57">
-        <v>0</v>
-      </c>
-      <c r="G36" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="H36" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="I36" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="J36" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="K36" s="57" t="s">
-        <v>70</v>
-      </c>
-      <c r="L36" s="58">
-        <v>0</v>
       </c>
       <c r="N36" s="7">
         <v>41750</v>
@@ -4206,87 +4851,516 @@
       <c r="Q36" s="60"/>
     </row>
     <row r="37" spans="5:17">
+      <c r="E37" s="43">
+        <v>2</v>
+      </c>
+      <c r="F37" s="118">
+        <v>2</v>
+      </c>
+      <c r="G37" s="118">
+        <v>6</v>
+      </c>
+      <c r="H37" s="118">
+        <v>3</v>
+      </c>
+      <c r="I37" s="118">
+        <v>7</v>
+      </c>
+      <c r="J37" s="118">
+        <v>4</v>
+      </c>
+      <c r="K37" s="118">
+        <v>1</v>
+      </c>
+      <c r="L37" s="124">
+        <v>8</v>
+      </c>
       <c r="N37" s="7"/>
     </row>
     <row r="38" spans="5:17">
+      <c r="E38" s="43">
+        <v>3</v>
+      </c>
+      <c r="F38" s="118">
+        <v>3</v>
+      </c>
+      <c r="G38" s="123">
+        <v>8</v>
+      </c>
+      <c r="H38" s="118">
+        <v>4</v>
+      </c>
+      <c r="I38" s="118">
+        <v>1</v>
+      </c>
+      <c r="J38" s="123">
+        <v>8</v>
+      </c>
+      <c r="K38" s="118">
+        <v>2</v>
+      </c>
+      <c r="L38" s="119">
+        <v>6</v>
+      </c>
       <c r="N38" s="7"/>
     </row>
-    <row r="39" spans="5:17">
+    <row r="39" spans="5:17" ht="15.75" thickBot="1">
+      <c r="E39" s="120">
+        <v>4</v>
+      </c>
+      <c r="F39" s="121">
+        <v>4</v>
+      </c>
+      <c r="G39" s="121">
+        <v>1</v>
+      </c>
+      <c r="H39" s="125">
+        <v>8</v>
+      </c>
+      <c r="I39" s="121">
+        <v>2</v>
+      </c>
+      <c r="J39" s="121">
+        <v>6</v>
+      </c>
+      <c r="K39" s="121">
+        <v>3</v>
+      </c>
+      <c r="L39" s="122">
+        <v>7</v>
+      </c>
       <c r="N39" s="7"/>
     </row>
-    <row r="40" spans="5:17">
+    <row r="40" spans="5:17" ht="15.75" thickBot="1">
       <c r="N40" s="7"/>
     </row>
-    <row r="41" spans="5:17">
+    <row r="41" spans="5:17" ht="15.75" thickBot="1">
+      <c r="E41" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" s="75"/>
+      <c r="G41" s="75"/>
+      <c r="H41" s="75"/>
+      <c r="I41" s="75"/>
+      <c r="J41" s="75"/>
+      <c r="K41" s="75"/>
+      <c r="L41" s="76"/>
       <c r="N41" s="7"/>
     </row>
     <row r="42" spans="5:17">
+      <c r="E42" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F42" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="G42" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="H42" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="I42" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="J42" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="K42" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="L42" s="35" t="s">
+        <v>48</v>
+      </c>
       <c r="N42" s="7"/>
     </row>
     <row r="43" spans="5:17">
+      <c r="E43" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="F43" s="45">
+        <v>0</v>
+      </c>
+      <c r="G43" s="45">
+        <v>9</v>
+      </c>
+      <c r="H43" s="45">
+        <v>13</v>
+      </c>
+      <c r="I43" s="45">
+        <v>14</v>
+      </c>
+      <c r="J43" s="45">
+        <v>13</v>
+      </c>
+      <c r="K43" s="45">
+        <v>9</v>
+      </c>
+      <c r="L43" s="38">
+        <v>0</v>
+      </c>
       <c r="N43" s="7"/>
     </row>
     <row r="44" spans="5:17">
+      <c r="E44" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="F44" s="45">
+        <v>0</v>
+      </c>
+      <c r="G44" s="45">
+        <v>10</v>
+      </c>
+      <c r="H44" s="45">
+        <v>10</v>
+      </c>
+      <c r="I44" s="45">
+        <v>10</v>
+      </c>
+      <c r="J44" s="45">
+        <v>11</v>
+      </c>
+      <c r="K44" s="45">
+        <v>12</v>
+      </c>
+      <c r="L44" s="38">
+        <v>0</v>
+      </c>
       <c r="N44" s="7"/>
     </row>
     <row r="45" spans="5:17">
+      <c r="E45" s="50">
+        <v>3.5</v>
+      </c>
+      <c r="F45" s="45">
+        <v>0</v>
+      </c>
+      <c r="G45" s="45">
+        <v>15</v>
+      </c>
+      <c r="H45" s="45">
+        <v>15</v>
+      </c>
+      <c r="I45" s="45">
+        <v>10</v>
+      </c>
+      <c r="J45" s="45">
+        <v>10</v>
+      </c>
+      <c r="K45" s="45">
+        <v>10</v>
+      </c>
+      <c r="L45" s="38">
+        <v>0</v>
+      </c>
       <c r="N45" s="7"/>
     </row>
-    <row r="46" spans="5:17">
+    <row r="46" spans="5:17" ht="15.75" thickBot="1">
+      <c r="E46" s="51">
+        <v>4.5</v>
+      </c>
+      <c r="F46" s="52">
+        <v>0</v>
+      </c>
+      <c r="G46" s="52">
+        <v>9</v>
+      </c>
+      <c r="H46" s="52">
+        <v>9</v>
+      </c>
+      <c r="I46" s="52">
+        <v>9</v>
+      </c>
+      <c r="J46" s="52">
+        <v>9</v>
+      </c>
+      <c r="K46" s="52">
+        <v>0</v>
+      </c>
+      <c r="L46" s="39">
+        <v>0</v>
+      </c>
       <c r="N46" s="7"/>
     </row>
-    <row r="47" spans="5:17">
+    <row r="47" spans="5:17" ht="15.75" thickBot="1">
+      <c r="E47" s="30"/>
       <c r="N47" s="7"/>
     </row>
-    <row r="48" spans="5:17">
+    <row r="48" spans="5:17" ht="15.75" thickBot="1">
+      <c r="E48" s="74" t="s">
+        <v>49</v>
+      </c>
+      <c r="F48" s="75"/>
+      <c r="G48" s="75"/>
+      <c r="H48" s="75"/>
+      <c r="I48" s="75"/>
+      <c r="J48" s="75"/>
+      <c r="K48" s="75"/>
+      <c r="L48" s="76"/>
       <c r="N48" s="7"/>
     </row>
-    <row r="49" spans="14:14">
+    <row r="49" spans="5:14">
+      <c r="E49" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F49" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="G49" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="H49" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="I49" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="J49" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="K49" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="L49" s="35" t="s">
+        <v>48</v>
+      </c>
       <c r="N49" s="7"/>
     </row>
-    <row r="50" spans="14:14">
+    <row r="50" spans="5:14">
+      <c r="E50" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="F50" s="55">
+        <v>0</v>
+      </c>
+      <c r="G50" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="H50" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="I50" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="J50" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="K50" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="L50" s="56">
+        <v>0</v>
+      </c>
       <c r="N50" s="7"/>
     </row>
-    <row r="51" spans="14:14">
+    <row r="51" spans="5:14">
+      <c r="E51" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="F51" s="55">
+        <v>0</v>
+      </c>
+      <c r="G51" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="H51" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="I51" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="J51" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="K51" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="L51" s="56">
+        <v>0</v>
+      </c>
       <c r="N51" s="7"/>
     </row>
-    <row r="52" spans="14:14">
+    <row r="52" spans="5:14">
+      <c r="E52" s="18">
+        <v>3.5</v>
+      </c>
+      <c r="F52" s="55">
+        <v>0</v>
+      </c>
+      <c r="G52" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="H52" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="I52" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="J52" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="K52" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="L52" s="56">
+        <v>0</v>
+      </c>
       <c r="N52" s="7"/>
     </row>
-    <row r="53" spans="14:14">
+    <row r="53" spans="5:14">
+      <c r="E53" s="18">
+        <v>4.5</v>
+      </c>
+      <c r="F53" s="55">
+        <v>0</v>
+      </c>
+      <c r="G53" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="H53" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I53" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="J53" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="K53" s="55">
+        <v>0</v>
+      </c>
+      <c r="L53" s="56">
+        <v>0</v>
+      </c>
       <c r="N53" s="7"/>
     </row>
-    <row r="54" spans="14:14">
+    <row r="54" spans="5:14">
+      <c r="E54" s="18">
+        <v>1</v>
+      </c>
+      <c r="F54" s="55">
+        <v>0</v>
+      </c>
+      <c r="G54" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="H54" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="I54" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="J54" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="K54" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="L54" s="56">
+        <v>0</v>
+      </c>
       <c r="N54" s="7"/>
     </row>
-    <row r="55" spans="14:14">
+    <row r="55" spans="5:14">
+      <c r="E55" s="18">
+        <v>2</v>
+      </c>
+      <c r="F55" s="55">
+        <v>0</v>
+      </c>
+      <c r="G55" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="H55" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="I55" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="J55" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="K55" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="L55" s="56">
+        <v>0</v>
+      </c>
       <c r="N55" s="7"/>
     </row>
-    <row r="56" spans="14:14">
+    <row r="56" spans="5:14">
+      <c r="E56" s="18">
+        <v>3</v>
+      </c>
+      <c r="F56" s="55">
+        <v>0</v>
+      </c>
+      <c r="G56" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="H56" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I56" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="J56" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="K56" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="L56" s="56">
+        <v>0</v>
+      </c>
       <c r="N56" s="7"/>
     </row>
-    <row r="57" spans="14:14">
+    <row r="57" spans="5:14" ht="15.75" thickBot="1">
+      <c r="E57" s="20">
+        <v>4</v>
+      </c>
+      <c r="F57" s="57">
+        <v>0</v>
+      </c>
+      <c r="G57" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="H57" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="I57" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="J57" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="K57" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="L57" s="58">
+        <v>0</v>
+      </c>
       <c r="N57" s="7"/>
     </row>
-    <row r="58" spans="14:14">
+    <row r="58" spans="5:14">
       <c r="N58" s="7"/>
     </row>
-    <row r="59" spans="14:14">
+    <row r="59" spans="5:14">
       <c r="N59" s="7"/>
     </row>
-    <row r="60" spans="14:14">
+    <row r="60" spans="5:14">
       <c r="N60" s="7"/>
     </row>
-    <row r="61" spans="14:14">
+    <row r="61" spans="5:14">
       <c r="N61" s="7"/>
     </row>
-    <row r="62" spans="14:14">
+    <row r="62" spans="5:14">
       <c r="N62" s="7"/>
     </row>
-    <row r="63" spans="14:14">
+    <row r="63" spans="5:14">
       <c r="N63" s="7"/>
     </row>
-    <row r="64" spans="14:14">
+    <row r="64" spans="5:14">
       <c r="N64" s="7"/>
     </row>
     <row r="65" spans="14:14">
@@ -4468,14 +5542,22 @@
     </row>
   </sheetData>
   <sheetProtection password="C836" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
-  <mergeCells count="21">
+  <mergeCells count="24">
+    <mergeCell ref="E20:L20"/>
+    <mergeCell ref="E27:L27"/>
+    <mergeCell ref="E34:L34"/>
+    <mergeCell ref="E41:L41"/>
+    <mergeCell ref="E48:L48"/>
+    <mergeCell ref="E9:I10"/>
+    <mergeCell ref="J10:L11"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="N3:S4"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E27:L27"/>
     <mergeCell ref="P10:S10"/>
     <mergeCell ref="E13:L13"/>
-    <mergeCell ref="E20:L20"/>
     <mergeCell ref="N5:S7"/>
     <mergeCell ref="E2:L2"/>
     <mergeCell ref="E3:I3"/>
@@ -4485,11 +5567,6 @@
     <mergeCell ref="E5:I8"/>
     <mergeCell ref="J6:L7"/>
     <mergeCell ref="J8:L9"/>
-    <mergeCell ref="E9:I10"/>
-    <mergeCell ref="J10:L11"/>
-    <mergeCell ref="E11:I11"/>
-    <mergeCell ref="N2:S2"/>
-    <mergeCell ref="N3:S4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>